<commit_message>
Planilla de metricas actualizada
21-04-2016: Se agregan metricas de metodos sumar(), restar(), producto(float).
</commit_message>
<xml_diff>
--- a/Documentacion/MatrizMath/MatrizMath - Planilla de Métricas V2.1.xlsx
+++ b/Documentacion/MatrizMath/MatrizMath - Planilla de Métricas V2.1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
   <si>
     <t>PROYECTO:</t>
   </si>
@@ -151,10 +151,13 @@
     <t>llevarACeroPosicionesPorDebajo()</t>
   </si>
   <si>
-    <t>producto() por un número</t>
+    <t>producto()por una matriz</t>
   </si>
   <si>
-    <t>producto()por una matriz</t>
+    <t>sumar() y restar()</t>
+  </si>
+  <si>
+    <t>producto(float)</t>
   </si>
 </sst>
 </file>
@@ -782,7 +785,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1037,23 +1040,74 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1064,62 +1118,513 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="46">
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFFFFFF"/>
@@ -1352,7 +1857,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
@@ -1363,8 +1868,8 @@
           <c:yMode val="edge"/>
           <c:x val="3.3565974707706982E-2"/>
           <c:y val="7.4074152627750078E-2"/>
-          <c:w val="0.40158680164979405"/>
-          <c:h val="0.85185169474450029"/>
+          <c:w val="0.40158680164979416"/>
+          <c:h val="0.85185169474450051"/>
         </c:manualLayout>
       </c:layout>
       <c:pieChart>
@@ -1491,7 +1996,6 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
       <c:spPr>
@@ -1510,7 +2014,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1806,7 +2310,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1817,10 +2321,10 @@
   <dimension ref="A1:Z1006"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
@@ -1836,23 +2340,23 @@
   <sheetData>
     <row r="1" spans="1:26" ht="23.25" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="121" t="s">
+      <c r="B1" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="113"/>
-      <c r="D1" s="120" t="s">
+      <c r="C1" s="87"/>
+      <c r="D1" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
-      <c r="M1" s="113"/>
-      <c r="N1" s="113"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="87"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -1896,12 +2400,12 @@
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
       <c r="A3" s="4"/>
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="88"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="90"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -2027,12 +2531,12 @@
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1">
       <c r="A7" s="4"/>
-      <c r="B7" s="86" t="s">
+      <c r="B7" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="88"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="89"/>
+      <c r="E7" s="90"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -2069,15 +2573,15 @@
       <c r="E8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="112"/>
-      <c r="G8" s="113"/>
-      <c r="H8" s="113"/>
-      <c r="I8" s="113"/>
-      <c r="J8" s="113"/>
-      <c r="K8" s="113"/>
-      <c r="L8" s="113"/>
-      <c r="M8" s="113"/>
-      <c r="N8" s="113"/>
+      <c r="F8" s="92"/>
+      <c r="G8" s="87"/>
+      <c r="H8" s="87"/>
+      <c r="I8" s="87"/>
+      <c r="J8" s="87"/>
+      <c r="K8" s="87"/>
+      <c r="L8" s="87"/>
+      <c r="M8" s="87"/>
+      <c r="N8" s="87"/>
       <c r="O8" s="7"/>
       <c r="P8" s="13"/>
       <c r="Q8" s="14"/>
@@ -2104,15 +2608,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C9),ISBLANK(D9)),"Completar",IF(D9&gt;=C9,D9-C9,"Error")),"Error")</f>
         <v>Completar</v>
       </c>
-      <c r="F9" s="114"/>
-      <c r="G9" s="113"/>
-      <c r="H9" s="113"/>
-      <c r="I9" s="113"/>
-      <c r="J9" s="113"/>
-      <c r="K9" s="113"/>
-      <c r="L9" s="113"/>
-      <c r="M9" s="113"/>
-      <c r="N9" s="113"/>
+      <c r="F9" s="93"/>
+      <c r="G9" s="87"/>
+      <c r="H9" s="87"/>
+      <c r="I9" s="87"/>
+      <c r="J9" s="87"/>
+      <c r="K9" s="87"/>
+      <c r="L9" s="87"/>
+      <c r="M9" s="87"/>
+      <c r="N9" s="87"/>
       <c r="O9" s="15"/>
       <c r="P9" s="21"/>
       <c r="Q9" s="22"/>
@@ -2156,12 +2660,12 @@
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" s="4"/>
-      <c r="B11" s="86" t="s">
+      <c r="B11" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="87"/>
-      <c r="D11" s="87"/>
-      <c r="E11" s="88"/>
+      <c r="C11" s="89"/>
+      <c r="D11" s="89"/>
+      <c r="E11" s="90"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -2198,15 +2702,15 @@
       <c r="E12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="112"/>
-      <c r="G12" s="113"/>
-      <c r="H12" s="113"/>
-      <c r="I12" s="113"/>
-      <c r="J12" s="113"/>
-      <c r="K12" s="113"/>
-      <c r="L12" s="113"/>
-      <c r="M12" s="113"/>
-      <c r="N12" s="113"/>
+      <c r="F12" s="92"/>
+      <c r="G12" s="87"/>
+      <c r="H12" s="87"/>
+      <c r="I12" s="87"/>
+      <c r="J12" s="87"/>
+      <c r="K12" s="87"/>
+      <c r="L12" s="87"/>
+      <c r="M12" s="87"/>
+      <c r="N12" s="87"/>
       <c r="O12" s="7"/>
       <c r="P12" s="13"/>
       <c r="Q12" s="14"/>
@@ -2231,15 +2735,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C13),ISBLANK(D13)),"Completar",IF(D13&gt;=C13,D13-C13,"Error")),"Error")</f>
         <v>Completar</v>
       </c>
-      <c r="F13" s="114"/>
-      <c r="G13" s="113"/>
-      <c r="H13" s="113"/>
-      <c r="I13" s="113"/>
-      <c r="J13" s="113"/>
-      <c r="K13" s="113"/>
-      <c r="L13" s="113"/>
-      <c r="M13" s="113"/>
-      <c r="N13" s="113"/>
+      <c r="F13" s="93"/>
+      <c r="G13" s="87"/>
+      <c r="H13" s="87"/>
+      <c r="I13" s="87"/>
+      <c r="J13" s="87"/>
+      <c r="K13" s="87"/>
+      <c r="L13" s="87"/>
+      <c r="M13" s="87"/>
+      <c r="N13" s="87"/>
       <c r="O13" s="15"/>
       <c r="P13" s="21"/>
       <c r="Q13" s="22"/>
@@ -2283,21 +2787,21 @@
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1">
       <c r="A15" s="4"/>
-      <c r="B15" s="86" t="s">
+      <c r="B15" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="87"/>
-      <c r="D15" s="87"/>
-      <c r="E15" s="87"/>
-      <c r="F15" s="87"/>
-      <c r="G15" s="87"/>
-      <c r="H15" s="87"/>
-      <c r="I15" s="87"/>
-      <c r="J15" s="87"/>
-      <c r="K15" s="87"/>
-      <c r="L15" s="87"/>
-      <c r="M15" s="87"/>
-      <c r="N15" s="88"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="89"/>
+      <c r="E15" s="89"/>
+      <c r="F15" s="89"/>
+      <c r="G15" s="89"/>
+      <c r="H15" s="89"/>
+      <c r="I15" s="89"/>
+      <c r="J15" s="89"/>
+      <c r="K15" s="89"/>
+      <c r="L15" s="89"/>
+      <c r="M15" s="89"/>
+      <c r="N15" s="90"/>
       <c r="O15" s="4"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
@@ -2313,31 +2817,31 @@
     </row>
     <row r="16" spans="1:26" ht="16.5" customHeight="1">
       <c r="A16" s="7"/>
-      <c r="B16" s="95" t="s">
+      <c r="B16" s="116" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="97" t="s">
+      <c r="C16" s="118" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="98"/>
-      <c r="E16" s="98"/>
-      <c r="F16" s="93" t="s">
+      <c r="D16" s="119"/>
+      <c r="E16" s="119"/>
+      <c r="F16" s="111" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="94"/>
-      <c r="H16" s="108" t="s">
+      <c r="G16" s="112"/>
+      <c r="H16" s="110" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="102"/>
-      <c r="J16" s="102"/>
-      <c r="K16" s="93" t="s">
+      <c r="I16" s="95"/>
+      <c r="J16" s="95"/>
+      <c r="K16" s="111" t="s">
         <v>14</v>
       </c>
-      <c r="L16" s="94"/>
-      <c r="M16" s="91" t="s">
+      <c r="L16" s="112"/>
+      <c r="M16" s="114" t="s">
         <v>15</v>
       </c>
-      <c r="N16" s="104" t="s">
+      <c r="N16" s="105" t="s">
         <v>6</v>
       </c>
       <c r="O16" s="7"/>
@@ -2355,10 +2859,10 @@
     </row>
     <row r="17" spans="1:26" ht="30" customHeight="1">
       <c r="A17" s="7"/>
-      <c r="B17" s="96"/>
-      <c r="C17" s="99"/>
-      <c r="D17" s="100"/>
-      <c r="E17" s="100"/>
+      <c r="B17" s="117"/>
+      <c r="C17" s="120"/>
+      <c r="D17" s="121"/>
+      <c r="E17" s="121"/>
       <c r="F17" s="26" t="s">
         <v>16</v>
       </c>
@@ -2380,8 +2884,8 @@
       <c r="L17" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="M17" s="92"/>
-      <c r="N17" s="105"/>
+      <c r="M17" s="115"/>
+      <c r="N17" s="106"/>
       <c r="O17" s="7"/>
       <c r="P17" s="13"/>
       <c r="Q17" s="14"/>
@@ -2401,11 +2905,11 @@
         <f t="shared" ref="B18:B31" si="0">ROW($B18)-16</f>
         <v>2</v>
       </c>
-      <c r="C18" s="101" t="s">
+      <c r="C18" s="107" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="102"/>
-      <c r="E18" s="102"/>
+      <c r="D18" s="95"/>
+      <c r="E18" s="95"/>
       <c r="F18" s="31">
         <v>60</v>
       </c>
@@ -2454,11 +2958,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C19" s="101" t="s">
+      <c r="C19" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="102"/>
-      <c r="E19" s="102"/>
+      <c r="D19" s="95"/>
+      <c r="E19" s="95"/>
       <c r="F19" s="31">
         <v>4</v>
       </c>
@@ -2507,11 +3011,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C20" s="101" t="s">
+      <c r="C20" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="102"/>
-      <c r="E20" s="102"/>
+      <c r="D20" s="95"/>
+      <c r="E20" s="95"/>
       <c r="F20" s="31">
         <v>8</v>
       </c>
@@ -2560,11 +3064,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C21" s="101" t="s">
+      <c r="C21" s="107" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="102"/>
-      <c r="E21" s="102"/>
+      <c r="D21" s="95"/>
+      <c r="E21" s="95"/>
       <c r="F21" s="31">
         <v>10</v>
       </c>
@@ -2613,11 +3117,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C22" s="106" t="s">
+      <c r="C22" s="108" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="107"/>
-      <c r="E22" s="107"/>
+      <c r="D22" s="109"/>
+      <c r="E22" s="109"/>
       <c r="F22" s="74">
         <v>8</v>
       </c>
@@ -2666,11 +3170,11 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C23" s="103" t="s">
+      <c r="C23" s="101" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="102"/>
-      <c r="E23" s="102"/>
+      <c r="D23" s="95"/>
+      <c r="E23" s="95"/>
       <c r="F23" s="42">
         <v>13</v>
       </c>
@@ -2719,11 +3223,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C24" s="103" t="s">
+      <c r="C24" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="102"/>
-      <c r="E24" s="102"/>
+      <c r="D24" s="95"/>
+      <c r="E24" s="95"/>
       <c r="F24" s="42">
         <v>25</v>
       </c>
@@ -2772,11 +3276,11 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C25" s="103" t="s">
+      <c r="C25" s="101" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="102"/>
-      <c r="E25" s="102"/>
+      <c r="D25" s="95"/>
+      <c r="E25" s="95"/>
       <c r="F25" s="42">
         <v>20</v>
       </c>
@@ -2825,11 +3329,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C26" s="103" t="s">
+      <c r="C26" s="101" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="102"/>
-      <c r="E26" s="102"/>
+      <c r="D26" s="95"/>
+      <c r="E26" s="95"/>
       <c r="F26" s="42">
         <v>16</v>
       </c>
@@ -2878,11 +3382,11 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C27" s="103" t="s">
+      <c r="C27" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="102"/>
-      <c r="E27" s="102"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="95"/>
       <c r="F27" s="42">
         <v>30</v>
       </c>
@@ -2931,39 +3435,39 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C28" s="103" t="s">
+      <c r="C28" s="101" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="102"/>
-      <c r="E28" s="102"/>
+      <c r="D28" s="122"/>
+      <c r="E28" s="123"/>
       <c r="F28" s="42">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G28" s="43">
-        <v>5.5555555555555558E-3</v>
+        <v>9.0277777777777787E-3</v>
       </c>
       <c r="H28" s="44">
-        <v>0.76736111111111116</v>
+        <v>0.77430555555555547</v>
       </c>
       <c r="I28" s="45">
-        <v>0.77361111111111114</v>
+        <v>0.78472222222222221</v>
       </c>
       <c r="J28" s="35">
-        <f t="shared" si="1"/>
-        <v>6.2499999999999778E-3</v>
+        <f t="shared" ref="J28" si="3">IFERROR(IF(OR(ISBLANK(H28),ISBLANK(I28)),"",IF(I28&gt;=H28,I28-H28,"Error")),"Error")</f>
+        <v>1.0416666666666741E-2</v>
       </c>
       <c r="K28" s="46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L28" s="47">
-        <v>6.9444444444444447E-4</v>
+        <v>2.7777777777777779E-3</v>
       </c>
       <c r="M28" s="48">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="N28" s="39">
-        <f t="shared" si="2"/>
-        <v>6.9444444444444224E-3</v>
+        <f t="shared" ref="N28:N30" si="4">IFERROR(IF(OR(J28="",ISBLANK(L28)),"",J28+L28),"Error")</f>
+        <v>1.3194444444444519E-2</v>
       </c>
       <c r="O28" s="71"/>
       <c r="P28" s="21"/>
@@ -2984,39 +3488,39 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C29" s="103" t="s">
+      <c r="C29" s="101" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="102"/>
-      <c r="E29" s="102"/>
+      <c r="D29" s="95"/>
+      <c r="E29" s="95"/>
       <c r="F29" s="42">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="G29" s="43">
-        <v>9.0277777777777787E-3</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="H29" s="44">
-        <v>0.77430555555555547</v>
+        <v>0.91527777777777775</v>
       </c>
       <c r="I29" s="45">
-        <v>0.78472222222222221</v>
+        <v>0.95208333333333339</v>
       </c>
       <c r="J29" s="35">
-        <f t="shared" si="1"/>
-        <v>1.0416666666666741E-2</v>
+        <f>IFERROR(IF(OR(ISBLANK(H29),ISBLANK(I29)),"",IF(I29&gt;=H29,I29-H29,"Error")),"Error")</f>
+        <v>3.6805555555555647E-2</v>
       </c>
       <c r="K29" s="46">
         <v>2</v>
       </c>
       <c r="L29" s="47">
-        <v>2.7777777777777779E-3</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="M29" s="48">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="N29" s="39">
-        <f t="shared" si="2"/>
-        <v>1.3194444444444519E-2</v>
+        <f t="shared" si="4"/>
+        <v>4.3750000000000094E-2</v>
       </c>
       <c r="O29" s="71"/>
       <c r="P29" s="21"/>
@@ -3037,23 +3541,39 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C30" s="103"/>
-      <c r="D30" s="102"/>
-      <c r="E30" s="102"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="C30" s="101" t="s">
+        <v>47</v>
       </c>
-      <c r="K30" s="46"/>
-      <c r="L30" s="47"/>
-      <c r="M30" s="48"/>
-      <c r="N30" s="39" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+      <c r="D30" s="95"/>
+      <c r="E30" s="95"/>
+      <c r="F30" s="42">
+        <v>15</v>
+      </c>
+      <c r="G30" s="43">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="H30" s="44">
+        <v>0.99375000000000002</v>
+      </c>
+      <c r="I30" s="45">
+        <v>0.99791666666666667</v>
+      </c>
+      <c r="J30" s="35">
+        <f t="shared" ref="J30" si="5">IFERROR(IF(OR(ISBLANK(H30),ISBLANK(I30)),"",IF(I30&gt;=H30,I30-H30,"Error")),"Error")</f>
+        <v>4.1666666666666519E-3</v>
+      </c>
+      <c r="K30" s="46">
+        <v>0</v>
+      </c>
+      <c r="L30" s="47">
+        <v>0</v>
+      </c>
+      <c r="M30" s="48">
+        <v>7</v>
+      </c>
+      <c r="N30" s="39">
+        <f t="shared" si="4"/>
+        <v>4.1666666666666519E-3</v>
       </c>
       <c r="O30" s="71"/>
       <c r="P30" s="21"/>
@@ -3068,15 +3588,15 @@
       <c r="Y30" s="22"/>
       <c r="Z30" s="22"/>
     </row>
-    <row r="31" spans="1:26">
+    <row r="31" spans="1:26" ht="15" customHeight="1">
       <c r="A31" s="71"/>
       <c r="B31" s="30">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C31" s="103"/>
-      <c r="D31" s="102"/>
-      <c r="E31" s="102"/>
+      <c r="C31" s="101"/>
+      <c r="D31" s="122"/>
+      <c r="E31" s="123"/>
       <c r="F31" s="42"/>
       <c r="G31" s="43"/>
       <c r="H31" s="44"/>
@@ -3107,19 +3627,19 @@
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1">
       <c r="A32" s="7"/>
-      <c r="B32" s="89" t="s">
+      <c r="B32" s="113" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="90"/>
-      <c r="D32" s="90"/>
-      <c r="E32" s="90"/>
+      <c r="C32" s="100"/>
+      <c r="D32" s="100"/>
+      <c r="E32" s="100"/>
       <c r="F32" s="49">
         <f>IF(SUM(F18:F31)=0,"Completar",SUM(F18:F31))</f>
-        <v>227</v>
+        <v>257</v>
       </c>
       <c r="G32" s="50">
         <f>IF(SUM(G18:G31)=0,"Completar",SUM(G18:G31))</f>
-        <v>0.13819444444444445</v>
+        <v>0.16388888888888886</v>
       </c>
       <c r="H32" s="51" t="s">
         <v>24</v>
@@ -3129,23 +3649,23 @@
       </c>
       <c r="J32" s="53">
         <f>IF(OR(COUNTIF(J18:J31,"Error")&gt;0,COUNTIF(J18:J31,"Completar")&gt;0),"Error",IF(SUM(J18:J31)=0,"Completar",SUM(J18:J31)))</f>
-        <v>0.11805555555555569</v>
+        <v>0.15277777777777801</v>
       </c>
       <c r="K32" s="54">
         <f>SUM(K18:K31)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L32" s="50">
         <f>SUM(L18:L31)</f>
-        <v>2.0833333333333336E-2</v>
+        <v>2.7083333333333334E-2</v>
       </c>
       <c r="M32" s="55">
         <f>IF(SUM(M18:M31)=0,"Completar",SUM(M18:M31))</f>
-        <v>207</v>
+        <v>233</v>
       </c>
       <c r="N32" s="18">
         <f>IF(OR(COUNTIF(N18:N31,"Error")&gt;0,COUNTIF(N18:N31,"Completar")&gt;0),"Error",IF(SUM(N18:N31)=0,"Completar",SUM(N18:N31)))</f>
-        <v>0.13888888888888901</v>
+        <v>0.17986111111111133</v>
       </c>
       <c r="O32" s="7"/>
       <c r="P32" s="56"/>
@@ -3190,12 +3710,12 @@
     </row>
     <row r="34" spans="1:26" ht="15" customHeight="1">
       <c r="A34" s="4"/>
-      <c r="B34" s="86" t="s">
+      <c r="B34" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="87"/>
-      <c r="D34" s="87"/>
-      <c r="E34" s="88"/>
+      <c r="C34" s="89"/>
+      <c r="D34" s="89"/>
+      <c r="E34" s="90"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
@@ -3315,21 +3835,21 @@
     </row>
     <row r="38" spans="1:26">
       <c r="A38" s="20"/>
-      <c r="B38" s="86" t="s">
+      <c r="B38" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="87"/>
-      <c r="D38" s="87"/>
-      <c r="E38" s="87"/>
-      <c r="F38" s="87"/>
-      <c r="G38" s="87"/>
-      <c r="H38" s="87"/>
-      <c r="I38" s="87"/>
-      <c r="J38" s="87"/>
-      <c r="K38" s="87"/>
-      <c r="L38" s="87"/>
-      <c r="M38" s="87"/>
-      <c r="N38" s="88"/>
+      <c r="C38" s="89"/>
+      <c r="D38" s="89"/>
+      <c r="E38" s="89"/>
+      <c r="F38" s="89"/>
+      <c r="G38" s="89"/>
+      <c r="H38" s="89"/>
+      <c r="I38" s="89"/>
+      <c r="J38" s="89"/>
+      <c r="K38" s="89"/>
+      <c r="L38" s="89"/>
+      <c r="M38" s="89"/>
+      <c r="N38" s="90"/>
       <c r="O38" s="20"/>
       <c r="P38" s="59"/>
       <c r="Q38" s="59"/>
@@ -3345,16 +3865,16 @@
     </row>
     <row r="39" spans="1:26" ht="15" customHeight="1">
       <c r="A39" s="20"/>
-      <c r="B39" s="109" t="s">
+      <c r="B39" s="94" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="102"/>
-      <c r="D39" s="110"/>
-      <c r="E39" s="111">
+      <c r="C39" s="95"/>
+      <c r="D39" s="96"/>
+      <c r="E39" s="104">
         <f>M32</f>
-        <v>207</v>
+        <v>233</v>
       </c>
-      <c r="F39" s="110"/>
+      <c r="F39" s="96"/>
       <c r="G39" s="60"/>
       <c r="H39" s="61"/>
       <c r="I39" s="61"/>
@@ -3378,16 +3898,16 @@
     </row>
     <row r="40" spans="1:26">
       <c r="A40" s="20"/>
-      <c r="B40" s="109" t="s">
+      <c r="B40" s="94" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="102"/>
-      <c r="D40" s="110"/>
-      <c r="E40" s="119">
+      <c r="C40" s="95"/>
+      <c r="D40" s="96"/>
+      <c r="E40" s="103">
         <f>IF(M32="Completar","Completar",IFERROR(M32/(N32*24),"Error"))</f>
-        <v>62.099999999999945</v>
+        <v>53.976833976833916</v>
       </c>
-      <c r="F40" s="110"/>
+      <c r="F40" s="96"/>
       <c r="G40" s="63"/>
       <c r="H40" s="64"/>
       <c r="I40" s="64"/>
@@ -3411,16 +3931,16 @@
     </row>
     <row r="41" spans="1:26" ht="15" customHeight="1">
       <c r="A41" s="20"/>
-      <c r="B41" s="109" t="s">
+      <c r="B41" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="C41" s="102"/>
-      <c r="D41" s="110"/>
-      <c r="E41" s="111">
+      <c r="C41" s="95"/>
+      <c r="D41" s="96"/>
+      <c r="E41" s="104">
         <f>IF(K32=0,0,IFERROR(ROUNDUP(K32/(M32/100),0),"Error"))</f>
         <v>6</v>
       </c>
-      <c r="F41" s="110"/>
+      <c r="F41" s="96"/>
       <c r="G41" s="63"/>
       <c r="H41" s="64"/>
       <c r="I41" s="64"/>
@@ -3444,16 +3964,16 @@
     </row>
     <row r="42" spans="1:26" ht="15" customHeight="1">
       <c r="A42" s="20"/>
-      <c r="B42" s="109" t="s">
+      <c r="B42" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="C42" s="102"/>
-      <c r="D42" s="110"/>
-      <c r="E42" s="118">
+      <c r="C42" s="95"/>
+      <c r="D42" s="96"/>
+      <c r="E42" s="102">
         <f>IF(K32=0,0,IFERROR(K32/M32,"Error"))</f>
-        <v>5.3140096618357488E-2</v>
+        <v>5.1502145922746781E-2</v>
       </c>
-      <c r="F42" s="110"/>
+      <c r="F42" s="96"/>
       <c r="G42" s="63"/>
       <c r="H42" s="64"/>
       <c r="I42" s="64"/>
@@ -3477,18 +3997,18 @@
     </row>
     <row r="43" spans="1:26" ht="15" customHeight="1">
       <c r="A43" s="20"/>
-      <c r="B43" s="109" t="s">
+      <c r="B43" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="102"/>
-      <c r="D43" s="110"/>
+      <c r="C43" s="95"/>
+      <c r="D43" s="96"/>
       <c r="E43" s="66">
         <f>E5</f>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="F43" s="67">
-        <f t="shared" ref="F43:F46" si="3">IF(E43="Completar",E43,IFERROR(E43/$E$49,"Error"))</f>
-        <v>4.7619047619047408E-2</v>
+        <f t="shared" ref="F43:F46" si="6">IF(E43="Completar",E43,IFERROR(E43/$E$49,"Error"))</f>
+        <v>3.7174721189590899E-2</v>
       </c>
       <c r="G43" s="63"/>
       <c r="H43" s="64"/>
@@ -3513,17 +4033,17 @@
     </row>
     <row r="44" spans="1:26" ht="15" customHeight="1">
       <c r="A44" s="20"/>
-      <c r="B44" s="109" t="s">
+      <c r="B44" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="102"/>
-      <c r="D44" s="110"/>
+      <c r="C44" s="95"/>
+      <c r="D44" s="96"/>
       <c r="E44" s="66" t="str">
         <f>E9</f>
         <v>Completar</v>
       </c>
       <c r="F44" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Completar</v>
       </c>
       <c r="G44" s="63"/>
@@ -3549,17 +4069,17 @@
     </row>
     <row r="45" spans="1:26" ht="15" customHeight="1">
       <c r="A45" s="20"/>
-      <c r="B45" s="109" t="s">
+      <c r="B45" s="94" t="s">
         <v>33</v>
       </c>
-      <c r="C45" s="102"/>
-      <c r="D45" s="110"/>
+      <c r="C45" s="95"/>
+      <c r="D45" s="96"/>
       <c r="E45" s="66" t="str">
         <f>E13</f>
         <v>Completar</v>
       </c>
       <c r="F45" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Completar</v>
       </c>
       <c r="G45" s="63"/>
@@ -3585,17 +4105,17 @@
     </row>
     <row r="46" spans="1:26" ht="15" customHeight="1">
       <c r="A46" s="20"/>
-      <c r="B46" s="109" t="s">
+      <c r="B46" s="94" t="s">
         <v>34</v>
       </c>
-      <c r="C46" s="102"/>
-      <c r="D46" s="110"/>
+      <c r="C46" s="95"/>
+      <c r="D46" s="96"/>
       <c r="E46" s="66" t="str">
         <f>E36</f>
         <v>Completar</v>
       </c>
       <c r="F46" s="67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>Completar</v>
       </c>
       <c r="G46" s="63"/>
@@ -3621,18 +4141,18 @@
     </row>
     <row r="47" spans="1:26" ht="15" customHeight="1">
       <c r="A47" s="20"/>
-      <c r="B47" s="109" t="s">
+      <c r="B47" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="C47" s="102"/>
-      <c r="D47" s="110"/>
+      <c r="C47" s="95"/>
+      <c r="D47" s="96"/>
       <c r="E47" s="66">
         <f>L32</f>
-        <v>2.0833333333333336E-2</v>
+        <v>2.7083333333333334E-2</v>
       </c>
       <c r="F47" s="67">
-        <f t="shared" ref="F47:F48" si="4">IF(E47="Completar",E47,IFERROR(E47/$E$49,"Completar"))</f>
-        <v>0.14285714285714277</v>
+        <f t="shared" ref="F47:F48" si="7">IF(E47="Completar",E47,IFERROR(E47/$E$49,"Completar"))</f>
+        <v>0.14498141263940503</v>
       </c>
       <c r="G47" s="63"/>
       <c r="H47" s="64"/>
@@ -3657,18 +4177,18 @@
     </row>
     <row r="48" spans="1:26" ht="15" customHeight="1">
       <c r="A48" s="20"/>
-      <c r="B48" s="109" t="s">
+      <c r="B48" s="94" t="s">
         <v>36</v>
       </c>
-      <c r="C48" s="102"/>
-      <c r="D48" s="110"/>
+      <c r="C48" s="95"/>
+      <c r="D48" s="96"/>
       <c r="E48" s="66">
         <f>J32</f>
-        <v>0.11805555555555569</v>
+        <v>0.15277777777777801</v>
       </c>
       <c r="F48" s="67">
-        <f t="shared" si="4"/>
-        <v>0.80952380952380976</v>
+        <f t="shared" si="7"/>
+        <v>0.81784386617100402</v>
       </c>
       <c r="G48" s="63"/>
       <c r="H48" s="64"/>
@@ -3693,16 +4213,16 @@
     </row>
     <row r="49" spans="1:26" ht="15" customHeight="1">
       <c r="A49" s="20"/>
-      <c r="B49" s="117" t="s">
+      <c r="B49" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="C49" s="90"/>
-      <c r="D49" s="116"/>
-      <c r="E49" s="115">
+      <c r="C49" s="100"/>
+      <c r="D49" s="98"/>
+      <c r="E49" s="97">
         <f>IF(COUNTIF(E43:E48,"Error")&gt;0,"Error",IF(SUM(E43:E48)=0,"Completar",SUM(E43:E48)))</f>
-        <v>0.14583333333333345</v>
+        <v>0.18680555555555578</v>
       </c>
-      <c r="F49" s="116"/>
+      <c r="F49" s="98"/>
       <c r="G49" s="68"/>
       <c r="H49" s="69"/>
       <c r="I49" s="69"/>
@@ -30522,13 +31042,33 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="D1:N1"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="F8:N8"/>
-    <mergeCell ref="F9:N9"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B38:N38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="B41:D41"/>
     <mergeCell ref="B15:N15"/>
     <mergeCell ref="F12:N12"/>
     <mergeCell ref="F13:N13"/>
@@ -30545,101 +31085,131 @@
     <mergeCell ref="E42:F42"/>
     <mergeCell ref="B42:D42"/>
     <mergeCell ref="E40:F40"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B38:N38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="D1:N1"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F8:N8"/>
+    <mergeCell ref="F9:N9"/>
   </mergeCells>
-  <conditionalFormatting sqref="D1:XFD24 C3:C24 A32:XFD1048576 N25:XFD31 A1:B31">
-    <cfRule type="cellIs" dxfId="13" priority="25" operator="equal">
+  <conditionalFormatting sqref="D1:XFD24 C3:C24 A32:XFD1048576 A1:B31 N25:XFD31">
+    <cfRule type="cellIs" dxfId="29" priority="35" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:XFD24 C3:C24 A32:XFD1048576 N25:XFD31 A1:B31">
-    <cfRule type="cellIs" dxfId="12" priority="26" operator="equal">
+  <conditionalFormatting sqref="D1:XFD24 C3:C24 A32:XFD1048576 A1:B31 N25:XFD31">
+    <cfRule type="cellIs" dxfId="28" priority="36" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:M25 C26:E26">
-    <cfRule type="cellIs" dxfId="11" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="33" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:M25 C26:E26">
-    <cfRule type="cellIs" dxfId="10" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="34" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C31:I31 F26:M26 K31:M31 J27:J31">
-    <cfRule type="cellIs" dxfId="9" priority="17" operator="equal">
+  <conditionalFormatting sqref="F26:M26 K31:M31 C31 F31:I31 J27:J31">
+    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C31:I31 F26:M26 K31:M31 J27:J31">
-    <cfRule type="cellIs" dxfId="8" priority="18" operator="equal">
+  <conditionalFormatting sqref="F26:M26 K31:M31 C31 F31:I31 J27:J31">
+    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:I27 K27:M27">
-    <cfRule type="cellIs" dxfId="7" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="23" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:I27 K27:M27">
-    <cfRule type="cellIs" dxfId="6" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="24" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:I28 K28:M28">
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
+  <conditionalFormatting sqref="K28:M28 C28 F28:I28">
+    <cfRule type="cellIs" dxfId="31" priority="19" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:I28 K28:M28">
-    <cfRule type="cellIs" dxfId="4" priority="10" operator="equal">
+  <conditionalFormatting sqref="K28:M28 C28 F28:I28">
+    <cfRule type="cellIs" dxfId="30" priority="20" operator="equal">
+      <formula>"Error"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K29:M29 C29 F29:I29">
+    <cfRule type="cellIs" dxfId="25" priority="15" operator="equal">
+      <formula>"Completar"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K29:M29 C29 F29:I29">
+    <cfRule type="cellIs" dxfId="24" priority="16" operator="equal">
+      <formula>"Error"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K30:M30 C30 F30:I30">
+    <cfRule type="cellIs" dxfId="33" priority="11" operator="equal">
+      <formula>"Completar"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K30:M30 C30 F30:I30">
+    <cfRule type="cellIs" dxfId="32" priority="12" operator="equal">
+      <formula>"Error"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K28:M28 C28 F28:I28">
+    <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
+      <formula>"Completar"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K28:M28 C28 F28:I28">
+    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+      <formula>"Error"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N29:N30">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
+      <formula>"Completar"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N29:N30">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+      <formula>"Error"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J29:J30">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+      <formula>"Completar"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J29:J30">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:I29 K29:M29">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:I29 K29:M29">
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:I30 K30:M30">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:I30 K30:M30">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Actualizacion planilla Métricas con agregando cuatro métodos
</commit_message>
<xml_diff>
--- a/Documentacion/MatrizMath/MatrizMath - Planilla de Métricas V2.1.xlsx
+++ b/Documentacion/MatrizMath/MatrizMath - Planilla de Métricas V2.1.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BKP ALMIRON\ENZO-AMS\TEIC\Nueva carpeta\PROG III\TP2\TP2-Repo\Documentacion\MatrizMath\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900"/>
   </bookViews>
   <sheets>
     <sheet name="Métricas" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
   <si>
     <t>PROYECTO:</t>
   </si>
@@ -159,16 +164,28 @@
   <si>
     <t>producto(float)</t>
   </si>
+  <si>
+    <t>llevarACeroPosicionesPorArriba()</t>
+  </si>
+  <si>
+    <t>determinanteCuadrada()</t>
+  </si>
+  <si>
+    <t>determinante()</t>
+  </si>
+  <si>
+    <t>diferenciaFilaConMultiploDeOtra()</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -223,6 +240,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -785,7 +809,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1040,6 +1064,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1061,7 +1092,6 @@
     <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1071,7 +1101,10 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1118,482 +1151,78 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="20" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="7" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="7" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="7" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="46">
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC00000"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC00000"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC00000"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC00000"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC00000"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC00000"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC00000"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC00000"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC00000"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC00000"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC00000"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC00000"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC00000"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC00000"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC00000"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <font>
         <color rgb="FFFFFFFF"/>
@@ -1856,9 +1485,18 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -1879,12 +1517,13 @@
           <c:order val="0"/>
           <c:dPt>
             <c:idx val="0"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="FFC000"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-49DD-4FD5-A2AE-26863999DE8F}"/>
               </c:ext>
@@ -1892,12 +1531,13 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="00B0F0"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-49DD-4FD5-A2AE-26863999DE8F}"/>
               </c:ext>
@@ -1905,12 +1545,13 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="0066FF"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-49DD-4FD5-A2AE-26863999DE8F}"/>
               </c:ext>
@@ -1918,12 +1559,13 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="009900"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-49DD-4FD5-A2AE-26863999DE8F}"/>
               </c:ext>
@@ -1931,12 +1573,13 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000009-49DD-4FD5-A2AE-26863999DE8F}"/>
               </c:ext>
@@ -1944,12 +1587,13 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="002060"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000B-49DD-4FD5-A2AE-26863999DE8F}"/>
               </c:ext>
@@ -1957,7 +1601,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Métricas!$B$43:$B$48</c:f>
+              <c:f>Métricas!$B$50:$B$55</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1983,19 +1627,28 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Métricas!$C$43:$C$48</c:f>
+              <c:f>Métricas!$C$50:$C$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000C-49DD-4FD5-A2AE-26863999DE8F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
       <c:spPr>
@@ -2006,7 +1659,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
@@ -2026,13 +1679,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2098,7 +1751,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2133,7 +1786,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2310,21 +1963,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z1006"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z1013"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31:E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
@@ -2340,23 +1993,23 @@
   <sheetData>
     <row r="1" spans="1:26" ht="23.25" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="91" t="s">
+      <c r="B1" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="86" t="s">
+      <c r="C1" s="90"/>
+      <c r="D1" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="90"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -2400,12 +2053,12 @@
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
       <c r="A3" s="4"/>
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="90"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="93"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -2531,12 +2184,12 @@
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1">
       <c r="A7" s="4"/>
-      <c r="B7" s="88" t="s">
+      <c r="B7" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="89"/>
-      <c r="D7" s="89"/>
-      <c r="E7" s="90"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="93"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -2573,15 +2226,15 @@
       <c r="E8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="92"/>
-      <c r="G8" s="87"/>
-      <c r="H8" s="87"/>
-      <c r="I8" s="87"/>
-      <c r="J8" s="87"/>
-      <c r="K8" s="87"/>
-      <c r="L8" s="87"/>
-      <c r="M8" s="87"/>
-      <c r="N8" s="87"/>
+      <c r="F8" s="95"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="90"/>
+      <c r="I8" s="90"/>
+      <c r="J8" s="90"/>
+      <c r="K8" s="90"/>
+      <c r="L8" s="90"/>
+      <c r="M8" s="90"/>
+      <c r="N8" s="90"/>
       <c r="O8" s="7"/>
       <c r="P8" s="13"/>
       <c r="Q8" s="14"/>
@@ -2608,15 +2261,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C9),ISBLANK(D9)),"Completar",IF(D9&gt;=C9,D9-C9,"Error")),"Error")</f>
         <v>Completar</v>
       </c>
-      <c r="F9" s="93"/>
-      <c r="G9" s="87"/>
-      <c r="H9" s="87"/>
-      <c r="I9" s="87"/>
-      <c r="J9" s="87"/>
-      <c r="K9" s="87"/>
-      <c r="L9" s="87"/>
-      <c r="M9" s="87"/>
-      <c r="N9" s="87"/>
+      <c r="F9" s="96"/>
+      <c r="G9" s="90"/>
+      <c r="H9" s="90"/>
+      <c r="I9" s="90"/>
+      <c r="J9" s="90"/>
+      <c r="K9" s="90"/>
+      <c r="L9" s="90"/>
+      <c r="M9" s="90"/>
+      <c r="N9" s="90"/>
       <c r="O9" s="15"/>
       <c r="P9" s="21"/>
       <c r="Q9" s="22"/>
@@ -2660,12 +2313,12 @@
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" s="4"/>
-      <c r="B11" s="88" t="s">
+      <c r="B11" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="89"/>
-      <c r="D11" s="89"/>
-      <c r="E11" s="90"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="92"/>
+      <c r="E11" s="93"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -2702,15 +2355,15 @@
       <c r="E12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="92"/>
-      <c r="G12" s="87"/>
-      <c r="H12" s="87"/>
-      <c r="I12" s="87"/>
-      <c r="J12" s="87"/>
-      <c r="K12" s="87"/>
-      <c r="L12" s="87"/>
-      <c r="M12" s="87"/>
-      <c r="N12" s="87"/>
+      <c r="F12" s="95"/>
+      <c r="G12" s="90"/>
+      <c r="H12" s="90"/>
+      <c r="I12" s="90"/>
+      <c r="J12" s="90"/>
+      <c r="K12" s="90"/>
+      <c r="L12" s="90"/>
+      <c r="M12" s="90"/>
+      <c r="N12" s="90"/>
       <c r="O12" s="7"/>
       <c r="P12" s="13"/>
       <c r="Q12" s="14"/>
@@ -2735,15 +2388,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C13),ISBLANK(D13)),"Completar",IF(D13&gt;=C13,D13-C13,"Error")),"Error")</f>
         <v>Completar</v>
       </c>
-      <c r="F13" s="93"/>
-      <c r="G13" s="87"/>
-      <c r="H13" s="87"/>
-      <c r="I13" s="87"/>
-      <c r="J13" s="87"/>
-      <c r="K13" s="87"/>
-      <c r="L13" s="87"/>
-      <c r="M13" s="87"/>
-      <c r="N13" s="87"/>
+      <c r="F13" s="96"/>
+      <c r="G13" s="90"/>
+      <c r="H13" s="90"/>
+      <c r="I13" s="90"/>
+      <c r="J13" s="90"/>
+      <c r="K13" s="90"/>
+      <c r="L13" s="90"/>
+      <c r="M13" s="90"/>
+      <c r="N13" s="90"/>
       <c r="O13" s="15"/>
       <c r="P13" s="21"/>
       <c r="Q13" s="22"/>
@@ -2787,21 +2440,21 @@
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1">
       <c r="A15" s="4"/>
-      <c r="B15" s="88" t="s">
+      <c r="B15" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="89"/>
-      <c r="D15" s="89"/>
-      <c r="E15" s="89"/>
-      <c r="F15" s="89"/>
-      <c r="G15" s="89"/>
-      <c r="H15" s="89"/>
-      <c r="I15" s="89"/>
-      <c r="J15" s="89"/>
-      <c r="K15" s="89"/>
-      <c r="L15" s="89"/>
-      <c r="M15" s="89"/>
-      <c r="N15" s="90"/>
+      <c r="C15" s="92"/>
+      <c r="D15" s="92"/>
+      <c r="E15" s="92"/>
+      <c r="F15" s="92"/>
+      <c r="G15" s="92"/>
+      <c r="H15" s="92"/>
+      <c r="I15" s="92"/>
+      <c r="J15" s="92"/>
+      <c r="K15" s="92"/>
+      <c r="L15" s="92"/>
+      <c r="M15" s="92"/>
+      <c r="N15" s="93"/>
       <c r="O15" s="4"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
@@ -2817,31 +2470,31 @@
     </row>
     <row r="16" spans="1:26" ht="16.5" customHeight="1">
       <c r="A16" s="7"/>
-      <c r="B16" s="116" t="s">
+      <c r="B16" s="119" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="118" t="s">
+      <c r="C16" s="121" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="119"/>
-      <c r="E16" s="119"/>
-      <c r="F16" s="111" t="s">
+      <c r="D16" s="122"/>
+      <c r="E16" s="122"/>
+      <c r="F16" s="114" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="112"/>
-      <c r="H16" s="110" t="s">
+      <c r="G16" s="115"/>
+      <c r="H16" s="113" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="95"/>
-      <c r="J16" s="95"/>
-      <c r="K16" s="111" t="s">
+      <c r="I16" s="88"/>
+      <c r="J16" s="88"/>
+      <c r="K16" s="114" t="s">
         <v>14</v>
       </c>
-      <c r="L16" s="112"/>
-      <c r="M16" s="114" t="s">
+      <c r="L16" s="115"/>
+      <c r="M16" s="117" t="s">
         <v>15</v>
       </c>
-      <c r="N16" s="105" t="s">
+      <c r="N16" s="108" t="s">
         <v>6</v>
       </c>
       <c r="O16" s="7"/>
@@ -2859,10 +2512,10 @@
     </row>
     <row r="17" spans="1:26" ht="30" customHeight="1">
       <c r="A17" s="7"/>
-      <c r="B17" s="117"/>
-      <c r="C17" s="120"/>
-      <c r="D17" s="121"/>
-      <c r="E17" s="121"/>
+      <c r="B17" s="120"/>
+      <c r="C17" s="123"/>
+      <c r="D17" s="124"/>
+      <c r="E17" s="124"/>
       <c r="F17" s="26" t="s">
         <v>16</v>
       </c>
@@ -2884,8 +2537,8 @@
       <c r="L17" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="M17" s="115"/>
-      <c r="N17" s="106"/>
+      <c r="M17" s="118"/>
+      <c r="N17" s="109"/>
       <c r="O17" s="7"/>
       <c r="P17" s="13"/>
       <c r="Q17" s="14"/>
@@ -2902,14 +2555,14 @@
     <row r="18" spans="1:26">
       <c r="A18" s="15"/>
       <c r="B18" s="30">
-        <f t="shared" ref="B18:B31" si="0">ROW($B18)-16</f>
+        <f t="shared" ref="B18:B38" si="0">ROW($B18)-16</f>
         <v>2</v>
       </c>
-      <c r="C18" s="107" t="s">
+      <c r="C18" s="110" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="95"/>
-      <c r="E18" s="95"/>
+      <c r="D18" s="88"/>
+      <c r="E18" s="88"/>
       <c r="F18" s="31">
         <v>60</v>
       </c>
@@ -2923,7 +2576,7 @@
         <v>0.68819444444444444</v>
       </c>
       <c r="J18" s="35">
-        <f t="shared" ref="J18:J31" si="1">IFERROR(IF(OR(ISBLANK(H18),ISBLANK(I18)),"",IF(I18&gt;=H18,I18-H18,"Error")),"Error")</f>
+        <f t="shared" ref="J18:J27" si="1">IFERROR(IF(OR(ISBLANK(H18),ISBLANK(I18)),"",IF(I18&gt;=H18,I18-H18,"Error")),"Error")</f>
         <v>2.1527777777777812E-2</v>
       </c>
       <c r="K18" s="36">
@@ -2936,7 +2589,7 @@
         <v>55</v>
       </c>
       <c r="N18" s="39">
-        <f t="shared" ref="N18:N31" si="2">IFERROR(IF(OR(J18="",ISBLANK(L18)),"",J18+L18),"Error")</f>
+        <f t="shared" ref="N18:N27" si="2">IFERROR(IF(OR(J18="",ISBLANK(L18)),"",J18+L18),"Error")</f>
         <v>2.9166666666666702E-2</v>
       </c>
       <c r="O18" s="15"/>
@@ -2958,11 +2611,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C19" s="107" t="s">
+      <c r="C19" s="110" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="95"/>
-      <c r="E19" s="95"/>
+      <c r="D19" s="88"/>
+      <c r="E19" s="88"/>
       <c r="F19" s="31">
         <v>4</v>
       </c>
@@ -3011,11 +2664,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C20" s="107" t="s">
+      <c r="C20" s="110" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="95"/>
-      <c r="E20" s="95"/>
+      <c r="D20" s="88"/>
+      <c r="E20" s="88"/>
       <c r="F20" s="31">
         <v>8</v>
       </c>
@@ -3064,11 +2717,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C21" s="107" t="s">
+      <c r="C21" s="110" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="95"/>
-      <c r="E21" s="95"/>
+      <c r="D21" s="88"/>
+      <c r="E21" s="88"/>
       <c r="F21" s="31">
         <v>10</v>
       </c>
@@ -3117,11 +2770,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C22" s="108" t="s">
+      <c r="C22" s="111" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="109"/>
-      <c r="E22" s="109"/>
+      <c r="D22" s="112"/>
+      <c r="E22" s="112"/>
       <c r="F22" s="74">
         <v>8</v>
       </c>
@@ -3170,11 +2823,11 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C23" s="101" t="s">
+      <c r="C23" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="95"/>
-      <c r="E23" s="95"/>
+      <c r="D23" s="88"/>
+      <c r="E23" s="88"/>
       <c r="F23" s="42">
         <v>13</v>
       </c>
@@ -3223,11 +2876,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C24" s="101" t="s">
+      <c r="C24" s="87" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="95"/>
-      <c r="E24" s="95"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="88"/>
       <c r="F24" s="42">
         <v>25</v>
       </c>
@@ -3276,11 +2929,11 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C25" s="101" t="s">
+      <c r="C25" s="87" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="95"/>
-      <c r="E25" s="95"/>
+      <c r="D25" s="88"/>
+      <c r="E25" s="88"/>
       <c r="F25" s="42">
         <v>20</v>
       </c>
@@ -3329,11 +2982,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C26" s="101" t="s">
+      <c r="C26" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="95"/>
-      <c r="E26" s="95"/>
+      <c r="D26" s="88"/>
+      <c r="E26" s="88"/>
       <c r="F26" s="42">
         <v>16</v>
       </c>
@@ -3382,11 +3035,11 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C27" s="101" t="s">
+      <c r="C27" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="95"/>
-      <c r="E27" s="95"/>
+      <c r="D27" s="88"/>
+      <c r="E27" s="88"/>
       <c r="F27" s="42">
         <v>30</v>
       </c>
@@ -3435,11 +3088,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C28" s="101" t="s">
+      <c r="C28" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="122"/>
-      <c r="E28" s="123"/>
+      <c r="D28" s="103"/>
+      <c r="E28" s="104"/>
       <c r="F28" s="42">
         <v>18</v>
       </c>
@@ -3466,7 +3119,7 @@
         <v>21</v>
       </c>
       <c r="N28" s="39">
-        <f t="shared" ref="N28:N30" si="4">IFERROR(IF(OR(J28="",ISBLANK(L28)),"",J28+L28),"Error")</f>
+        <f t="shared" ref="N28:N38" si="4">IFERROR(IF(OR(J28="",ISBLANK(L28)),"",J28+L28),"Error")</f>
         <v>1.3194444444444519E-2</v>
       </c>
       <c r="O28" s="71"/>
@@ -3488,11 +3141,11 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C29" s="101" t="s">
+      <c r="C29" s="87" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="95"/>
-      <c r="E29" s="95"/>
+      <c r="D29" s="88"/>
+      <c r="E29" s="88"/>
       <c r="F29" s="42">
         <v>30</v>
       </c>
@@ -3541,11 +3194,11 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C30" s="101" t="s">
+      <c r="C30" s="87" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="95"/>
-      <c r="E30" s="95"/>
+      <c r="D30" s="88"/>
+      <c r="E30" s="88"/>
       <c r="F30" s="42">
         <v>15</v>
       </c>
@@ -3559,7 +3212,7 @@
         <v>0.99791666666666667</v>
       </c>
       <c r="J30" s="35">
-        <f t="shared" ref="J30" si="5">IFERROR(IF(OR(ISBLANK(H30),ISBLANK(I30)),"",IF(I30&gt;=H30,I30-H30,"Error")),"Error")</f>
+        <f t="shared" ref="J30:J38" si="5">IFERROR(IF(OR(ISBLANK(H30),ISBLANK(I30)),"",IF(I30&gt;=H30,I30-H30,"Error")),"Error")</f>
         <v>4.1666666666666519E-3</v>
       </c>
       <c r="K30" s="46">
@@ -3589,30 +3242,44 @@
       <c r="Z30" s="22"/>
     </row>
     <row r="31" spans="1:26" ht="15" customHeight="1">
-      <c r="A31" s="71"/>
+      <c r="A31" s="86"/>
       <c r="B31" s="30">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C31" s="101"/>
-      <c r="D31" s="122"/>
-      <c r="E31" s="123"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="44"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="C31" s="87" t="s">
+        <v>48</v>
       </c>
-      <c r="K31" s="46"/>
-      <c r="L31" s="47"/>
-      <c r="M31" s="48"/>
-      <c r="N31" s="39" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+      <c r="D31" s="103"/>
+      <c r="E31" s="104"/>
+      <c r="F31" s="125">
+        <v>17</v>
       </c>
-      <c r="O31" s="71"/>
+      <c r="G31" s="132">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="H31" s="126">
+        <v>3.0555555555555555E-2</v>
+      </c>
+      <c r="I31" s="127">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="J31" s="128">
+        <v>1.4583333333333171E-2</v>
+      </c>
+      <c r="K31" s="129">
+        <v>0</v>
+      </c>
+      <c r="L31" s="133">
+        <v>0</v>
+      </c>
+      <c r="M31" s="130">
+        <v>17</v>
+      </c>
+      <c r="N31" s="131">
+        <v>1.4583333333333171E-2</v>
+      </c>
+      <c r="O31" s="86"/>
       <c r="P31" s="21"/>
       <c r="Q31" s="22"/>
       <c r="R31" s="22"/>
@@ -3625,174 +3292,221 @@
       <c r="Y31" s="22"/>
       <c r="Z31" s="22"/>
     </row>
-    <row r="32" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A32" s="7"/>
-      <c r="B32" s="113" t="s">
-        <v>23</v>
+    <row r="32" spans="1:26" s="147" customFormat="1" ht="15" customHeight="1">
+      <c r="A32" s="134"/>
+      <c r="B32" s="135">
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
-      <c r="C32" s="100"/>
-      <c r="D32" s="100"/>
-      <c r="E32" s="100"/>
-      <c r="F32" s="49">
-        <f>IF(SUM(F18:F31)=0,"Completar",SUM(F18:F31))</f>
-        <v>257</v>
+      <c r="C32" s="111" t="s">
+        <v>49</v>
       </c>
-      <c r="G32" s="50">
-        <f>IF(SUM(G18:G31)=0,"Completar",SUM(G18:G31))</f>
-        <v>0.16388888888888886</v>
+      <c r="D32" s="112"/>
+      <c r="E32" s="112"/>
+      <c r="F32" s="136">
+        <v>20</v>
       </c>
-      <c r="H32" s="51" t="s">
-        <v>24</v>
+      <c r="G32" s="137">
+        <v>2.0833333333333332E-2</v>
       </c>
-      <c r="I32" s="52" t="s">
-        <v>24</v>
+      <c r="H32" s="138">
+        <v>0.41388888888888892</v>
       </c>
-      <c r="J32" s="53">
-        <f>IF(OR(COUNTIF(J18:J31,"Error")&gt;0,COUNTIF(J18:J31,"Completar")&gt;0),"Error",IF(SUM(J18:J31)=0,"Completar",SUM(J18:J31)))</f>
-        <v>0.15277777777777801</v>
+      <c r="I32" s="139">
+        <v>0.43541666666666662</v>
       </c>
-      <c r="K32" s="54">
-        <f>SUM(K18:K31)</f>
-        <v>12</v>
+      <c r="J32" s="140">
+        <v>2.1527777777777701E-2</v>
       </c>
-      <c r="L32" s="50">
-        <f>SUM(L18:L31)</f>
-        <v>2.7083333333333334E-2</v>
+      <c r="K32" s="141">
+        <v>1</v>
       </c>
-      <c r="M32" s="55">
-        <f>IF(SUM(M18:M31)=0,"Completar",SUM(M18:M31))</f>
-        <v>233</v>
+      <c r="L32" s="142">
+        <v>1.3888888888888889E-3</v>
       </c>
-      <c r="N32" s="18">
-        <f>IF(OR(COUNTIF(N18:N31,"Error")&gt;0,COUNTIF(N18:N31,"Completar")&gt;0),"Error",IF(SUM(N18:N31)=0,"Completar",SUM(N18:N31)))</f>
-        <v>0.17986111111111133</v>
+      <c r="M32" s="143">
+        <v>13</v>
       </c>
-      <c r="O32" s="7"/>
-      <c r="P32" s="56"/>
-      <c r="Q32" s="57"/>
-      <c r="R32" s="57"/>
-      <c r="S32" s="57"/>
-      <c r="T32" s="57"/>
-      <c r="U32" s="57"/>
-      <c r="V32" s="57"/>
-      <c r="W32" s="57"/>
-      <c r="X32" s="57"/>
-      <c r="Y32" s="57"/>
-      <c r="Z32" s="57"/>
-    </row>
-    <row r="33" spans="1:26" ht="6" customHeight="1">
-      <c r="A33" s="20"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="20"/>
-      <c r="M33" s="20"/>
-      <c r="N33" s="20"/>
-      <c r="O33" s="20"/>
-      <c r="P33" s="23"/>
-      <c r="Q33" s="23"/>
-      <c r="R33" s="23"/>
-      <c r="S33" s="23"/>
-      <c r="T33" s="23"/>
-      <c r="U33" s="23"/>
-      <c r="V33" s="23"/>
-      <c r="W33" s="23"/>
-      <c r="X33" s="23"/>
-      <c r="Y33" s="23"/>
-      <c r="Z33" s="23"/>
-    </row>
-    <row r="34" spans="1:26" ht="15" customHeight="1">
-      <c r="A34" s="4"/>
-      <c r="B34" s="88" t="s">
-        <v>25</v>
+      <c r="N32" s="144">
+        <v>2.2916666666666589E-2</v>
       </c>
-      <c r="C34" s="89"/>
-      <c r="D34" s="89"/>
-      <c r="E34" s="90"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
-      <c r="M34" s="5"/>
-      <c r="N34" s="5"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="6"/>
-      <c r="Q34" s="6"/>
-      <c r="R34" s="6"/>
-      <c r="S34" s="6"/>
-      <c r="T34" s="6"/>
-      <c r="U34" s="6"/>
-      <c r="V34" s="6"/>
-      <c r="W34" s="6"/>
-      <c r="X34" s="6"/>
-      <c r="Y34" s="6"/>
-      <c r="Z34" s="6"/>
-    </row>
-    <row r="35" spans="1:26" ht="30" customHeight="1">
-      <c r="A35" s="7"/>
-      <c r="B35" s="8" t="s">
-        <v>3</v>
+      <c r="O32" s="134"/>
+      <c r="P32" s="145"/>
+      <c r="Q32" s="146"/>
+      <c r="R32" s="146"/>
+      <c r="S32" s="146"/>
+      <c r="T32" s="146"/>
+      <c r="U32" s="146"/>
+      <c r="V32" s="146"/>
+      <c r="W32" s="146"/>
+      <c r="X32" s="146"/>
+      <c r="Y32" s="146"/>
+      <c r="Z32" s="146"/>
+    </row>
+    <row r="33" spans="1:26" s="147" customFormat="1" ht="15" customHeight="1">
+      <c r="A33" s="134"/>
+      <c r="B33" s="135">
+        <f t="shared" si="0"/>
+        <v>17</v>
       </c>
-      <c r="C35" s="9" t="s">
-        <v>4</v>
+      <c r="C33" s="111" t="s">
+        <v>50</v>
       </c>
-      <c r="D35" s="9" t="s">
-        <v>5</v>
+      <c r="D33" s="112"/>
+      <c r="E33" s="112"/>
+      <c r="F33" s="136">
+        <v>18</v>
       </c>
-      <c r="E35" s="10" t="s">
-        <v>6</v>
+      <c r="G33" s="137">
+        <v>1.3888888888888888E-2</v>
       </c>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="7"/>
-      <c r="K35" s="7"/>
-      <c r="L35" s="7"/>
-      <c r="M35" s="7"/>
-      <c r="N35" s="7"/>
-      <c r="O35" s="7"/>
-      <c r="P35" s="13"/>
-      <c r="Q35" s="14"/>
-      <c r="R35" s="14"/>
-      <c r="S35" s="14"/>
-      <c r="T35" s="14"/>
-      <c r="U35" s="14"/>
-      <c r="V35" s="14"/>
-      <c r="W35" s="14"/>
-      <c r="X35" s="14"/>
-      <c r="Y35" s="14"/>
-      <c r="Z35" s="14"/>
-    </row>
-    <row r="36" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A36" s="15"/>
-      <c r="B36" s="58"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="18" t="str">
-        <f>IFERROR(IF(OR(ISBLANK(C36),ISBLANK(D36)),"Completar",IF(D36&gt;=C36,D36-C36,"Error")),"Error")</f>
-        <v>Completar</v>
+      <c r="H33" s="138">
+        <v>0.43611111111111112</v>
       </c>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="15"/>
-      <c r="O36" s="15"/>
+      <c r="I33" s="139">
+        <v>0.4597222222222222</v>
+      </c>
+      <c r="J33" s="140">
+        <v>2.3611111111111083E-2</v>
+      </c>
+      <c r="K33" s="141">
+        <v>0</v>
+      </c>
+      <c r="L33" s="142">
+        <v>0</v>
+      </c>
+      <c r="M33" s="143">
+        <v>14</v>
+      </c>
+      <c r="N33" s="144">
+        <v>2.3611111111111083E-2</v>
+      </c>
+      <c r="O33" s="134"/>
+      <c r="P33" s="145"/>
+      <c r="Q33" s="146"/>
+      <c r="R33" s="146"/>
+      <c r="S33" s="146"/>
+      <c r="T33" s="146"/>
+      <c r="U33" s="146"/>
+      <c r="V33" s="146"/>
+      <c r="W33" s="146"/>
+      <c r="X33" s="146"/>
+      <c r="Y33" s="146"/>
+      <c r="Z33" s="146"/>
+    </row>
+    <row r="34" spans="1:26" s="147" customFormat="1" ht="15" customHeight="1">
+      <c r="A34" s="134"/>
+      <c r="B34" s="135">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C34" s="111" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="112"/>
+      <c r="E34" s="112"/>
+      <c r="F34" s="136">
+        <v>20</v>
+      </c>
+      <c r="G34" s="137">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H34" s="138">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="I34" s="139">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="J34" s="140">
+        <v>1.736111111111116E-2</v>
+      </c>
+      <c r="K34" s="141">
+        <v>1</v>
+      </c>
+      <c r="L34" s="142">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="M34" s="143">
+        <v>15</v>
+      </c>
+      <c r="N34" s="144">
+        <v>1.9444444444444493E-2</v>
+      </c>
+      <c r="O34" s="134"/>
+      <c r="P34" s="145"/>
+      <c r="Q34" s="146"/>
+      <c r="R34" s="146"/>
+      <c r="S34" s="146"/>
+      <c r="T34" s="146"/>
+      <c r="U34" s="146"/>
+      <c r="V34" s="146"/>
+      <c r="W34" s="146"/>
+      <c r="X34" s="146"/>
+      <c r="Y34" s="146"/>
+      <c r="Z34" s="146"/>
+    </row>
+    <row r="35" spans="1:26" ht="15" customHeight="1">
+      <c r="A35" s="86"/>
+      <c r="B35" s="30">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C35" s="87"/>
+      <c r="D35" s="88"/>
+      <c r="E35" s="88"/>
+      <c r="F35" s="42"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="K35" s="46"/>
+      <c r="L35" s="47"/>
+      <c r="M35" s="48"/>
+      <c r="N35" s="39" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="O35" s="86"/>
+      <c r="P35" s="21"/>
+      <c r="Q35" s="22"/>
+      <c r="R35" s="22"/>
+      <c r="S35" s="22"/>
+      <c r="T35" s="22"/>
+      <c r="U35" s="22"/>
+      <c r="V35" s="22"/>
+      <c r="W35" s="22"/>
+      <c r="X35" s="22"/>
+      <c r="Y35" s="22"/>
+      <c r="Z35" s="22"/>
+    </row>
+    <row r="36" spans="1:26" ht="15" customHeight="1">
+      <c r="A36" s="86"/>
+      <c r="B36" s="30">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C36" s="87"/>
+      <c r="D36" s="88"/>
+      <c r="E36" s="88"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="44"/>
+      <c r="I36" s="45"/>
+      <c r="J36" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="K36" s="46"/>
+      <c r="L36" s="47"/>
+      <c r="M36" s="48"/>
+      <c r="N36" s="39" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="O36" s="86"/>
       <c r="P36" s="21"/>
       <c r="Q36" s="22"/>
       <c r="R36" s="22"/>
@@ -3805,291 +3519,305 @@
       <c r="Y36" s="22"/>
       <c r="Z36" s="22"/>
     </row>
-    <row r="37" spans="1:26" ht="6" customHeight="1">
-      <c r="A37" s="20"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="20"/>
-      <c r="L37" s="20"/>
-      <c r="M37" s="20"/>
-      <c r="N37" s="20"/>
-      <c r="O37" s="20"/>
-      <c r="P37" s="23"/>
-      <c r="Q37" s="23"/>
-      <c r="R37" s="23"/>
-      <c r="S37" s="23"/>
-      <c r="T37" s="23"/>
-      <c r="U37" s="23"/>
-      <c r="V37" s="23"/>
-      <c r="W37" s="23"/>
-      <c r="X37" s="23"/>
-      <c r="Y37" s="23"/>
-      <c r="Z37" s="23"/>
-    </row>
-    <row r="38" spans="1:26">
-      <c r="A38" s="20"/>
-      <c r="B38" s="88" t="s">
+    <row r="37" spans="1:26" ht="15" customHeight="1">
+      <c r="A37" s="86"/>
+      <c r="B37" s="30">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C37" s="87"/>
+      <c r="D37" s="88"/>
+      <c r="E37" s="88"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="43"/>
+      <c r="H37" s="44"/>
+      <c r="I37" s="45"/>
+      <c r="J37" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="K37" s="46"/>
+      <c r="L37" s="47"/>
+      <c r="M37" s="48"/>
+      <c r="N37" s="39" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="O37" s="86"/>
+      <c r="P37" s="21"/>
+      <c r="Q37" s="22"/>
+      <c r="R37" s="22"/>
+      <c r="S37" s="22"/>
+      <c r="T37" s="22"/>
+      <c r="U37" s="22"/>
+      <c r="V37" s="22"/>
+      <c r="W37" s="22"/>
+      <c r="X37" s="22"/>
+      <c r="Y37" s="22"/>
+      <c r="Z37" s="22"/>
+    </row>
+    <row r="38" spans="1:26" ht="15" customHeight="1">
+      <c r="A38" s="71"/>
+      <c r="B38" s="30">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="C38" s="87"/>
+      <c r="D38" s="103"/>
+      <c r="E38" s="104"/>
+      <c r="F38" s="42"/>
+      <c r="G38" s="43"/>
+      <c r="H38" s="44"/>
+      <c r="I38" s="45"/>
+      <c r="J38" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="K38" s="46"/>
+      <c r="L38" s="47"/>
+      <c r="M38" s="48"/>
+      <c r="N38" s="39" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="O38" s="71"/>
+      <c r="P38" s="21"/>
+      <c r="Q38" s="22"/>
+      <c r="R38" s="22"/>
+      <c r="S38" s="22"/>
+      <c r="T38" s="22"/>
+      <c r="U38" s="22"/>
+      <c r="V38" s="22"/>
+      <c r="W38" s="22"/>
+      <c r="X38" s="22"/>
+      <c r="Y38" s="22"/>
+      <c r="Z38" s="22"/>
+    </row>
+    <row r="39" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A39" s="7"/>
+      <c r="B39" s="116" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="102"/>
+      <c r="D39" s="102"/>
+      <c r="E39" s="102"/>
+      <c r="F39" s="49">
+        <f>IF(SUM(F18:F38)=0,"Completar",SUM(F18:F38))</f>
+        <v>332</v>
+      </c>
+      <c r="G39" s="50">
+        <f>IF(SUM(G18:G38)=0,"Completar",SUM(G18:G38))</f>
+        <v>0.24374999999999999</v>
+      </c>
+      <c r="H39" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I39" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="J39" s="53">
+        <f>IF(OR(COUNTIF(J18:J38,"Error")&gt;0,COUNTIF(J18:J38,"Completar")&gt;0),"Error",IF(SUM(J18:J38)=0,"Completar",SUM(J18:J38)))</f>
+        <v>0.22986111111111113</v>
+      </c>
+      <c r="K39" s="54">
+        <f>SUM(K18:K38)</f>
+        <v>14</v>
+      </c>
+      <c r="L39" s="50">
+        <f>SUM(L18:L38)</f>
+        <v>3.0555555555555555E-2</v>
+      </c>
+      <c r="M39" s="55">
+        <f>IF(SUM(M18:M38)=0,"Completar",SUM(M18:M38))</f>
+        <v>292</v>
+      </c>
+      <c r="N39" s="18">
+        <f>IF(OR(COUNTIF(N18:N38,"Error")&gt;0,COUNTIF(N18:N38,"Completar")&gt;0),"Error",IF(SUM(N18:N38)=0,"Completar",SUM(N18:N38)))</f>
+        <v>0.26041666666666669</v>
+      </c>
+      <c r="O39" s="7"/>
+      <c r="P39" s="56"/>
+      <c r="Q39" s="57"/>
+      <c r="R39" s="57"/>
+      <c r="S39" s="57"/>
+      <c r="T39" s="57"/>
+      <c r="U39" s="57"/>
+      <c r="V39" s="57"/>
+      <c r="W39" s="57"/>
+      <c r="X39" s="57"/>
+      <c r="Y39" s="57"/>
+      <c r="Z39" s="57"/>
+    </row>
+    <row r="40" spans="1:26" ht="6" customHeight="1">
+      <c r="A40" s="20"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
+      <c r="L40" s="20"/>
+      <c r="M40" s="20"/>
+      <c r="N40" s="20"/>
+      <c r="O40" s="20"/>
+      <c r="P40" s="23"/>
+      <c r="Q40" s="23"/>
+      <c r="R40" s="23"/>
+      <c r="S40" s="23"/>
+      <c r="T40" s="23"/>
+      <c r="U40" s="23"/>
+      <c r="V40" s="23"/>
+      <c r="W40" s="23"/>
+      <c r="X40" s="23"/>
+      <c r="Y40" s="23"/>
+      <c r="Z40" s="23"/>
+    </row>
+    <row r="41" spans="1:26" ht="15" customHeight="1">
+      <c r="A41" s="4"/>
+      <c r="B41" s="91" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="92"/>
+      <c r="D41" s="92"/>
+      <c r="E41" s="93"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+      <c r="N41" s="5"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="6"/>
+      <c r="Q41" s="6"/>
+      <c r="R41" s="6"/>
+      <c r="S41" s="6"/>
+      <c r="T41" s="6"/>
+      <c r="U41" s="6"/>
+      <c r="V41" s="6"/>
+      <c r="W41" s="6"/>
+      <c r="X41" s="6"/>
+      <c r="Y41" s="6"/>
+      <c r="Z41" s="6"/>
+    </row>
+    <row r="42" spans="1:26" ht="30" customHeight="1">
+      <c r="A42" s="7"/>
+      <c r="B42" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="13"/>
+      <c r="Q42" s="14"/>
+      <c r="R42" s="14"/>
+      <c r="S42" s="14"/>
+      <c r="T42" s="14"/>
+      <c r="U42" s="14"/>
+      <c r="V42" s="14"/>
+      <c r="W42" s="14"/>
+      <c r="X42" s="14"/>
+      <c r="Y42" s="14"/>
+      <c r="Z42" s="14"/>
+    </row>
+    <row r="43" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A43" s="15"/>
+      <c r="B43" s="58"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="18" t="str">
+        <f>IFERROR(IF(OR(ISBLANK(C43),ISBLANK(D43)),"Completar",IF(D43&gt;=C43,D43-C43,"Error")),"Error")</f>
+        <v>Completar</v>
+      </c>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="15"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="15"/>
+      <c r="O43" s="15"/>
+      <c r="P43" s="21"/>
+      <c r="Q43" s="22"/>
+      <c r="R43" s="22"/>
+      <c r="S43" s="22"/>
+      <c r="T43" s="22"/>
+      <c r="U43" s="22"/>
+      <c r="V43" s="22"/>
+      <c r="W43" s="22"/>
+      <c r="X43" s="22"/>
+      <c r="Y43" s="22"/>
+      <c r="Z43" s="22"/>
+    </row>
+    <row r="44" spans="1:26" ht="6" customHeight="1">
+      <c r="A44" s="20"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="20"/>
+      <c r="L44" s="20"/>
+      <c r="M44" s="20"/>
+      <c r="N44" s="20"/>
+      <c r="O44" s="20"/>
+      <c r="P44" s="23"/>
+      <c r="Q44" s="23"/>
+      <c r="R44" s="23"/>
+      <c r="S44" s="23"/>
+      <c r="T44" s="23"/>
+      <c r="U44" s="23"/>
+      <c r="V44" s="23"/>
+      <c r="W44" s="23"/>
+      <c r="X44" s="23"/>
+      <c r="Y44" s="23"/>
+      <c r="Z44" s="23"/>
+    </row>
+    <row r="45" spans="1:26">
+      <c r="A45" s="20"/>
+      <c r="B45" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="89"/>
-      <c r="D38" s="89"/>
-      <c r="E38" s="89"/>
-      <c r="F38" s="89"/>
-      <c r="G38" s="89"/>
-      <c r="H38" s="89"/>
-      <c r="I38" s="89"/>
-      <c r="J38" s="89"/>
-      <c r="K38" s="89"/>
-      <c r="L38" s="89"/>
-      <c r="M38" s="89"/>
-      <c r="N38" s="90"/>
-      <c r="O38" s="20"/>
-      <c r="P38" s="59"/>
-      <c r="Q38" s="59"/>
-      <c r="R38" s="59"/>
-      <c r="S38" s="59"/>
-      <c r="T38" s="59"/>
-      <c r="U38" s="59"/>
-      <c r="V38" s="59"/>
-      <c r="W38" s="59"/>
-      <c r="X38" s="59"/>
-      <c r="Y38" s="59"/>
-      <c r="Z38" s="59"/>
-    </row>
-    <row r="39" spans="1:26" ht="15" customHeight="1">
-      <c r="A39" s="20"/>
-      <c r="B39" s="94" t="s">
-        <v>27</v>
-      </c>
-      <c r="C39" s="95"/>
-      <c r="D39" s="96"/>
-      <c r="E39" s="104">
-        <f>M32</f>
-        <v>233</v>
-      </c>
-      <c r="F39" s="96"/>
-      <c r="G39" s="60"/>
-      <c r="H39" s="61"/>
-      <c r="I39" s="61"/>
-      <c r="J39" s="61"/>
-      <c r="K39" s="61"/>
-      <c r="L39" s="61"/>
-      <c r="M39" s="61"/>
-      <c r="N39" s="62"/>
-      <c r="O39" s="20"/>
-      <c r="P39" s="59"/>
-      <c r="Q39" s="59"/>
-      <c r="R39" s="59"/>
-      <c r="S39" s="59"/>
-      <c r="T39" s="59"/>
-      <c r="U39" s="59"/>
-      <c r="V39" s="59"/>
-      <c r="W39" s="59"/>
-      <c r="X39" s="59"/>
-      <c r="Y39" s="59"/>
-      <c r="Z39" s="59"/>
-    </row>
-    <row r="40" spans="1:26">
-      <c r="A40" s="20"/>
-      <c r="B40" s="94" t="s">
-        <v>28</v>
-      </c>
-      <c r="C40" s="95"/>
-      <c r="D40" s="96"/>
-      <c r="E40" s="103">
-        <f>IF(M32="Completar","Completar",IFERROR(M32/(N32*24),"Error"))</f>
-        <v>53.976833976833916</v>
-      </c>
-      <c r="F40" s="96"/>
-      <c r="G40" s="63"/>
-      <c r="H40" s="64"/>
-      <c r="I40" s="64"/>
-      <c r="J40" s="64"/>
-      <c r="K40" s="64"/>
-      <c r="L40" s="64"/>
-      <c r="M40" s="64"/>
-      <c r="N40" s="65"/>
-      <c r="O40" s="20"/>
-      <c r="P40" s="59"/>
-      <c r="Q40" s="59"/>
-      <c r="R40" s="59"/>
-      <c r="S40" s="59"/>
-      <c r="T40" s="59"/>
-      <c r="U40" s="59"/>
-      <c r="V40" s="59"/>
-      <c r="W40" s="59"/>
-      <c r="X40" s="59"/>
-      <c r="Y40" s="59"/>
-      <c r="Z40" s="59"/>
-    </row>
-    <row r="41" spans="1:26" ht="15" customHeight="1">
-      <c r="A41" s="20"/>
-      <c r="B41" s="94" t="s">
-        <v>29</v>
-      </c>
-      <c r="C41" s="95"/>
-      <c r="D41" s="96"/>
-      <c r="E41" s="104">
-        <f>IF(K32=0,0,IFERROR(ROUNDUP(K32/(M32/100),0),"Error"))</f>
-        <v>6</v>
-      </c>
-      <c r="F41" s="96"/>
-      <c r="G41" s="63"/>
-      <c r="H41" s="64"/>
-      <c r="I41" s="64"/>
-      <c r="J41" s="64"/>
-      <c r="K41" s="64"/>
-      <c r="L41" s="64"/>
-      <c r="M41" s="64"/>
-      <c r="N41" s="65"/>
-      <c r="O41" s="20"/>
-      <c r="P41" s="59"/>
-      <c r="Q41" s="59"/>
-      <c r="R41" s="59"/>
-      <c r="S41" s="59"/>
-      <c r="T41" s="59"/>
-      <c r="U41" s="59"/>
-      <c r="V41" s="59"/>
-      <c r="W41" s="59"/>
-      <c r="X41" s="59"/>
-      <c r="Y41" s="59"/>
-      <c r="Z41" s="59"/>
-    </row>
-    <row r="42" spans="1:26" ht="15" customHeight="1">
-      <c r="A42" s="20"/>
-      <c r="B42" s="94" t="s">
-        <v>30</v>
-      </c>
-      <c r="C42" s="95"/>
-      <c r="D42" s="96"/>
-      <c r="E42" s="102">
-        <f>IF(K32=0,0,IFERROR(K32/M32,"Error"))</f>
-        <v>5.1502145922746781E-2</v>
-      </c>
-      <c r="F42" s="96"/>
-      <c r="G42" s="63"/>
-      <c r="H42" s="64"/>
-      <c r="I42" s="64"/>
-      <c r="J42" s="64"/>
-      <c r="K42" s="64"/>
-      <c r="L42" s="64"/>
-      <c r="M42" s="64"/>
-      <c r="N42" s="65"/>
-      <c r="O42" s="20"/>
-      <c r="P42" s="59"/>
-      <c r="Q42" s="59"/>
-      <c r="R42" s="59"/>
-      <c r="S42" s="59"/>
-      <c r="T42" s="59"/>
-      <c r="U42" s="59"/>
-      <c r="V42" s="59"/>
-      <c r="W42" s="59"/>
-      <c r="X42" s="59"/>
-      <c r="Y42" s="59"/>
-      <c r="Z42" s="59"/>
-    </row>
-    <row r="43" spans="1:26" ht="15" customHeight="1">
-      <c r="A43" s="20"/>
-      <c r="B43" s="94" t="s">
-        <v>31</v>
-      </c>
-      <c r="C43" s="95"/>
-      <c r="D43" s="96"/>
-      <c r="E43" s="66">
-        <f>E5</f>
-        <v>6.9444444444444198E-3</v>
-      </c>
-      <c r="F43" s="67">
-        <f t="shared" ref="F43:F46" si="6">IF(E43="Completar",E43,IFERROR(E43/$E$49,"Error"))</f>
-        <v>3.7174721189590899E-2</v>
-      </c>
-      <c r="G43" s="63"/>
-      <c r="H43" s="64"/>
-      <c r="I43" s="64"/>
-      <c r="J43" s="64"/>
-      <c r="K43" s="64"/>
-      <c r="L43" s="64"/>
-      <c r="M43" s="64"/>
-      <c r="N43" s="65"/>
-      <c r="O43" s="20"/>
-      <c r="P43" s="59"/>
-      <c r="Q43" s="59"/>
-      <c r="R43" s="59"/>
-      <c r="S43" s="59"/>
-      <c r="T43" s="59"/>
-      <c r="U43" s="59"/>
-      <c r="V43" s="59"/>
-      <c r="W43" s="59"/>
-      <c r="X43" s="59"/>
-      <c r="Y43" s="59"/>
-      <c r="Z43" s="59"/>
-    </row>
-    <row r="44" spans="1:26" ht="15" customHeight="1">
-      <c r="A44" s="20"/>
-      <c r="B44" s="94" t="s">
-        <v>32</v>
-      </c>
-      <c r="C44" s="95"/>
-      <c r="D44" s="96"/>
-      <c r="E44" s="66" t="str">
-        <f>E9</f>
-        <v>Completar</v>
-      </c>
-      <c r="F44" s="67" t="str">
-        <f t="shared" si="6"/>
-        <v>Completar</v>
-      </c>
-      <c r="G44" s="63"/>
-      <c r="H44" s="64"/>
-      <c r="I44" s="64"/>
-      <c r="J44" s="64"/>
-      <c r="K44" s="64"/>
-      <c r="L44" s="64"/>
-      <c r="M44" s="64"/>
-      <c r="N44" s="65"/>
-      <c r="O44" s="20"/>
-      <c r="P44" s="59"/>
-      <c r="Q44" s="59"/>
-      <c r="R44" s="59"/>
-      <c r="S44" s="59"/>
-      <c r="T44" s="59"/>
-      <c r="U44" s="59"/>
-      <c r="V44" s="59"/>
-      <c r="W44" s="59"/>
-      <c r="X44" s="59"/>
-      <c r="Y44" s="59"/>
-      <c r="Z44" s="59"/>
-    </row>
-    <row r="45" spans="1:26" ht="15" customHeight="1">
-      <c r="A45" s="20"/>
-      <c r="B45" s="94" t="s">
-        <v>33</v>
-      </c>
-      <c r="C45" s="95"/>
-      <c r="D45" s="96"/>
-      <c r="E45" s="66" t="str">
-        <f>E13</f>
-        <v>Completar</v>
-      </c>
-      <c r="F45" s="67" t="str">
-        <f t="shared" si="6"/>
-        <v>Completar</v>
-      </c>
-      <c r="G45" s="63"/>
-      <c r="H45" s="64"/>
-      <c r="I45" s="64"/>
-      <c r="J45" s="64"/>
-      <c r="K45" s="64"/>
-      <c r="L45" s="64"/>
-      <c r="M45" s="64"/>
-      <c r="N45" s="65"/>
+      <c r="C45" s="92"/>
+      <c r="D45" s="92"/>
+      <c r="E45" s="92"/>
+      <c r="F45" s="92"/>
+      <c r="G45" s="92"/>
+      <c r="H45" s="92"/>
+      <c r="I45" s="92"/>
+      <c r="J45" s="92"/>
+      <c r="K45" s="92"/>
+      <c r="L45" s="92"/>
+      <c r="M45" s="92"/>
+      <c r="N45" s="93"/>
       <c r="O45" s="20"/>
       <c r="P45" s="59"/>
       <c r="Q45" s="59"/>
@@ -4105,27 +3833,24 @@
     </row>
     <row r="46" spans="1:26" ht="15" customHeight="1">
       <c r="A46" s="20"/>
-      <c r="B46" s="94" t="s">
-        <v>34</v>
+      <c r="B46" s="97" t="s">
+        <v>27</v>
       </c>
-      <c r="C46" s="95"/>
-      <c r="D46" s="96"/>
-      <c r="E46" s="66" t="str">
-        <f>E36</f>
-        <v>Completar</v>
+      <c r="C46" s="88"/>
+      <c r="D46" s="98"/>
+      <c r="E46" s="107">
+        <f>M39</f>
+        <v>292</v>
       </c>
-      <c r="F46" s="67" t="str">
-        <f t="shared" si="6"/>
-        <v>Completar</v>
-      </c>
-      <c r="G46" s="63"/>
-      <c r="H46" s="64"/>
-      <c r="I46" s="64"/>
-      <c r="J46" s="64"/>
-      <c r="K46" s="64"/>
-      <c r="L46" s="64"/>
-      <c r="M46" s="64"/>
-      <c r="N46" s="65"/>
+      <c r="F46" s="98"/>
+      <c r="G46" s="60"/>
+      <c r="H46" s="61"/>
+      <c r="I46" s="61"/>
+      <c r="J46" s="61"/>
+      <c r="K46" s="61"/>
+      <c r="L46" s="61"/>
+      <c r="M46" s="61"/>
+      <c r="N46" s="62"/>
       <c r="O46" s="20"/>
       <c r="P46" s="59"/>
       <c r="Q46" s="59"/>
@@ -4139,21 +3864,18 @@
       <c r="Y46" s="59"/>
       <c r="Z46" s="59"/>
     </row>
-    <row r="47" spans="1:26" ht="15" customHeight="1">
+    <row r="47" spans="1:26">
       <c r="A47" s="20"/>
-      <c r="B47" s="94" t="s">
-        <v>35</v>
+      <c r="B47" s="97" t="s">
+        <v>28</v>
       </c>
-      <c r="C47" s="95"/>
-      <c r="D47" s="96"/>
-      <c r="E47" s="66">
-        <f>L32</f>
-        <v>2.7083333333333334E-2</v>
+      <c r="C47" s="88"/>
+      <c r="D47" s="98"/>
+      <c r="E47" s="106">
+        <f>IF(M39="Completar","Completar",IFERROR(M39/(N39*24),"Error"))</f>
+        <v>46.72</v>
       </c>
-      <c r="F47" s="67">
-        <f t="shared" ref="F47:F48" si="7">IF(E47="Completar",E47,IFERROR(E47/$E$49,"Completar"))</f>
-        <v>0.14498141263940503</v>
-      </c>
+      <c r="F47" s="98"/>
       <c r="G47" s="63"/>
       <c r="H47" s="64"/>
       <c r="I47" s="64"/>
@@ -4177,19 +3899,16 @@
     </row>
     <row r="48" spans="1:26" ht="15" customHeight="1">
       <c r="A48" s="20"/>
-      <c r="B48" s="94" t="s">
-        <v>36</v>
+      <c r="B48" s="97" t="s">
+        <v>29</v>
       </c>
-      <c r="C48" s="95"/>
-      <c r="D48" s="96"/>
-      <c r="E48" s="66">
-        <f>J32</f>
-        <v>0.15277777777777801</v>
+      <c r="C48" s="88"/>
+      <c r="D48" s="98"/>
+      <c r="E48" s="107">
+        <f>IF(K39=0,0,IFERROR(ROUNDUP(K39/(M39/100),0),"Error"))</f>
+        <v>5</v>
       </c>
-      <c r="F48" s="67">
-        <f t="shared" si="7"/>
-        <v>0.81784386617100402</v>
-      </c>
+      <c r="F48" s="98"/>
       <c r="G48" s="63"/>
       <c r="H48" s="64"/>
       <c r="I48" s="64"/>
@@ -4213,24 +3932,24 @@
     </row>
     <row r="49" spans="1:26" ht="15" customHeight="1">
       <c r="A49" s="20"/>
-      <c r="B49" s="99" t="s">
-        <v>37</v>
+      <c r="B49" s="97" t="s">
+        <v>30</v>
       </c>
-      <c r="C49" s="100"/>
+      <c r="C49" s="88"/>
       <c r="D49" s="98"/>
-      <c r="E49" s="97">
-        <f>IF(COUNTIF(E43:E48,"Error")&gt;0,"Error",IF(SUM(E43:E48)=0,"Completar",SUM(E43:E48)))</f>
-        <v>0.18680555555555578</v>
+      <c r="E49" s="105">
+        <f>IF(K39=0,0,IFERROR(K39/M39,"Error"))</f>
+        <v>4.7945205479452052E-2</v>
       </c>
       <c r="F49" s="98"/>
-      <c r="G49" s="68"/>
-      <c r="H49" s="69"/>
-      <c r="I49" s="69"/>
-      <c r="J49" s="69"/>
-      <c r="K49" s="69"/>
-      <c r="L49" s="69"/>
-      <c r="M49" s="69"/>
-      <c r="N49" s="70"/>
+      <c r="G49" s="63"/>
+      <c r="H49" s="64"/>
+      <c r="I49" s="64"/>
+      <c r="J49" s="64"/>
+      <c r="K49" s="64"/>
+      <c r="L49" s="64"/>
+      <c r="M49" s="64"/>
+      <c r="N49" s="65"/>
       <c r="O49" s="20"/>
       <c r="P49" s="59"/>
       <c r="Q49" s="59"/>
@@ -4244,49 +3963,65 @@
       <c r="Y49" s="59"/>
       <c r="Z49" s="59"/>
     </row>
-    <row r="50" spans="1:26" ht="6" customHeight="1">
+    <row r="50" spans="1:26" ht="15" customHeight="1">
       <c r="A50" s="20"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="20"/>
-      <c r="H50" s="20"/>
-      <c r="I50" s="20"/>
-      <c r="J50" s="20"/>
-      <c r="K50" s="20"/>
-      <c r="L50" s="20"/>
-      <c r="M50" s="20"/>
-      <c r="N50" s="20"/>
+      <c r="B50" s="97" t="s">
+        <v>31</v>
+      </c>
+      <c r="C50" s="88"/>
+      <c r="D50" s="98"/>
+      <c r="E50" s="66">
+        <f>E5</f>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="F50" s="67">
+        <f t="shared" ref="F50:F53" si="6">IF(E50="Completar",E50,IFERROR(E50/$E$56,"Error"))</f>
+        <v>2.5974025974025882E-2</v>
+      </c>
+      <c r="G50" s="63"/>
+      <c r="H50" s="64"/>
+      <c r="I50" s="64"/>
+      <c r="J50" s="64"/>
+      <c r="K50" s="64"/>
+      <c r="L50" s="64"/>
+      <c r="M50" s="64"/>
+      <c r="N50" s="65"/>
       <c r="O50" s="20"/>
-      <c r="P50" s="20"/>
-      <c r="Q50" s="20"/>
-      <c r="R50" s="20"/>
-      <c r="S50" s="20"/>
-      <c r="T50" s="20"/>
-      <c r="U50" s="20"/>
-      <c r="V50" s="20"/>
-      <c r="W50" s="20"/>
-      <c r="X50" s="20"/>
-      <c r="Y50" s="20"/>
-      <c r="Z50" s="20"/>
-    </row>
-    <row r="51" spans="1:26" hidden="1">
+      <c r="P50" s="59"/>
+      <c r="Q50" s="59"/>
+      <c r="R50" s="59"/>
+      <c r="S50" s="59"/>
+      <c r="T50" s="59"/>
+      <c r="U50" s="59"/>
+      <c r="V50" s="59"/>
+      <c r="W50" s="59"/>
+      <c r="X50" s="59"/>
+      <c r="Y50" s="59"/>
+      <c r="Z50" s="59"/>
+    </row>
+    <row r="51" spans="1:26" ht="15" customHeight="1">
       <c r="A51" s="20"/>
-      <c r="B51" s="59"/>
-      <c r="C51" s="59"/>
-      <c r="D51" s="59"/>
-      <c r="E51" s="59"/>
-      <c r="F51" s="59"/>
-      <c r="G51" s="59"/>
-      <c r="H51" s="59"/>
-      <c r="I51" s="59"/>
-      <c r="J51" s="59"/>
-      <c r="K51" s="59"/>
-      <c r="L51" s="59"/>
-      <c r="M51" s="59"/>
-      <c r="N51" s="59"/>
+      <c r="B51" s="97" t="s">
+        <v>32</v>
+      </c>
+      <c r="C51" s="88"/>
+      <c r="D51" s="98"/>
+      <c r="E51" s="66" t="str">
+        <f>E9</f>
+        <v>Completar</v>
+      </c>
+      <c r="F51" s="67" t="str">
+        <f t="shared" si="6"/>
+        <v>Completar</v>
+      </c>
+      <c r="G51" s="63"/>
+      <c r="H51" s="64"/>
+      <c r="I51" s="64"/>
+      <c r="J51" s="64"/>
+      <c r="K51" s="64"/>
+      <c r="L51" s="64"/>
+      <c r="M51" s="64"/>
+      <c r="N51" s="65"/>
       <c r="O51" s="20"/>
       <c r="P51" s="59"/>
       <c r="Q51" s="59"/>
@@ -4300,21 +4035,29 @@
       <c r="Y51" s="59"/>
       <c r="Z51" s="59"/>
     </row>
-    <row r="52" spans="1:26">
+    <row r="52" spans="1:26" ht="15" customHeight="1">
       <c r="A52" s="20"/>
-      <c r="B52" s="59"/>
-      <c r="C52" s="59"/>
-      <c r="D52" s="59"/>
-      <c r="E52" s="59"/>
-      <c r="F52" s="59"/>
-      <c r="G52" s="59"/>
-      <c r="H52" s="59"/>
-      <c r="I52" s="59"/>
-      <c r="J52" s="59"/>
-      <c r="K52" s="59"/>
-      <c r="L52" s="59"/>
-      <c r="M52" s="59"/>
-      <c r="N52" s="59"/>
+      <c r="B52" s="97" t="s">
+        <v>33</v>
+      </c>
+      <c r="C52" s="88"/>
+      <c r="D52" s="98"/>
+      <c r="E52" s="66" t="str">
+        <f>E13</f>
+        <v>Completar</v>
+      </c>
+      <c r="F52" s="67" t="str">
+        <f t="shared" si="6"/>
+        <v>Completar</v>
+      </c>
+      <c r="G52" s="63"/>
+      <c r="H52" s="64"/>
+      <c r="I52" s="64"/>
+      <c r="J52" s="64"/>
+      <c r="K52" s="64"/>
+      <c r="L52" s="64"/>
+      <c r="M52" s="64"/>
+      <c r="N52" s="65"/>
       <c r="O52" s="20"/>
       <c r="P52" s="59"/>
       <c r="Q52" s="59"/>
@@ -4328,21 +4071,29 @@
       <c r="Y52" s="59"/>
       <c r="Z52" s="59"/>
     </row>
-    <row r="53" spans="1:26">
+    <row r="53" spans="1:26" ht="15" customHeight="1">
       <c r="A53" s="20"/>
-      <c r="B53" s="59"/>
-      <c r="C53" s="59"/>
-      <c r="D53" s="59"/>
-      <c r="E53" s="59"/>
-      <c r="F53" s="59"/>
-      <c r="G53" s="59"/>
-      <c r="H53" s="59"/>
-      <c r="I53" s="59"/>
-      <c r="J53" s="59"/>
-      <c r="K53" s="59"/>
-      <c r="L53" s="59"/>
-      <c r="M53" s="59"/>
-      <c r="N53" s="59"/>
+      <c r="B53" s="97" t="s">
+        <v>34</v>
+      </c>
+      <c r="C53" s="88"/>
+      <c r="D53" s="98"/>
+      <c r="E53" s="66" t="str">
+        <f>E43</f>
+        <v>Completar</v>
+      </c>
+      <c r="F53" s="67" t="str">
+        <f t="shared" si="6"/>
+        <v>Completar</v>
+      </c>
+      <c r="G53" s="63"/>
+      <c r="H53" s="64"/>
+      <c r="I53" s="64"/>
+      <c r="J53" s="64"/>
+      <c r="K53" s="64"/>
+      <c r="L53" s="64"/>
+      <c r="M53" s="64"/>
+      <c r="N53" s="65"/>
       <c r="O53" s="20"/>
       <c r="P53" s="59"/>
       <c r="Q53" s="59"/>
@@ -4356,21 +4107,29 @@
       <c r="Y53" s="59"/>
       <c r="Z53" s="59"/>
     </row>
-    <row r="54" spans="1:26">
+    <row r="54" spans="1:26" ht="15" customHeight="1">
       <c r="A54" s="20"/>
-      <c r="B54" s="59"/>
-      <c r="C54" s="59"/>
-      <c r="D54" s="59"/>
-      <c r="E54" s="59"/>
-      <c r="F54" s="59"/>
-      <c r="G54" s="59"/>
-      <c r="H54" s="59"/>
-      <c r="I54" s="59"/>
-      <c r="J54" s="59"/>
-      <c r="K54" s="59"/>
-      <c r="L54" s="59"/>
-      <c r="M54" s="59"/>
-      <c r="N54" s="59"/>
+      <c r="B54" s="97" t="s">
+        <v>35</v>
+      </c>
+      <c r="C54" s="88"/>
+      <c r="D54" s="98"/>
+      <c r="E54" s="66">
+        <f>L39</f>
+        <v>3.0555555555555555E-2</v>
+      </c>
+      <c r="F54" s="67">
+        <f t="shared" ref="F54:F55" si="7">IF(E54="Completar",E54,IFERROR(E54/$E$56,"Completar"))</f>
+        <v>0.11428571428571428</v>
+      </c>
+      <c r="G54" s="63"/>
+      <c r="H54" s="64"/>
+      <c r="I54" s="64"/>
+      <c r="J54" s="64"/>
+      <c r="K54" s="64"/>
+      <c r="L54" s="64"/>
+      <c r="M54" s="64"/>
+      <c r="N54" s="65"/>
       <c r="O54" s="20"/>
       <c r="P54" s="59"/>
       <c r="Q54" s="59"/>
@@ -4384,21 +4143,29 @@
       <c r="Y54" s="59"/>
       <c r="Z54" s="59"/>
     </row>
-    <row r="55" spans="1:26">
+    <row r="55" spans="1:26" ht="15" customHeight="1">
       <c r="A55" s="20"/>
-      <c r="B55" s="59"/>
-      <c r="C55" s="59"/>
-      <c r="D55" s="59"/>
-      <c r="E55" s="59"/>
-      <c r="F55" s="59"/>
-      <c r="G55" s="59"/>
-      <c r="H55" s="59"/>
-      <c r="I55" s="59"/>
-      <c r="J55" s="59"/>
-      <c r="K55" s="59"/>
-      <c r="L55" s="59"/>
-      <c r="M55" s="59"/>
-      <c r="N55" s="59"/>
+      <c r="B55" s="97" t="s">
+        <v>36</v>
+      </c>
+      <c r="C55" s="88"/>
+      <c r="D55" s="98"/>
+      <c r="E55" s="66">
+        <f>J39</f>
+        <v>0.22986111111111113</v>
+      </c>
+      <c r="F55" s="67">
+        <f t="shared" si="7"/>
+        <v>0.8597402597402598</v>
+      </c>
+      <c r="G55" s="63"/>
+      <c r="H55" s="64"/>
+      <c r="I55" s="64"/>
+      <c r="J55" s="64"/>
+      <c r="K55" s="64"/>
+      <c r="L55" s="64"/>
+      <c r="M55" s="64"/>
+      <c r="N55" s="65"/>
       <c r="O55" s="20"/>
       <c r="P55" s="59"/>
       <c r="Q55" s="59"/>
@@ -4412,21 +4179,26 @@
       <c r="Y55" s="59"/>
       <c r="Z55" s="59"/>
     </row>
-    <row r="56" spans="1:26">
+    <row r="56" spans="1:26" ht="15" customHeight="1">
       <c r="A56" s="20"/>
-      <c r="B56" s="59"/>
-      <c r="C56" s="59"/>
-      <c r="D56" s="59"/>
-      <c r="E56" s="59"/>
-      <c r="F56" s="59"/>
-      <c r="G56" s="59"/>
-      <c r="H56" s="59"/>
-      <c r="I56" s="59"/>
-      <c r="J56" s="59"/>
-      <c r="K56" s="59"/>
-      <c r="L56" s="59"/>
-      <c r="M56" s="59"/>
-      <c r="N56" s="59"/>
+      <c r="B56" s="101" t="s">
+        <v>37</v>
+      </c>
+      <c r="C56" s="102"/>
+      <c r="D56" s="100"/>
+      <c r="E56" s="99">
+        <f>IF(COUNTIF(E50:E55,"Error")&gt;0,"Error",IF(SUM(E50:E55)=0,"Completar",SUM(E50:E55)))</f>
+        <v>0.2673611111111111</v>
+      </c>
+      <c r="F56" s="100"/>
+      <c r="G56" s="68"/>
+      <c r="H56" s="69"/>
+      <c r="I56" s="69"/>
+      <c r="J56" s="69"/>
+      <c r="K56" s="69"/>
+      <c r="L56" s="69"/>
+      <c r="M56" s="69"/>
+      <c r="N56" s="70"/>
       <c r="O56" s="20"/>
       <c r="P56" s="59"/>
       <c r="Q56" s="59"/>
@@ -4440,35 +4212,35 @@
       <c r="Y56" s="59"/>
       <c r="Z56" s="59"/>
     </row>
-    <row r="57" spans="1:26">
+    <row r="57" spans="1:26" ht="6" customHeight="1">
       <c r="A57" s="20"/>
-      <c r="B57" s="59"/>
-      <c r="C57" s="59"/>
-      <c r="D57" s="59"/>
-      <c r="E57" s="59"/>
-      <c r="F57" s="59"/>
-      <c r="G57" s="59"/>
-      <c r="H57" s="59"/>
-      <c r="I57" s="59"/>
-      <c r="J57" s="59"/>
-      <c r="K57" s="59"/>
-      <c r="L57" s="59"/>
-      <c r="M57" s="59"/>
-      <c r="N57" s="59"/>
+      <c r="B57" s="20"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="20"/>
+      <c r="H57" s="20"/>
+      <c r="I57" s="20"/>
+      <c r="J57" s="20"/>
+      <c r="K57" s="20"/>
+      <c r="L57" s="20"/>
+      <c r="M57" s="20"/>
+      <c r="N57" s="20"/>
       <c r="O57" s="20"/>
-      <c r="P57" s="59"/>
-      <c r="Q57" s="59"/>
-      <c r="R57" s="59"/>
-      <c r="S57" s="59"/>
-      <c r="T57" s="59"/>
-      <c r="U57" s="59"/>
-      <c r="V57" s="59"/>
-      <c r="W57" s="59"/>
-      <c r="X57" s="59"/>
-      <c r="Y57" s="59"/>
-      <c r="Z57" s="59"/>
-    </row>
-    <row r="58" spans="1:26">
+      <c r="P57" s="20"/>
+      <c r="Q57" s="20"/>
+      <c r="R57" s="20"/>
+      <c r="S57" s="20"/>
+      <c r="T57" s="20"/>
+      <c r="U57" s="20"/>
+      <c r="V57" s="20"/>
+      <c r="W57" s="20"/>
+      <c r="X57" s="20"/>
+      <c r="Y57" s="20"/>
+      <c r="Z57" s="20"/>
+    </row>
+    <row r="58" spans="1:26" hidden="1">
       <c r="A58" s="20"/>
       <c r="B58" s="59"/>
       <c r="C58" s="59"/>
@@ -31040,10 +30812,209 @@
       <c r="Y1006" s="59"/>
       <c r="Z1006" s="59"/>
     </row>
+    <row r="1007" spans="1:26">
+      <c r="A1007" s="20"/>
+      <c r="B1007" s="59"/>
+      <c r="C1007" s="59"/>
+      <c r="D1007" s="59"/>
+      <c r="E1007" s="59"/>
+      <c r="F1007" s="59"/>
+      <c r="G1007" s="59"/>
+      <c r="H1007" s="59"/>
+      <c r="I1007" s="59"/>
+      <c r="J1007" s="59"/>
+      <c r="K1007" s="59"/>
+      <c r="L1007" s="59"/>
+      <c r="M1007" s="59"/>
+      <c r="N1007" s="59"/>
+      <c r="O1007" s="20"/>
+      <c r="P1007" s="59"/>
+      <c r="Q1007" s="59"/>
+      <c r="R1007" s="59"/>
+      <c r="S1007" s="59"/>
+      <c r="T1007" s="59"/>
+      <c r="U1007" s="59"/>
+      <c r="V1007" s="59"/>
+      <c r="W1007" s="59"/>
+      <c r="X1007" s="59"/>
+      <c r="Y1007" s="59"/>
+      <c r="Z1007" s="59"/>
+    </row>
+    <row r="1008" spans="1:26">
+      <c r="A1008" s="20"/>
+      <c r="B1008" s="59"/>
+      <c r="C1008" s="59"/>
+      <c r="D1008" s="59"/>
+      <c r="E1008" s="59"/>
+      <c r="F1008" s="59"/>
+      <c r="G1008" s="59"/>
+      <c r="H1008" s="59"/>
+      <c r="I1008" s="59"/>
+      <c r="J1008" s="59"/>
+      <c r="K1008" s="59"/>
+      <c r="L1008" s="59"/>
+      <c r="M1008" s="59"/>
+      <c r="N1008" s="59"/>
+      <c r="O1008" s="20"/>
+      <c r="P1008" s="59"/>
+      <c r="Q1008" s="59"/>
+      <c r="R1008" s="59"/>
+      <c r="S1008" s="59"/>
+      <c r="T1008" s="59"/>
+      <c r="U1008" s="59"/>
+      <c r="V1008" s="59"/>
+      <c r="W1008" s="59"/>
+      <c r="X1008" s="59"/>
+      <c r="Y1008" s="59"/>
+      <c r="Z1008" s="59"/>
+    </row>
+    <row r="1009" spans="1:26">
+      <c r="A1009" s="20"/>
+      <c r="B1009" s="59"/>
+      <c r="C1009" s="59"/>
+      <c r="D1009" s="59"/>
+      <c r="E1009" s="59"/>
+      <c r="F1009" s="59"/>
+      <c r="G1009" s="59"/>
+      <c r="H1009" s="59"/>
+      <c r="I1009" s="59"/>
+      <c r="J1009" s="59"/>
+      <c r="K1009" s="59"/>
+      <c r="L1009" s="59"/>
+      <c r="M1009" s="59"/>
+      <c r="N1009" s="59"/>
+      <c r="O1009" s="20"/>
+      <c r="P1009" s="59"/>
+      <c r="Q1009" s="59"/>
+      <c r="R1009" s="59"/>
+      <c r="S1009" s="59"/>
+      <c r="T1009" s="59"/>
+      <c r="U1009" s="59"/>
+      <c r="V1009" s="59"/>
+      <c r="W1009" s="59"/>
+      <c r="X1009" s="59"/>
+      <c r="Y1009" s="59"/>
+      <c r="Z1009" s="59"/>
+    </row>
+    <row r="1010" spans="1:26">
+      <c r="A1010" s="20"/>
+      <c r="B1010" s="59"/>
+      <c r="C1010" s="59"/>
+      <c r="D1010" s="59"/>
+      <c r="E1010" s="59"/>
+      <c r="F1010" s="59"/>
+      <c r="G1010" s="59"/>
+      <c r="H1010" s="59"/>
+      <c r="I1010" s="59"/>
+      <c r="J1010" s="59"/>
+      <c r="K1010" s="59"/>
+      <c r="L1010" s="59"/>
+      <c r="M1010" s="59"/>
+      <c r="N1010" s="59"/>
+      <c r="O1010" s="20"/>
+      <c r="P1010" s="59"/>
+      <c r="Q1010" s="59"/>
+      <c r="R1010" s="59"/>
+      <c r="S1010" s="59"/>
+      <c r="T1010" s="59"/>
+      <c r="U1010" s="59"/>
+      <c r="V1010" s="59"/>
+      <c r="W1010" s="59"/>
+      <c r="X1010" s="59"/>
+      <c r="Y1010" s="59"/>
+      <c r="Z1010" s="59"/>
+    </row>
+    <row r="1011" spans="1:26">
+      <c r="A1011" s="20"/>
+      <c r="B1011" s="59"/>
+      <c r="C1011" s="59"/>
+      <c r="D1011" s="59"/>
+      <c r="E1011" s="59"/>
+      <c r="F1011" s="59"/>
+      <c r="G1011" s="59"/>
+      <c r="H1011" s="59"/>
+      <c r="I1011" s="59"/>
+      <c r="J1011" s="59"/>
+      <c r="K1011" s="59"/>
+      <c r="L1011" s="59"/>
+      <c r="M1011" s="59"/>
+      <c r="N1011" s="59"/>
+      <c r="O1011" s="20"/>
+      <c r="P1011" s="59"/>
+      <c r="Q1011" s="59"/>
+      <c r="R1011" s="59"/>
+      <c r="S1011" s="59"/>
+      <c r="T1011" s="59"/>
+      <c r="U1011" s="59"/>
+      <c r="V1011" s="59"/>
+      <c r="W1011" s="59"/>
+      <c r="X1011" s="59"/>
+      <c r="Y1011" s="59"/>
+      <c r="Z1011" s="59"/>
+    </row>
+    <row r="1012" spans="1:26">
+      <c r="A1012" s="20"/>
+      <c r="B1012" s="59"/>
+      <c r="C1012" s="59"/>
+      <c r="D1012" s="59"/>
+      <c r="E1012" s="59"/>
+      <c r="F1012" s="59"/>
+      <c r="G1012" s="59"/>
+      <c r="H1012" s="59"/>
+      <c r="I1012" s="59"/>
+      <c r="J1012" s="59"/>
+      <c r="K1012" s="59"/>
+      <c r="L1012" s="59"/>
+      <c r="M1012" s="59"/>
+      <c r="N1012" s="59"/>
+      <c r="O1012" s="20"/>
+      <c r="P1012" s="59"/>
+      <c r="Q1012" s="59"/>
+      <c r="R1012" s="59"/>
+      <c r="S1012" s="59"/>
+      <c r="T1012" s="59"/>
+      <c r="U1012" s="59"/>
+      <c r="V1012" s="59"/>
+      <c r="W1012" s="59"/>
+      <c r="X1012" s="59"/>
+      <c r="Y1012" s="59"/>
+      <c r="Z1012" s="59"/>
+    </row>
+    <row r="1013" spans="1:26">
+      <c r="A1013" s="20"/>
+      <c r="B1013" s="59"/>
+      <c r="C1013" s="59"/>
+      <c r="D1013" s="59"/>
+      <c r="E1013" s="59"/>
+      <c r="F1013" s="59"/>
+      <c r="G1013" s="59"/>
+      <c r="H1013" s="59"/>
+      <c r="I1013" s="59"/>
+      <c r="J1013" s="59"/>
+      <c r="K1013" s="59"/>
+      <c r="L1013" s="59"/>
+      <c r="M1013" s="59"/>
+      <c r="N1013" s="59"/>
+      <c r="O1013" s="20"/>
+      <c r="P1013" s="59"/>
+      <c r="Q1013" s="59"/>
+      <c r="R1013" s="59"/>
+      <c r="S1013" s="59"/>
+      <c r="T1013" s="59"/>
+      <c r="U1013" s="59"/>
+      <c r="V1013" s="59"/>
+      <c r="W1013" s="59"/>
+      <c r="X1013" s="59"/>
+      <c r="Y1013" s="59"/>
+      <c r="Z1013" s="59"/>
+    </row>
   </sheetData>
-  <mergeCells count="50">
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="B32:E32"/>
+  <mergeCells count="57">
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="B39:E39"/>
     <mergeCell ref="M16:M17"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="B16:B17"/>
@@ -31063,28 +31034,28 @@
     <mergeCell ref="C23:E23"/>
     <mergeCell ref="H16:J16"/>
     <mergeCell ref="K16:L16"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B38:N38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B45:N45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="B48:D48"/>
     <mergeCell ref="B15:N15"/>
     <mergeCell ref="F12:N12"/>
     <mergeCell ref="F13:N13"/>
-    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C38:E38"/>
     <mergeCell ref="E49:F49"/>
     <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E47:F47"/>
     <mergeCell ref="D1:N1"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B7:E7"/>
@@ -31092,124 +31063,88 @@
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="F8:N8"/>
     <mergeCell ref="F9:N9"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C33:E33"/>
   </mergeCells>
-  <conditionalFormatting sqref="D1:XFD24 C3:C24 A32:XFD1048576 A1:B31 N25:XFD31">
-    <cfRule type="cellIs" dxfId="29" priority="35" operator="equal">
+  <conditionalFormatting sqref="D1:XFD24 C3:C24 A39:XFD1048576 A1:B38 N25:XFD38 J27:J38 C30:I37 K30:M37">
+    <cfRule type="cellIs" dxfId="15" priority="35" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:XFD24 C3:C24 A32:XFD1048576 A1:B31 N25:XFD31">
-    <cfRule type="cellIs" dxfId="28" priority="36" operator="equal">
+  <conditionalFormatting sqref="D1:XFD24 C3:C24 A39:XFD1048576 A1:B38 N25:XFD38 J27:J38 C30:I37 K30:M37">
+    <cfRule type="cellIs" dxfId="14" priority="36" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:M25 C26:E26">
-    <cfRule type="cellIs" dxfId="37" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="33" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:M25 C26:E26">
-    <cfRule type="cellIs" dxfId="36" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="34" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F26:M26 K31:M31 C31 F31:I31 J27:J31">
-    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
+  <conditionalFormatting sqref="F26:M26 C38 F38:I38 K38:M38">
+    <cfRule type="cellIs" dxfId="11" priority="27" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F26:M26 K31:M31 C31 F31:I31 J27:J31">
-    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
+  <conditionalFormatting sqref="F26:M26 C38 F38:I38 K38:M38">
+    <cfRule type="cellIs" dxfId="10" priority="28" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:I27 K27:M27">
-    <cfRule type="cellIs" dxfId="35" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="23" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:I27 K27:M27">
-    <cfRule type="cellIs" dxfId="34" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="24" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28:M28 C28 F28:I28">
-    <cfRule type="cellIs" dxfId="31" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="19" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28:M28 C28 F28:I28">
-    <cfRule type="cellIs" dxfId="30" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="20" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K29:M29 C29 F29:I29">
-    <cfRule type="cellIs" dxfId="25" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="15" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K29:M29 C29 F29:I29">
-    <cfRule type="cellIs" dxfId="24" priority="16" operator="equal">
-      <formula>"Error"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K30:M30 C30 F30:I30">
-    <cfRule type="cellIs" dxfId="33" priority="11" operator="equal">
-      <formula>"Completar"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K30:M30 C30 F30:I30">
-    <cfRule type="cellIs" dxfId="32" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="16" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28:M28 C28 F28:I28">
-    <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="10" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28:M28 C28 F28:I28">
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
-      <formula>"Error"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N29:N30">
-    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
-      <formula>"Completar"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N29:N30">
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
-      <formula>"Error"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J29:J30">
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
-      <formula>"Completar"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J29:J30">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="9" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:I29 K29:M29">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:I29 K29:M29">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
-      <formula>"Error"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30:I30 K30:M30">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
-      <formula>"Completar"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30:I30 K30:M30">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update de metricas y diag clases
Se agrega metricas de producto Matriz x Vector y se actualiza diagrama de clases.
</commit_message>
<xml_diff>
--- a/Documentacion/MatrizMath/MatrizMath - Planilla de Métricas V2.1.xlsx
+++ b/Documentacion/MatrizMath/MatrizMath - Planilla de Métricas V2.1.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BKP ALMIRON\ENZO-AMS\TEIC\Nueva carpeta\PROG III\TP2\TP2-Repo\Documentacion\MatrizMath\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900"/>
   </bookViews>
   <sheets>
     <sheet name="Métricas" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
   <si>
     <t>PROYECTO:</t>
   </si>
@@ -176,11 +171,14 @@
   <si>
     <t>diferenciaFilaConMultiploDeOtra()</t>
   </si>
+  <si>
+    <t>producto(VectorMath)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -1067,90 +1065,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1218,6 +1132,90 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1485,18 +1483,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -1506,8 +1495,8 @@
           <c:yMode val="edge"/>
           <c:x val="3.3565974707706982E-2"/>
           <c:y val="7.4074152627750078E-2"/>
-          <c:w val="0.40158680164979416"/>
-          <c:h val="0.85185169474450051"/>
+          <c:w val="0.40158680164979427"/>
+          <c:h val="0.85185169474450073"/>
         </c:manualLayout>
       </c:layout>
       <c:pieChart>
@@ -1517,13 +1506,12 @@
           <c:order val="0"/>
           <c:dPt>
             <c:idx val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="FFC000"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-49DD-4FD5-A2AE-26863999DE8F}"/>
               </c:ext>
@@ -1531,13 +1519,12 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="00B0F0"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-49DD-4FD5-A2AE-26863999DE8F}"/>
               </c:ext>
@@ -1545,13 +1532,12 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="0066FF"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-49DD-4FD5-A2AE-26863999DE8F}"/>
               </c:ext>
@@ -1559,13 +1545,12 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="009900"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-49DD-4FD5-A2AE-26863999DE8F}"/>
               </c:ext>
@@ -1573,13 +1558,12 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000009-49DD-4FD5-A2AE-26863999DE8F}"/>
               </c:ext>
@@ -1587,13 +1571,12 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="002060"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000B-49DD-4FD5-A2AE-26863999DE8F}"/>
               </c:ext>
@@ -1634,21 +1617,13 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000C-49DD-4FD5-A2AE-26863999DE8F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
       <c:spPr>
@@ -1659,7 +1634,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
@@ -1667,7 +1642,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1751,7 +1726,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1786,7 +1761,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1963,21 +1938,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z1013"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31:E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
@@ -1993,23 +1968,23 @@
   <sheetData>
     <row r="1" spans="1:26" ht="23.25" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="94" t="s">
+      <c r="B1" s="147" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="89" t="s">
+      <c r="C1" s="139"/>
+      <c r="D1" s="146" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="90"/>
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="139"/>
+      <c r="K1" s="139"/>
+      <c r="L1" s="139"/>
+      <c r="M1" s="139"/>
+      <c r="N1" s="139"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -2053,12 +2028,12 @@
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
       <c r="A3" s="4"/>
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="115" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="93"/>
+      <c r="C3" s="116"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="117"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -2184,12 +2159,12 @@
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1">
       <c r="A7" s="4"/>
-      <c r="B7" s="91" t="s">
+      <c r="B7" s="115" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="92"/>
-      <c r="D7" s="92"/>
-      <c r="E7" s="93"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="116"/>
+      <c r="E7" s="117"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -2226,15 +2201,15 @@
       <c r="E8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="95"/>
-      <c r="G8" s="90"/>
-      <c r="H8" s="90"/>
-      <c r="I8" s="90"/>
-      <c r="J8" s="90"/>
-      <c r="K8" s="90"/>
-      <c r="L8" s="90"/>
-      <c r="M8" s="90"/>
-      <c r="N8" s="90"/>
+      <c r="F8" s="138"/>
+      <c r="G8" s="139"/>
+      <c r="H8" s="139"/>
+      <c r="I8" s="139"/>
+      <c r="J8" s="139"/>
+      <c r="K8" s="139"/>
+      <c r="L8" s="139"/>
+      <c r="M8" s="139"/>
+      <c r="N8" s="139"/>
       <c r="O8" s="7"/>
       <c r="P8" s="13"/>
       <c r="Q8" s="14"/>
@@ -2261,15 +2236,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C9),ISBLANK(D9)),"Completar",IF(D9&gt;=C9,D9-C9,"Error")),"Error")</f>
         <v>Completar</v>
       </c>
-      <c r="F9" s="96"/>
-      <c r="G9" s="90"/>
-      <c r="H9" s="90"/>
-      <c r="I9" s="90"/>
-      <c r="J9" s="90"/>
-      <c r="K9" s="90"/>
-      <c r="L9" s="90"/>
-      <c r="M9" s="90"/>
-      <c r="N9" s="90"/>
+      <c r="F9" s="140"/>
+      <c r="G9" s="139"/>
+      <c r="H9" s="139"/>
+      <c r="I9" s="139"/>
+      <c r="J9" s="139"/>
+      <c r="K9" s="139"/>
+      <c r="L9" s="139"/>
+      <c r="M9" s="139"/>
+      <c r="N9" s="139"/>
       <c r="O9" s="15"/>
       <c r="P9" s="21"/>
       <c r="Q9" s="22"/>
@@ -2313,12 +2288,12 @@
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" s="4"/>
-      <c r="B11" s="91" t="s">
+      <c r="B11" s="115" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="92"/>
-      <c r="D11" s="92"/>
-      <c r="E11" s="93"/>
+      <c r="C11" s="116"/>
+      <c r="D11" s="116"/>
+      <c r="E11" s="117"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -2355,15 +2330,15 @@
       <c r="E12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="95"/>
-      <c r="G12" s="90"/>
-      <c r="H12" s="90"/>
-      <c r="I12" s="90"/>
-      <c r="J12" s="90"/>
-      <c r="K12" s="90"/>
-      <c r="L12" s="90"/>
-      <c r="M12" s="90"/>
-      <c r="N12" s="90"/>
+      <c r="F12" s="138"/>
+      <c r="G12" s="139"/>
+      <c r="H12" s="139"/>
+      <c r="I12" s="139"/>
+      <c r="J12" s="139"/>
+      <c r="K12" s="139"/>
+      <c r="L12" s="139"/>
+      <c r="M12" s="139"/>
+      <c r="N12" s="139"/>
       <c r="O12" s="7"/>
       <c r="P12" s="13"/>
       <c r="Q12" s="14"/>
@@ -2388,15 +2363,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C13),ISBLANK(D13)),"Completar",IF(D13&gt;=C13,D13-C13,"Error")),"Error")</f>
         <v>Completar</v>
       </c>
-      <c r="F13" s="96"/>
-      <c r="G13" s="90"/>
-      <c r="H13" s="90"/>
-      <c r="I13" s="90"/>
-      <c r="J13" s="90"/>
-      <c r="K13" s="90"/>
-      <c r="L13" s="90"/>
-      <c r="M13" s="90"/>
-      <c r="N13" s="90"/>
+      <c r="F13" s="140"/>
+      <c r="G13" s="139"/>
+      <c r="H13" s="139"/>
+      <c r="I13" s="139"/>
+      <c r="J13" s="139"/>
+      <c r="K13" s="139"/>
+      <c r="L13" s="139"/>
+      <c r="M13" s="139"/>
+      <c r="N13" s="139"/>
       <c r="O13" s="15"/>
       <c r="P13" s="21"/>
       <c r="Q13" s="22"/>
@@ -2440,21 +2415,21 @@
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1">
       <c r="A15" s="4"/>
-      <c r="B15" s="91" t="s">
+      <c r="B15" s="115" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="92"/>
-      <c r="D15" s="92"/>
-      <c r="E15" s="92"/>
-      <c r="F15" s="92"/>
-      <c r="G15" s="92"/>
-      <c r="H15" s="92"/>
-      <c r="I15" s="92"/>
-      <c r="J15" s="92"/>
-      <c r="K15" s="92"/>
-      <c r="L15" s="92"/>
-      <c r="M15" s="92"/>
-      <c r="N15" s="93"/>
+      <c r="C15" s="116"/>
+      <c r="D15" s="116"/>
+      <c r="E15" s="116"/>
+      <c r="F15" s="116"/>
+      <c r="G15" s="116"/>
+      <c r="H15" s="116"/>
+      <c r="I15" s="116"/>
+      <c r="J15" s="116"/>
+      <c r="K15" s="116"/>
+      <c r="L15" s="116"/>
+      <c r="M15" s="116"/>
+      <c r="N15" s="117"/>
       <c r="O15" s="4"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
@@ -2470,31 +2445,31 @@
     </row>
     <row r="16" spans="1:26" ht="16.5" customHeight="1">
       <c r="A16" s="7"/>
-      <c r="B16" s="119" t="s">
+      <c r="B16" s="124" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="121" t="s">
+      <c r="C16" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="122"/>
-      <c r="E16" s="122"/>
-      <c r="F16" s="114" t="s">
+      <c r="D16" s="127"/>
+      <c r="E16" s="127"/>
+      <c r="F16" s="122" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="115"/>
-      <c r="H16" s="113" t="s">
+      <c r="G16" s="123"/>
+      <c r="H16" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="88"/>
-      <c r="J16" s="88"/>
-      <c r="K16" s="114" t="s">
+      <c r="I16" s="131"/>
+      <c r="J16" s="131"/>
+      <c r="K16" s="122" t="s">
         <v>14</v>
       </c>
-      <c r="L16" s="115"/>
-      <c r="M16" s="117" t="s">
+      <c r="L16" s="123"/>
+      <c r="M16" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="N16" s="108" t="s">
+      <c r="N16" s="132" t="s">
         <v>6</v>
       </c>
       <c r="O16" s="7"/>
@@ -2512,10 +2487,10 @@
     </row>
     <row r="17" spans="1:26" ht="30" customHeight="1">
       <c r="A17" s="7"/>
-      <c r="B17" s="120"/>
-      <c r="C17" s="123"/>
-      <c r="D17" s="124"/>
-      <c r="E17" s="124"/>
+      <c r="B17" s="125"/>
+      <c r="C17" s="128"/>
+      <c r="D17" s="129"/>
+      <c r="E17" s="129"/>
       <c r="F17" s="26" t="s">
         <v>16</v>
       </c>
@@ -2537,8 +2512,8 @@
       <c r="L17" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="M17" s="118"/>
-      <c r="N17" s="109"/>
+      <c r="M17" s="121"/>
+      <c r="N17" s="133"/>
       <c r="O17" s="7"/>
       <c r="P17" s="13"/>
       <c r="Q17" s="14"/>
@@ -2558,11 +2533,11 @@
         <f t="shared" ref="B18:B38" si="0">ROW($B18)-16</f>
         <v>2</v>
       </c>
-      <c r="C18" s="110" t="s">
+      <c r="C18" s="130" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="88"/>
-      <c r="E18" s="88"/>
+      <c r="D18" s="131"/>
+      <c r="E18" s="131"/>
       <c r="F18" s="31">
         <v>60</v>
       </c>
@@ -2611,11 +2586,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C19" s="110" t="s">
+      <c r="C19" s="130" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="88"/>
-      <c r="E19" s="88"/>
+      <c r="D19" s="131"/>
+      <c r="E19" s="131"/>
       <c r="F19" s="31">
         <v>4</v>
       </c>
@@ -2664,11 +2639,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C20" s="110" t="s">
+      <c r="C20" s="130" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="88"/>
-      <c r="E20" s="88"/>
+      <c r="D20" s="131"/>
+      <c r="E20" s="131"/>
       <c r="F20" s="31">
         <v>8</v>
       </c>
@@ -2717,11 +2692,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C21" s="110" t="s">
+      <c r="C21" s="130" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="88"/>
-      <c r="E21" s="88"/>
+      <c r="D21" s="131"/>
+      <c r="E21" s="131"/>
       <c r="F21" s="31">
         <v>10</v>
       </c>
@@ -2770,11 +2745,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C22" s="111" t="s">
+      <c r="C22" s="113" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="112"/>
-      <c r="E22" s="112"/>
+      <c r="D22" s="114"/>
+      <c r="E22" s="114"/>
       <c r="F22" s="74">
         <v>8</v>
       </c>
@@ -2823,11 +2798,11 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C23" s="87" t="s">
+      <c r="C23" s="110" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="88"/>
-      <c r="E23" s="88"/>
+      <c r="D23" s="131"/>
+      <c r="E23" s="131"/>
       <c r="F23" s="42">
         <v>13</v>
       </c>
@@ -2876,11 +2851,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C24" s="87" t="s">
+      <c r="C24" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
+      <c r="D24" s="131"/>
+      <c r="E24" s="131"/>
       <c r="F24" s="42">
         <v>25</v>
       </c>
@@ -2929,11 +2904,11 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C25" s="87" t="s">
+      <c r="C25" s="110" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="88"/>
-      <c r="E25" s="88"/>
+      <c r="D25" s="131"/>
+      <c r="E25" s="131"/>
       <c r="F25" s="42">
         <v>20</v>
       </c>
@@ -2982,11 +2957,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C26" s="87" t="s">
+      <c r="C26" s="110" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="88"/>
-      <c r="E26" s="88"/>
+      <c r="D26" s="131"/>
+      <c r="E26" s="131"/>
       <c r="F26" s="42">
         <v>16</v>
       </c>
@@ -3035,11 +3010,11 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C27" s="87" t="s">
+      <c r="C27" s="110" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="88"/>
-      <c r="E27" s="88"/>
+      <c r="D27" s="131"/>
+      <c r="E27" s="131"/>
       <c r="F27" s="42">
         <v>30</v>
       </c>
@@ -3088,11 +3063,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C28" s="87" t="s">
+      <c r="C28" s="110" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="103"/>
-      <c r="E28" s="104"/>
+      <c r="D28" s="111"/>
+      <c r="E28" s="112"/>
       <c r="F28" s="42">
         <v>18</v>
       </c>
@@ -3141,11 +3116,11 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C29" s="87" t="s">
+      <c r="C29" s="110" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="88"/>
-      <c r="E29" s="88"/>
+      <c r="D29" s="131"/>
+      <c r="E29" s="131"/>
       <c r="F29" s="42">
         <v>30</v>
       </c>
@@ -3194,11 +3169,11 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C30" s="87" t="s">
+      <c r="C30" s="110" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="88"/>
-      <c r="E30" s="88"/>
+      <c r="D30" s="131"/>
+      <c r="E30" s="131"/>
       <c r="F30" s="42">
         <v>15</v>
       </c>
@@ -3247,36 +3222,36 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C31" s="87" t="s">
+      <c r="C31" s="110" t="s">
         <v>48</v>
       </c>
-      <c r="D31" s="103"/>
-      <c r="E31" s="104"/>
-      <c r="F31" s="125">
+      <c r="D31" s="111"/>
+      <c r="E31" s="112"/>
+      <c r="F31" s="87">
         <v>17</v>
       </c>
-      <c r="G31" s="132">
+      <c r="G31" s="94">
         <v>2.4305555555555556E-2</v>
       </c>
-      <c r="H31" s="126">
+      <c r="H31" s="88">
         <v>3.0555555555555555E-2</v>
       </c>
-      <c r="I31" s="127">
+      <c r="I31" s="89">
         <v>4.5138888888888888E-2</v>
       </c>
-      <c r="J31" s="128">
+      <c r="J31" s="90">
         <v>1.4583333333333171E-2</v>
       </c>
-      <c r="K31" s="129">
+      <c r="K31" s="91">
         <v>0</v>
       </c>
-      <c r="L31" s="133">
+      <c r="L31" s="95">
         <v>0</v>
       </c>
-      <c r="M31" s="130">
+      <c r="M31" s="92">
         <v>17</v>
       </c>
-      <c r="N31" s="131">
+      <c r="N31" s="93">
         <v>1.4583333333333171E-2</v>
       </c>
       <c r="O31" s="86"/>
@@ -3292,158 +3267,158 @@
       <c r="Y31" s="22"/>
       <c r="Z31" s="22"/>
     </row>
-    <row r="32" spans="1:26" s="147" customFormat="1" ht="15" customHeight="1">
-      <c r="A32" s="134"/>
-      <c r="B32" s="135">
+    <row r="32" spans="1:26" s="109" customFormat="1" ht="15" customHeight="1">
+      <c r="A32" s="96"/>
+      <c r="B32" s="97">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C32" s="111" t="s">
+      <c r="C32" s="113" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="112"/>
-      <c r="E32" s="112"/>
-      <c r="F32" s="136">
+      <c r="D32" s="114"/>
+      <c r="E32" s="114"/>
+      <c r="F32" s="98">
         <v>20</v>
       </c>
-      <c r="G32" s="137">
+      <c r="G32" s="99">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="H32" s="138">
+      <c r="H32" s="100">
         <v>0.41388888888888892</v>
       </c>
-      <c r="I32" s="139">
+      <c r="I32" s="101">
         <v>0.43541666666666662</v>
       </c>
-      <c r="J32" s="140">
+      <c r="J32" s="102">
         <v>2.1527777777777701E-2</v>
       </c>
-      <c r="K32" s="141">
+      <c r="K32" s="103">
         <v>1</v>
       </c>
-      <c r="L32" s="142">
+      <c r="L32" s="104">
         <v>1.3888888888888889E-3</v>
       </c>
-      <c r="M32" s="143">
+      <c r="M32" s="105">
         <v>13</v>
       </c>
-      <c r="N32" s="144">
+      <c r="N32" s="106">
         <v>2.2916666666666589E-2</v>
       </c>
-      <c r="O32" s="134"/>
-      <c r="P32" s="145"/>
-      <c r="Q32" s="146"/>
-      <c r="R32" s="146"/>
-      <c r="S32" s="146"/>
-      <c r="T32" s="146"/>
-      <c r="U32" s="146"/>
-      <c r="V32" s="146"/>
-      <c r="W32" s="146"/>
-      <c r="X32" s="146"/>
-      <c r="Y32" s="146"/>
-      <c r="Z32" s="146"/>
-    </row>
-    <row r="33" spans="1:26" s="147" customFormat="1" ht="15" customHeight="1">
-      <c r="A33" s="134"/>
-      <c r="B33" s="135">
+      <c r="O32" s="96"/>
+      <c r="P32" s="107"/>
+      <c r="Q32" s="108"/>
+      <c r="R32" s="108"/>
+      <c r="S32" s="108"/>
+      <c r="T32" s="108"/>
+      <c r="U32" s="108"/>
+      <c r="V32" s="108"/>
+      <c r="W32" s="108"/>
+      <c r="X32" s="108"/>
+      <c r="Y32" s="108"/>
+      <c r="Z32" s="108"/>
+    </row>
+    <row r="33" spans="1:26" s="109" customFormat="1" ht="15" customHeight="1">
+      <c r="A33" s="96"/>
+      <c r="B33" s="97">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C33" s="111" t="s">
+      <c r="C33" s="113" t="s">
         <v>50</v>
       </c>
-      <c r="D33" s="112"/>
-      <c r="E33" s="112"/>
-      <c r="F33" s="136">
+      <c r="D33" s="114"/>
+      <c r="E33" s="114"/>
+      <c r="F33" s="98">
         <v>18</v>
       </c>
-      <c r="G33" s="137">
+      <c r="G33" s="99">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="H33" s="138">
+      <c r="H33" s="100">
         <v>0.43611111111111112</v>
       </c>
-      <c r="I33" s="139">
+      <c r="I33" s="101">
         <v>0.4597222222222222</v>
       </c>
-      <c r="J33" s="140">
+      <c r="J33" s="102">
         <v>2.3611111111111083E-2</v>
       </c>
-      <c r="K33" s="141">
+      <c r="K33" s="103">
         <v>0</v>
       </c>
-      <c r="L33" s="142">
+      <c r="L33" s="104">
         <v>0</v>
       </c>
-      <c r="M33" s="143">
+      <c r="M33" s="105">
         <v>14</v>
       </c>
-      <c r="N33" s="144">
+      <c r="N33" s="106">
         <v>2.3611111111111083E-2</v>
       </c>
-      <c r="O33" s="134"/>
-      <c r="P33" s="145"/>
-      <c r="Q33" s="146"/>
-      <c r="R33" s="146"/>
-      <c r="S33" s="146"/>
-      <c r="T33" s="146"/>
-      <c r="U33" s="146"/>
-      <c r="V33" s="146"/>
-      <c r="W33" s="146"/>
-      <c r="X33" s="146"/>
-      <c r="Y33" s="146"/>
-      <c r="Z33" s="146"/>
-    </row>
-    <row r="34" spans="1:26" s="147" customFormat="1" ht="15" customHeight="1">
-      <c r="A34" s="134"/>
-      <c r="B34" s="135">
+      <c r="O33" s="96"/>
+      <c r="P33" s="107"/>
+      <c r="Q33" s="108"/>
+      <c r="R33" s="108"/>
+      <c r="S33" s="108"/>
+      <c r="T33" s="108"/>
+      <c r="U33" s="108"/>
+      <c r="V33" s="108"/>
+      <c r="W33" s="108"/>
+      <c r="X33" s="108"/>
+      <c r="Y33" s="108"/>
+      <c r="Z33" s="108"/>
+    </row>
+    <row r="34" spans="1:26" s="109" customFormat="1" ht="15" customHeight="1">
+      <c r="A34" s="96"/>
+      <c r="B34" s="97">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C34" s="111" t="s">
+      <c r="C34" s="113" t="s">
         <v>51</v>
       </c>
-      <c r="D34" s="112"/>
-      <c r="E34" s="112"/>
-      <c r="F34" s="136">
+      <c r="D34" s="114"/>
+      <c r="E34" s="114"/>
+      <c r="F34" s="98">
         <v>20</v>
       </c>
-      <c r="G34" s="137">
+      <c r="G34" s="99">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="H34" s="138">
+      <c r="H34" s="100">
         <v>0.46527777777777773</v>
       </c>
-      <c r="I34" s="139">
+      <c r="I34" s="101">
         <v>0.4826388888888889</v>
       </c>
-      <c r="J34" s="140">
+      <c r="J34" s="102">
         <v>1.736111111111116E-2</v>
       </c>
-      <c r="K34" s="141">
+      <c r="K34" s="103">
         <v>1</v>
       </c>
-      <c r="L34" s="142">
+      <c r="L34" s="104">
         <v>2.0833333333333333E-3</v>
       </c>
-      <c r="M34" s="143">
+      <c r="M34" s="105">
         <v>15</v>
       </c>
-      <c r="N34" s="144">
+      <c r="N34" s="106">
         <v>1.9444444444444493E-2</v>
       </c>
-      <c r="O34" s="134"/>
-      <c r="P34" s="145"/>
-      <c r="Q34" s="146"/>
-      <c r="R34" s="146"/>
-      <c r="S34" s="146"/>
-      <c r="T34" s="146"/>
-      <c r="U34" s="146"/>
-      <c r="V34" s="146"/>
-      <c r="W34" s="146"/>
-      <c r="X34" s="146"/>
-      <c r="Y34" s="146"/>
-      <c r="Z34" s="146"/>
+      <c r="O34" s="96"/>
+      <c r="P34" s="107"/>
+      <c r="Q34" s="108"/>
+      <c r="R34" s="108"/>
+      <c r="S34" s="108"/>
+      <c r="T34" s="108"/>
+      <c r="U34" s="108"/>
+      <c r="V34" s="108"/>
+      <c r="W34" s="108"/>
+      <c r="X34" s="108"/>
+      <c r="Y34" s="108"/>
+      <c r="Z34" s="108"/>
     </row>
     <row r="35" spans="1:26" ht="15" customHeight="1">
       <c r="A35" s="86"/>
@@ -3451,23 +3426,39 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C35" s="87"/>
-      <c r="D35" s="88"/>
-      <c r="E35" s="88"/>
-      <c r="F35" s="42"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="44"/>
-      <c r="I35" s="45"/>
-      <c r="J35" s="35" t="str">
+      <c r="C35" s="110" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="131"/>
+      <c r="E35" s="131"/>
+      <c r="F35" s="42">
+        <v>25</v>
+      </c>
+      <c r="G35" s="43">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="H35" s="44">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="I35" s="45">
+        <v>6.25E-2</v>
+      </c>
+      <c r="J35" s="35">
         <f t="shared" si="5"/>
-        <v/>
+        <v>4.1666666666666671E-2</v>
       </c>
-      <c r="K35" s="46"/>
-      <c r="L35" s="47"/>
-      <c r="M35" s="48"/>
-      <c r="N35" s="39" t="str">
+      <c r="K35" s="46">
+        <v>2</v>
+      </c>
+      <c r="L35" s="47">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="M35" s="48">
+        <v>16</v>
+      </c>
+      <c r="N35" s="39">
         <f t="shared" si="4"/>
-        <v/>
+        <v>5.5555555555555559E-2</v>
       </c>
       <c r="O35" s="86"/>
       <c r="P35" s="21"/>
@@ -3488,9 +3479,9 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C36" s="87"/>
-      <c r="D36" s="88"/>
-      <c r="E36" s="88"/>
+      <c r="C36" s="110"/>
+      <c r="D36" s="131"/>
+      <c r="E36" s="131"/>
       <c r="F36" s="42"/>
       <c r="G36" s="43"/>
       <c r="H36" s="44"/>
@@ -3525,9 +3516,9 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C37" s="87"/>
-      <c r="D37" s="88"/>
-      <c r="E37" s="88"/>
+      <c r="C37" s="110"/>
+      <c r="D37" s="131"/>
+      <c r="E37" s="131"/>
       <c r="F37" s="42"/>
       <c r="G37" s="43"/>
       <c r="H37" s="44"/>
@@ -3562,9 +3553,9 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C38" s="87"/>
-      <c r="D38" s="103"/>
-      <c r="E38" s="104"/>
+      <c r="C38" s="110"/>
+      <c r="D38" s="111"/>
+      <c r="E38" s="112"/>
       <c r="F38" s="42"/>
       <c r="G38" s="43"/>
       <c r="H38" s="44"/>
@@ -3595,19 +3586,19 @@
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1">
       <c r="A39" s="7"/>
-      <c r="B39" s="116" t="s">
+      <c r="B39" s="118" t="s">
         <v>23</v>
       </c>
-      <c r="C39" s="102"/>
-      <c r="D39" s="102"/>
-      <c r="E39" s="102"/>
+      <c r="C39" s="119"/>
+      <c r="D39" s="119"/>
+      <c r="E39" s="119"/>
       <c r="F39" s="49">
         <f>IF(SUM(F18:F38)=0,"Completar",SUM(F18:F38))</f>
-        <v>332</v>
+        <v>357</v>
       </c>
       <c r="G39" s="50">
         <f>IF(SUM(G18:G38)=0,"Completar",SUM(G18:G38))</f>
-        <v>0.24374999999999999</v>
+        <v>0.27152777777777776</v>
       </c>
       <c r="H39" s="51" t="s">
         <v>24</v>
@@ -3617,23 +3608,23 @@
       </c>
       <c r="J39" s="53">
         <f>IF(OR(COUNTIF(J18:J38,"Error")&gt;0,COUNTIF(J18:J38,"Completar")&gt;0),"Error",IF(SUM(J18:J38)=0,"Completar",SUM(J18:J38)))</f>
-        <v>0.22986111111111113</v>
+        <v>0.27152777777777781</v>
       </c>
       <c r="K39" s="54">
         <f>SUM(K18:K38)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="L39" s="50">
         <f>SUM(L18:L38)</f>
-        <v>3.0555555555555555E-2</v>
+        <v>4.4444444444444439E-2</v>
       </c>
       <c r="M39" s="55">
         <f>IF(SUM(M18:M38)=0,"Completar",SUM(M18:M38))</f>
-        <v>292</v>
+        <v>308</v>
       </c>
       <c r="N39" s="18">
         <f>IF(OR(COUNTIF(N18:N38,"Error")&gt;0,COUNTIF(N18:N38,"Completar")&gt;0),"Error",IF(SUM(N18:N38)=0,"Completar",SUM(N18:N38)))</f>
-        <v>0.26041666666666669</v>
+        <v>0.31597222222222227</v>
       </c>
       <c r="O39" s="7"/>
       <c r="P39" s="56"/>
@@ -3678,12 +3669,12 @@
     </row>
     <row r="41" spans="1:26" ht="15" customHeight="1">
       <c r="A41" s="4"/>
-      <c r="B41" s="91" t="s">
+      <c r="B41" s="115" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="92"/>
-      <c r="D41" s="92"/>
-      <c r="E41" s="93"/>
+      <c r="C41" s="116"/>
+      <c r="D41" s="116"/>
+      <c r="E41" s="117"/>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
@@ -3803,21 +3794,21 @@
     </row>
     <row r="45" spans="1:26">
       <c r="A45" s="20"/>
-      <c r="B45" s="91" t="s">
+      <c r="B45" s="115" t="s">
         <v>26</v>
       </c>
-      <c r="C45" s="92"/>
-      <c r="D45" s="92"/>
-      <c r="E45" s="92"/>
-      <c r="F45" s="92"/>
-      <c r="G45" s="92"/>
-      <c r="H45" s="92"/>
-      <c r="I45" s="92"/>
-      <c r="J45" s="92"/>
-      <c r="K45" s="92"/>
-      <c r="L45" s="92"/>
-      <c r="M45" s="92"/>
-      <c r="N45" s="93"/>
+      <c r="C45" s="116"/>
+      <c r="D45" s="116"/>
+      <c r="E45" s="116"/>
+      <c r="F45" s="116"/>
+      <c r="G45" s="116"/>
+      <c r="H45" s="116"/>
+      <c r="I45" s="116"/>
+      <c r="J45" s="116"/>
+      <c r="K45" s="116"/>
+      <c r="L45" s="116"/>
+      <c r="M45" s="116"/>
+      <c r="N45" s="117"/>
       <c r="O45" s="20"/>
       <c r="P45" s="59"/>
       <c r="Q45" s="59"/>
@@ -3833,16 +3824,16 @@
     </row>
     <row r="46" spans="1:26" ht="15" customHeight="1">
       <c r="A46" s="20"/>
-      <c r="B46" s="97" t="s">
+      <c r="B46" s="135" t="s">
         <v>27</v>
       </c>
-      <c r="C46" s="88"/>
-      <c r="D46" s="98"/>
-      <c r="E46" s="107">
+      <c r="C46" s="131"/>
+      <c r="D46" s="136"/>
+      <c r="E46" s="137">
         <f>M39</f>
-        <v>292</v>
+        <v>308</v>
       </c>
-      <c r="F46" s="98"/>
+      <c r="F46" s="136"/>
       <c r="G46" s="60"/>
       <c r="H46" s="61"/>
       <c r="I46" s="61"/>
@@ -3866,16 +3857,16 @@
     </row>
     <row r="47" spans="1:26">
       <c r="A47" s="20"/>
-      <c r="B47" s="97" t="s">
+      <c r="B47" s="135" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="88"/>
-      <c r="D47" s="98"/>
-      <c r="E47" s="106">
+      <c r="C47" s="131"/>
+      <c r="D47" s="136"/>
+      <c r="E47" s="145">
         <f>IF(M39="Completar","Completar",IFERROR(M39/(N39*24),"Error"))</f>
-        <v>46.72</v>
+        <v>40.615384615384613</v>
       </c>
-      <c r="F47" s="98"/>
+      <c r="F47" s="136"/>
       <c r="G47" s="63"/>
       <c r="H47" s="64"/>
       <c r="I47" s="64"/>
@@ -3899,16 +3890,16 @@
     </row>
     <row r="48" spans="1:26" ht="15" customHeight="1">
       <c r="A48" s="20"/>
-      <c r="B48" s="97" t="s">
+      <c r="B48" s="135" t="s">
         <v>29</v>
       </c>
-      <c r="C48" s="88"/>
-      <c r="D48" s="98"/>
-      <c r="E48" s="107">
+      <c r="C48" s="131"/>
+      <c r="D48" s="136"/>
+      <c r="E48" s="137">
         <f>IF(K39=0,0,IFERROR(ROUNDUP(K39/(M39/100),0),"Error"))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
-      <c r="F48" s="98"/>
+      <c r="F48" s="136"/>
       <c r="G48" s="63"/>
       <c r="H48" s="64"/>
       <c r="I48" s="64"/>
@@ -3932,16 +3923,16 @@
     </row>
     <row r="49" spans="1:26" ht="15" customHeight="1">
       <c r="A49" s="20"/>
-      <c r="B49" s="97" t="s">
+      <c r="B49" s="135" t="s">
         <v>30</v>
       </c>
-      <c r="C49" s="88"/>
-      <c r="D49" s="98"/>
-      <c r="E49" s="105">
+      <c r="C49" s="131"/>
+      <c r="D49" s="136"/>
+      <c r="E49" s="144">
         <f>IF(K39=0,0,IFERROR(K39/M39,"Error"))</f>
-        <v>4.7945205479452052E-2</v>
+        <v>5.1948051948051951E-2</v>
       </c>
-      <c r="F49" s="98"/>
+      <c r="F49" s="136"/>
       <c r="G49" s="63"/>
       <c r="H49" s="64"/>
       <c r="I49" s="64"/>
@@ -3965,18 +3956,18 @@
     </row>
     <row r="50" spans="1:26" ht="15" customHeight="1">
       <c r="A50" s="20"/>
-      <c r="B50" s="97" t="s">
+      <c r="B50" s="135" t="s">
         <v>31</v>
       </c>
-      <c r="C50" s="88"/>
-      <c r="D50" s="98"/>
+      <c r="C50" s="131"/>
+      <c r="D50" s="136"/>
       <c r="E50" s="66">
         <f>E5</f>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="F50" s="67">
         <f t="shared" ref="F50:F53" si="6">IF(E50="Completar",E50,IFERROR(E50/$E$56,"Error"))</f>
-        <v>2.5974025974025882E-2</v>
+        <v>2.1505376344085943E-2</v>
       </c>
       <c r="G50" s="63"/>
       <c r="H50" s="64"/>
@@ -4001,11 +3992,11 @@
     </row>
     <row r="51" spans="1:26" ht="15" customHeight="1">
       <c r="A51" s="20"/>
-      <c r="B51" s="97" t="s">
+      <c r="B51" s="135" t="s">
         <v>32</v>
       </c>
-      <c r="C51" s="88"/>
-      <c r="D51" s="98"/>
+      <c r="C51" s="131"/>
+      <c r="D51" s="136"/>
       <c r="E51" s="66" t="str">
         <f>E9</f>
         <v>Completar</v>
@@ -4037,11 +4028,11 @@
     </row>
     <row r="52" spans="1:26" ht="15" customHeight="1">
       <c r="A52" s="20"/>
-      <c r="B52" s="97" t="s">
+      <c r="B52" s="135" t="s">
         <v>33</v>
       </c>
-      <c r="C52" s="88"/>
-      <c r="D52" s="98"/>
+      <c r="C52" s="131"/>
+      <c r="D52" s="136"/>
       <c r="E52" s="66" t="str">
         <f>E13</f>
         <v>Completar</v>
@@ -4073,11 +4064,11 @@
     </row>
     <row r="53" spans="1:26" ht="15" customHeight="1">
       <c r="A53" s="20"/>
-      <c r="B53" s="97" t="s">
+      <c r="B53" s="135" t="s">
         <v>34</v>
       </c>
-      <c r="C53" s="88"/>
-      <c r="D53" s="98"/>
+      <c r="C53" s="131"/>
+      <c r="D53" s="136"/>
       <c r="E53" s="66" t="str">
         <f>E43</f>
         <v>Completar</v>
@@ -4109,18 +4100,18 @@
     </row>
     <row r="54" spans="1:26" ht="15" customHeight="1">
       <c r="A54" s="20"/>
-      <c r="B54" s="97" t="s">
+      <c r="B54" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="C54" s="88"/>
-      <c r="D54" s="98"/>
+      <c r="C54" s="131"/>
+      <c r="D54" s="136"/>
       <c r="E54" s="66">
         <f>L39</f>
-        <v>3.0555555555555555E-2</v>
+        <v>4.4444444444444439E-2</v>
       </c>
       <c r="F54" s="67">
         <f t="shared" ref="F54:F55" si="7">IF(E54="Completar",E54,IFERROR(E54/$E$56,"Completar"))</f>
-        <v>0.11428571428571428</v>
+        <v>0.13763440860215051</v>
       </c>
       <c r="G54" s="63"/>
       <c r="H54" s="64"/>
@@ -4145,18 +4136,18 @@
     </row>
     <row r="55" spans="1:26" ht="15" customHeight="1">
       <c r="A55" s="20"/>
-      <c r="B55" s="97" t="s">
+      <c r="B55" s="135" t="s">
         <v>36</v>
       </c>
-      <c r="C55" s="88"/>
-      <c r="D55" s="98"/>
+      <c r="C55" s="131"/>
+      <c r="D55" s="136"/>
       <c r="E55" s="66">
         <f>J39</f>
-        <v>0.22986111111111113</v>
+        <v>0.27152777777777781</v>
       </c>
       <c r="F55" s="67">
         <f t="shared" si="7"/>
-        <v>0.8597402597402598</v>
+        <v>0.84086021505376352</v>
       </c>
       <c r="G55" s="63"/>
       <c r="H55" s="64"/>
@@ -4181,16 +4172,16 @@
     </row>
     <row r="56" spans="1:26" ht="15" customHeight="1">
       <c r="A56" s="20"/>
-      <c r="B56" s="101" t="s">
+      <c r="B56" s="143" t="s">
         <v>37</v>
       </c>
-      <c r="C56" s="102"/>
-      <c r="D56" s="100"/>
-      <c r="E56" s="99">
+      <c r="C56" s="119"/>
+      <c r="D56" s="142"/>
+      <c r="E56" s="141">
         <f>IF(COUNTIF(E50:E55,"Error")&gt;0,"Error",IF(SUM(E50:E55)=0,"Completar",SUM(E50:E55)))</f>
-        <v>0.2673611111111111</v>
+        <v>0.32291666666666669</v>
       </c>
-      <c r="F56" s="100"/>
+      <c r="F56" s="142"/>
       <c r="G56" s="68"/>
       <c r="H56" s="69"/>
       <c r="I56" s="69"/>
@@ -31010,36 +31001,13 @@
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B45:N45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="D1:N1"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F8:N8"/>
+    <mergeCell ref="F9:N9"/>
     <mergeCell ref="B15:N15"/>
     <mergeCell ref="F12:N12"/>
     <mergeCell ref="F13:N13"/>
@@ -31056,13 +31024,36 @@
     <mergeCell ref="E49:F49"/>
     <mergeCell ref="B49:D49"/>
     <mergeCell ref="E47:F47"/>
-    <mergeCell ref="D1:N1"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="F8:N8"/>
-    <mergeCell ref="F9:N9"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B45:N45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="B39:E39"/>
     <mergeCell ref="C37:E37"/>
     <mergeCell ref="C35:E35"/>
     <mergeCell ref="C36:E36"/>

</xml_diff>

<commit_message>
Agregado Ultimos Metodos MatrizMath - Luego corrijo formato
</commit_message>
<xml_diff>
--- a/Documentacion/MatrizMath/MatrizMath - Planilla de Métricas V2.1.xlsx
+++ b/Documentacion/MatrizMath/MatrizMath - Planilla de Métricas V2.1.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BKP ALMIRON\ENZO-AMS\TEIC\Nueva carpeta\PROG III\TP2\TP2-RepoGus\Documentacion\MatrizMath\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900"/>
   </bookViews>
   <sheets>
     <sheet name="Métricas" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
   <si>
     <t>PROYECTO:</t>
   </si>
@@ -174,16 +179,28 @@
   <si>
     <t>producto(VectorMath)</t>
   </si>
+  <si>
+    <t>adjuntarDerechaIdentidad()</t>
+  </si>
+  <si>
+    <t>tomarMatrizCuadradaALaDerecha()</t>
+  </si>
+  <si>
+    <t>tratarDiagonalPrincipal()</t>
+  </si>
+  <si>
+    <t>invertir() MatrizMath</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -248,8 +265,27 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12.1"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12.1"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12.1"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -298,8 +334,20 @@
         <bgColor rgb="FFC6D9F0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDBE5F1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF95B3D7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="41">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -803,11 +851,102 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="double">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1132,6 +1271,40 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="8" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1141,27 +1314,37 @@
     <xf numFmtId="49" fontId="8" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1172,49 +1355,62 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="12" fillId="9" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="12" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="13" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="7" fillId="9" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="7" fillId="9" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="7" fillId="10" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="7" fillId="10" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1483,9 +1679,18 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -1506,12 +1711,13 @@
           <c:order val="0"/>
           <c:dPt>
             <c:idx val="0"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="FFC000"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-49DD-4FD5-A2AE-26863999DE8F}"/>
               </c:ext>
@@ -1519,12 +1725,13 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="00B0F0"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-49DD-4FD5-A2AE-26863999DE8F}"/>
               </c:ext>
@@ -1532,12 +1739,13 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="0066FF"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-49DD-4FD5-A2AE-26863999DE8F}"/>
               </c:ext>
@@ -1545,12 +1753,13 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="009900"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-49DD-4FD5-A2AE-26863999DE8F}"/>
               </c:ext>
@@ -1558,12 +1767,13 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000009-49DD-4FD5-A2AE-26863999DE8F}"/>
               </c:ext>
@@ -1571,12 +1781,13 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="002060"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000B-49DD-4FD5-A2AE-26863999DE8F}"/>
               </c:ext>
@@ -1584,7 +1795,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Métricas!$B$50:$B$55</c:f>
+              <c:f>Métricas!$B$53:$B$58</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1610,20 +1821,28 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Métricas!$C$50:$C$55</c:f>
+              <c:f>Métricas!$C$53:$C$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000C-49DD-4FD5-A2AE-26863999DE8F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
       <c:spPr>
@@ -1635,6 +1854,7 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
@@ -1654,13 +1874,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1938,21 +2158,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z1013"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N35" sqref="N35"/>
+    <sheetView tabSelected="1" topLeftCell="B33" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
@@ -1968,23 +2188,23 @@
   <sheetData>
     <row r="1" spans="1:26" ht="23.25" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="147" t="s">
+      <c r="B1" s="116" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="139"/>
-      <c r="D1" s="146" t="s">
+      <c r="C1" s="112"/>
+      <c r="D1" s="111" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="139"/>
-      <c r="F1" s="139"/>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
-      <c r="J1" s="139"/>
-      <c r="K1" s="139"/>
-      <c r="L1" s="139"/>
-      <c r="M1" s="139"/>
-      <c r="N1" s="139"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="112"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -2028,12 +2248,12 @@
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
       <c r="A3" s="4"/>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="116"/>
-      <c r="D3" s="116"/>
-      <c r="E3" s="117"/>
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="115"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -2159,12 +2379,12 @@
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1">
       <c r="A7" s="4"/>
-      <c r="B7" s="115" t="s">
+      <c r="B7" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="116"/>
-      <c r="D7" s="116"/>
-      <c r="E7" s="117"/>
+      <c r="C7" s="114"/>
+      <c r="D7" s="114"/>
+      <c r="E7" s="115"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -2201,15 +2421,15 @@
       <c r="E8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="138"/>
-      <c r="G8" s="139"/>
-      <c r="H8" s="139"/>
-      <c r="I8" s="139"/>
-      <c r="J8" s="139"/>
-      <c r="K8" s="139"/>
-      <c r="L8" s="139"/>
-      <c r="M8" s="139"/>
-      <c r="N8" s="139"/>
+      <c r="F8" s="117"/>
+      <c r="G8" s="112"/>
+      <c r="H8" s="112"/>
+      <c r="I8" s="112"/>
+      <c r="J8" s="112"/>
+      <c r="K8" s="112"/>
+      <c r="L8" s="112"/>
+      <c r="M8" s="112"/>
+      <c r="N8" s="112"/>
       <c r="O8" s="7"/>
       <c r="P8" s="13"/>
       <c r="Q8" s="14"/>
@@ -2236,15 +2456,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C9),ISBLANK(D9)),"Completar",IF(D9&gt;=C9,D9-C9,"Error")),"Error")</f>
         <v>Completar</v>
       </c>
-      <c r="F9" s="140"/>
-      <c r="G9" s="139"/>
-      <c r="H9" s="139"/>
-      <c r="I9" s="139"/>
-      <c r="J9" s="139"/>
-      <c r="K9" s="139"/>
-      <c r="L9" s="139"/>
-      <c r="M9" s="139"/>
-      <c r="N9" s="139"/>
+      <c r="F9" s="118"/>
+      <c r="G9" s="112"/>
+      <c r="H9" s="112"/>
+      <c r="I9" s="112"/>
+      <c r="J9" s="112"/>
+      <c r="K9" s="112"/>
+      <c r="L9" s="112"/>
+      <c r="M9" s="112"/>
+      <c r="N9" s="112"/>
       <c r="O9" s="15"/>
       <c r="P9" s="21"/>
       <c r="Q9" s="22"/>
@@ -2288,12 +2508,12 @@
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" s="4"/>
-      <c r="B11" s="115" t="s">
+      <c r="B11" s="113" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="116"/>
-      <c r="D11" s="116"/>
-      <c r="E11" s="117"/>
+      <c r="C11" s="114"/>
+      <c r="D11" s="114"/>
+      <c r="E11" s="115"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -2330,15 +2550,15 @@
       <c r="E12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="138"/>
-      <c r="G12" s="139"/>
-      <c r="H12" s="139"/>
-      <c r="I12" s="139"/>
-      <c r="J12" s="139"/>
-      <c r="K12" s="139"/>
-      <c r="L12" s="139"/>
-      <c r="M12" s="139"/>
-      <c r="N12" s="139"/>
+      <c r="F12" s="117"/>
+      <c r="G12" s="112"/>
+      <c r="H12" s="112"/>
+      <c r="I12" s="112"/>
+      <c r="J12" s="112"/>
+      <c r="K12" s="112"/>
+      <c r="L12" s="112"/>
+      <c r="M12" s="112"/>
+      <c r="N12" s="112"/>
       <c r="O12" s="7"/>
       <c r="P12" s="13"/>
       <c r="Q12" s="14"/>
@@ -2363,15 +2583,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C13),ISBLANK(D13)),"Completar",IF(D13&gt;=C13,D13-C13,"Error")),"Error")</f>
         <v>Completar</v>
       </c>
-      <c r="F13" s="140"/>
-      <c r="G13" s="139"/>
-      <c r="H13" s="139"/>
-      <c r="I13" s="139"/>
-      <c r="J13" s="139"/>
-      <c r="K13" s="139"/>
-      <c r="L13" s="139"/>
-      <c r="M13" s="139"/>
-      <c r="N13" s="139"/>
+      <c r="F13" s="118"/>
+      <c r="G13" s="112"/>
+      <c r="H13" s="112"/>
+      <c r="I13" s="112"/>
+      <c r="J13" s="112"/>
+      <c r="K13" s="112"/>
+      <c r="L13" s="112"/>
+      <c r="M13" s="112"/>
+      <c r="N13" s="112"/>
       <c r="O13" s="15"/>
       <c r="P13" s="21"/>
       <c r="Q13" s="22"/>
@@ -2415,21 +2635,21 @@
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1">
       <c r="A15" s="4"/>
-      <c r="B15" s="115" t="s">
+      <c r="B15" s="113" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="116"/>
-      <c r="D15" s="116"/>
-      <c r="E15" s="116"/>
-      <c r="F15" s="116"/>
-      <c r="G15" s="116"/>
-      <c r="H15" s="116"/>
-      <c r="I15" s="116"/>
-      <c r="J15" s="116"/>
-      <c r="K15" s="116"/>
-      <c r="L15" s="116"/>
-      <c r="M15" s="116"/>
-      <c r="N15" s="117"/>
+      <c r="C15" s="114"/>
+      <c r="D15" s="114"/>
+      <c r="E15" s="114"/>
+      <c r="F15" s="114"/>
+      <c r="G15" s="114"/>
+      <c r="H15" s="114"/>
+      <c r="I15" s="114"/>
+      <c r="J15" s="114"/>
+      <c r="K15" s="114"/>
+      <c r="L15" s="114"/>
+      <c r="M15" s="114"/>
+      <c r="N15" s="115"/>
       <c r="O15" s="4"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
@@ -2445,28 +2665,28 @@
     </row>
     <row r="16" spans="1:26" ht="16.5" customHeight="1">
       <c r="A16" s="7"/>
-      <c r="B16" s="124" t="s">
+      <c r="B16" s="142" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="126" t="s">
+      <c r="C16" s="144" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="127"/>
-      <c r="E16" s="127"/>
-      <c r="F16" s="122" t="s">
+      <c r="D16" s="145"/>
+      <c r="E16" s="145"/>
+      <c r="F16" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="123"/>
-      <c r="H16" s="134" t="s">
+      <c r="G16" s="139"/>
+      <c r="H16" s="137" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="131"/>
-      <c r="J16" s="131"/>
-      <c r="K16" s="122" t="s">
+      <c r="I16" s="120"/>
+      <c r="J16" s="120"/>
+      <c r="K16" s="138" t="s">
         <v>14</v>
       </c>
-      <c r="L16" s="123"/>
-      <c r="M16" s="120" t="s">
+      <c r="L16" s="139"/>
+      <c r="M16" s="140" t="s">
         <v>15</v>
       </c>
       <c r="N16" s="132" t="s">
@@ -2487,10 +2707,10 @@
     </row>
     <row r="17" spans="1:26" ht="30" customHeight="1">
       <c r="A17" s="7"/>
-      <c r="B17" s="125"/>
-      <c r="C17" s="128"/>
-      <c r="D17" s="129"/>
-      <c r="E17" s="129"/>
+      <c r="B17" s="143"/>
+      <c r="C17" s="146"/>
+      <c r="D17" s="147"/>
+      <c r="E17" s="147"/>
       <c r="F17" s="26" t="s">
         <v>16</v>
       </c>
@@ -2512,7 +2732,7 @@
       <c r="L17" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="M17" s="121"/>
+      <c r="M17" s="141"/>
       <c r="N17" s="133"/>
       <c r="O17" s="7"/>
       <c r="P17" s="13"/>
@@ -2530,14 +2750,14 @@
     <row r="18" spans="1:26">
       <c r="A18" s="15"/>
       <c r="B18" s="30">
-        <f t="shared" ref="B18:B38" si="0">ROW($B18)-16</f>
+        <f t="shared" ref="B18:B41" si="0">ROW($B18)-16</f>
         <v>2</v>
       </c>
-      <c r="C18" s="130" t="s">
+      <c r="C18" s="134" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="131"/>
-      <c r="E18" s="131"/>
+      <c r="D18" s="120"/>
+      <c r="E18" s="120"/>
       <c r="F18" s="31">
         <v>60</v>
       </c>
@@ -2561,7 +2781,7 @@
         <v>7.6388888888888886E-3</v>
       </c>
       <c r="M18" s="38">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="N18" s="39">
         <f t="shared" ref="N18:N27" si="2">IFERROR(IF(OR(J18="",ISBLANK(L18)),"",J18+L18),"Error")</f>
@@ -2586,11 +2806,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C19" s="130" t="s">
+      <c r="C19" s="134" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="131"/>
-      <c r="E19" s="131"/>
+      <c r="D19" s="120"/>
+      <c r="E19" s="120"/>
       <c r="F19" s="31">
         <v>4</v>
       </c>
@@ -2614,7 +2834,7 @@
         <v>0</v>
       </c>
       <c r="M19" s="38">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="N19" s="39">
         <f t="shared" si="2"/>
@@ -2639,11 +2859,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C20" s="130" t="s">
+      <c r="C20" s="134" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="131"/>
-      <c r="E20" s="131"/>
+      <c r="D20" s="120"/>
+      <c r="E20" s="120"/>
       <c r="F20" s="31">
         <v>8</v>
       </c>
@@ -2692,11 +2912,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C21" s="130" t="s">
+      <c r="C21" s="134" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="131"/>
-      <c r="E21" s="131"/>
+      <c r="D21" s="120"/>
+      <c r="E21" s="120"/>
       <c r="F21" s="31">
         <v>10</v>
       </c>
@@ -2745,11 +2965,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C22" s="113" t="s">
+      <c r="C22" s="135" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="114"/>
-      <c r="E22" s="114"/>
+      <c r="D22" s="136"/>
+      <c r="E22" s="136"/>
       <c r="F22" s="74">
         <v>8</v>
       </c>
@@ -2798,11 +3018,11 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C23" s="110" t="s">
+      <c r="C23" s="126" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="131"/>
-      <c r="E23" s="131"/>
+      <c r="D23" s="120"/>
+      <c r="E23" s="120"/>
       <c r="F23" s="42">
         <v>13</v>
       </c>
@@ -2851,11 +3071,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C24" s="110" t="s">
+      <c r="C24" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="131"/>
-      <c r="E24" s="131"/>
+      <c r="D24" s="120"/>
+      <c r="E24" s="120"/>
       <c r="F24" s="42">
         <v>25</v>
       </c>
@@ -2904,11 +3124,11 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C25" s="110" t="s">
+      <c r="C25" s="126" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="131"/>
-      <c r="E25" s="131"/>
+      <c r="D25" s="120"/>
+      <c r="E25" s="120"/>
       <c r="F25" s="42">
         <v>20</v>
       </c>
@@ -2957,11 +3177,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C26" s="110" t="s">
+      <c r="C26" s="126" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="131"/>
-      <c r="E26" s="131"/>
+      <c r="D26" s="120"/>
+      <c r="E26" s="120"/>
       <c r="F26" s="42">
         <v>16</v>
       </c>
@@ -3010,11 +3230,11 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C27" s="110" t="s">
+      <c r="C27" s="126" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="131"/>
-      <c r="E27" s="131"/>
+      <c r="D27" s="120"/>
+      <c r="E27" s="120"/>
       <c r="F27" s="42">
         <v>30</v>
       </c>
@@ -3063,11 +3283,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C28" s="110" t="s">
+      <c r="C28" s="126" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="111"/>
-      <c r="E28" s="112"/>
+      <c r="D28" s="127"/>
+      <c r="E28" s="128"/>
       <c r="F28" s="42">
         <v>18</v>
       </c>
@@ -3094,7 +3314,7 @@
         <v>21</v>
       </c>
       <c r="N28" s="39">
-        <f t="shared" ref="N28:N38" si="4">IFERROR(IF(OR(J28="",ISBLANK(L28)),"",J28+L28),"Error")</f>
+        <f t="shared" ref="N28:N41" si="4">IFERROR(IF(OR(J28="",ISBLANK(L28)),"",J28+L28),"Error")</f>
         <v>1.3194444444444519E-2</v>
       </c>
       <c r="O28" s="71"/>
@@ -3116,11 +3336,11 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C29" s="110" t="s">
+      <c r="C29" s="126" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="131"/>
-      <c r="E29" s="131"/>
+      <c r="D29" s="120"/>
+      <c r="E29" s="120"/>
       <c r="F29" s="42">
         <v>30</v>
       </c>
@@ -3169,11 +3389,11 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C30" s="110" t="s">
+      <c r="C30" s="126" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="131"/>
-      <c r="E30" s="131"/>
+      <c r="D30" s="120"/>
+      <c r="E30" s="120"/>
       <c r="F30" s="42">
         <v>15</v>
       </c>
@@ -3187,7 +3407,7 @@
         <v>0.99791666666666667</v>
       </c>
       <c r="J30" s="35">
-        <f t="shared" ref="J30:J38" si="5">IFERROR(IF(OR(ISBLANK(H30),ISBLANK(I30)),"",IF(I30&gt;=H30,I30-H30,"Error")),"Error")</f>
+        <f t="shared" ref="J30:J41" si="5">IFERROR(IF(OR(ISBLANK(H30),ISBLANK(I30)),"",IF(I30&gt;=H30,I30-H30,"Error")),"Error")</f>
         <v>4.1666666666666519E-3</v>
       </c>
       <c r="K30" s="46">
@@ -3222,11 +3442,11 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C31" s="110" t="s">
+      <c r="C31" s="126" t="s">
         <v>48</v>
       </c>
-      <c r="D31" s="111"/>
-      <c r="E31" s="112"/>
+      <c r="D31" s="127"/>
+      <c r="E31" s="128"/>
       <c r="F31" s="87">
         <v>17</v>
       </c>
@@ -3273,11 +3493,11 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C32" s="113" t="s">
+      <c r="C32" s="135" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="114"/>
-      <c r="E32" s="114"/>
+      <c r="D32" s="136"/>
+      <c r="E32" s="136"/>
       <c r="F32" s="98">
         <v>20</v>
       </c>
@@ -3324,11 +3544,11 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C33" s="113" t="s">
+      <c r="C33" s="135" t="s">
         <v>50</v>
       </c>
-      <c r="D33" s="114"/>
-      <c r="E33" s="114"/>
+      <c r="D33" s="136"/>
+      <c r="E33" s="136"/>
       <c r="F33" s="98">
         <v>18</v>
       </c>
@@ -3375,11 +3595,11 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C34" s="113" t="s">
+      <c r="C34" s="135" t="s">
         <v>51</v>
       </c>
-      <c r="D34" s="114"/>
-      <c r="E34" s="114"/>
+      <c r="D34" s="136"/>
+      <c r="E34" s="136"/>
       <c r="F34" s="98">
         <v>20</v>
       </c>
@@ -3420,17 +3640,17 @@
       <c r="Y34" s="108"/>
       <c r="Z34" s="108"/>
     </row>
-    <row r="35" spans="1:26" ht="15" customHeight="1">
+    <row r="35" spans="1:26" ht="15" customHeight="1" thickBot="1">
       <c r="A35" s="86"/>
       <c r="B35" s="30">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C35" s="110" t="s">
+      <c r="C35" s="126" t="s">
         <v>52</v>
       </c>
-      <c r="D35" s="131"/>
-      <c r="E35" s="131"/>
+      <c r="D35" s="120"/>
+      <c r="E35" s="120"/>
       <c r="F35" s="42">
         <v>25</v>
       </c>
@@ -3473,30 +3693,36 @@
       <c r="Y35" s="22"/>
       <c r="Z35" s="22"/>
     </row>
-    <row r="36" spans="1:26" ht="15" customHeight="1">
+    <row r="36" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A36" s="86"/>
       <c r="B36" s="30">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C36" s="110"/>
-      <c r="D36" s="131"/>
-      <c r="E36" s="131"/>
-      <c r="F36" s="42"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="44"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="35" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="K36" s="46"/>
-      <c r="L36" s="47"/>
-      <c r="M36" s="48"/>
-      <c r="N36" s="39" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="C36" s="156" t="s">
+        <v>53</v>
+      </c>
+      <c r="D36" s="157"/>
+      <c r="E36" s="158"/>
+      <c r="F36" s="159">
+        <v>20</v>
+      </c>
+      <c r="G36" s="160">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H36" s="161">
+        <v>0.87361111111111101</v>
+      </c>
+      <c r="I36" s="161">
+        <v>0.89861111111111114</v>
+      </c>
+      <c r="J36" s="162">
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="K36" s="163"/>
+      <c r="L36" s="164"/>
+      <c r="M36" s="163"/>
+      <c r="N36" s="165"/>
       <c r="O36" s="86"/>
       <c r="P36" s="21"/>
       <c r="Q36" s="22"/>
@@ -3510,29 +3736,43 @@
       <c r="Y36" s="22"/>
       <c r="Z36" s="22"/>
     </row>
-    <row r="37" spans="1:26" ht="15" customHeight="1">
+    <row r="37" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A37" s="86"/>
       <c r="B37" s="30">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C37" s="110"/>
-      <c r="D37" s="131"/>
-      <c r="E37" s="131"/>
-      <c r="F37" s="42"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="44"/>
-      <c r="I37" s="45"/>
-      <c r="J37" s="35" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="K37" s="46"/>
-      <c r="L37" s="47"/>
-      <c r="M37" s="48"/>
-      <c r="N37" s="39" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+      <c r="C37" s="156" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" s="157"/>
+      <c r="E37" s="158"/>
+      <c r="F37" s="159">
+        <v>20</v>
+      </c>
+      <c r="G37" s="160">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="H37" s="161">
+        <v>4.0972222222222222E-2</v>
+      </c>
+      <c r="I37" s="161">
+        <v>5.486111111111111E-2</v>
+      </c>
+      <c r="J37" s="162">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="K37" s="159">
+        <v>2</v>
+      </c>
+      <c r="L37" s="160">
+        <v>9.7222222222222224E-3</v>
+      </c>
+      <c r="M37" s="159">
+        <v>15</v>
+      </c>
+      <c r="N37" s="166">
+        <v>2.361111111111111E-2</v>
       </c>
       <c r="O37" s="86"/>
       <c r="P37" s="21"/>
@@ -3547,31 +3787,45 @@
       <c r="Y37" s="22"/>
       <c r="Z37" s="22"/>
     </row>
-    <row r="38" spans="1:26" ht="15" customHeight="1">
-      <c r="A38" s="71"/>
+    <row r="38" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A38" s="110"/>
       <c r="B38" s="30">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C38" s="110"/>
-      <c r="D38" s="111"/>
-      <c r="E38" s="112"/>
-      <c r="F38" s="42"/>
-      <c r="G38" s="43"/>
-      <c r="H38" s="44"/>
-      <c r="I38" s="45"/>
-      <c r="J38" s="35" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="K38" s="46"/>
-      <c r="L38" s="47"/>
-      <c r="M38" s="48"/>
-      <c r="N38" s="39" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O38" s="71"/>
+      <c r="C38" s="156" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="157"/>
+      <c r="E38" s="158"/>
+      <c r="F38" s="159">
+        <v>25</v>
+      </c>
+      <c r="G38" s="160">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H38" s="161">
+        <v>5.6944444444444443E-2</v>
+      </c>
+      <c r="I38" s="161">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="J38" s="162">
+        <v>1.9444444444444445E-2</v>
+      </c>
+      <c r="K38" s="159">
+        <v>2</v>
+      </c>
+      <c r="L38" s="160">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="M38" s="159">
+        <v>16</v>
+      </c>
+      <c r="N38" s="166">
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O38" s="110"/>
       <c r="P38" s="21"/>
       <c r="Q38" s="22"/>
       <c r="R38" s="22"/>
@@ -3584,330 +3838,350 @@
       <c r="Y38" s="22"/>
       <c r="Z38" s="22"/>
     </row>
-    <row r="39" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A39" s="7"/>
-      <c r="B39" s="118" t="s">
+    <row r="39" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A39" s="110"/>
+      <c r="B39" s="30">
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="C39" s="119"/>
-      <c r="D39" s="119"/>
-      <c r="E39" s="119"/>
-      <c r="F39" s="49">
-        <f>IF(SUM(F18:F38)=0,"Completar",SUM(F18:F38))</f>
-        <v>357</v>
-      </c>
-      <c r="G39" s="50">
-        <f>IF(SUM(G18:G38)=0,"Completar",SUM(G18:G38))</f>
-        <v>0.27152777777777776</v>
-      </c>
-      <c r="H39" s="51" t="s">
+      <c r="C39" s="156" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" s="157"/>
+      <c r="E39" s="158"/>
+      <c r="F39" s="159">
+        <v>25</v>
+      </c>
+      <c r="G39" s="160">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H39" s="161">
+        <v>0.37013888888888885</v>
+      </c>
+      <c r="I39" s="161">
+        <v>0.39166666666666666</v>
+      </c>
+      <c r="J39" s="162">
+        <v>2.1527777777777781E-2</v>
+      </c>
+      <c r="K39" s="159">
+        <v>3</v>
+      </c>
+      <c r="L39" s="160">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="M39" s="159">
+        <v>62</v>
+      </c>
+      <c r="N39" s="166">
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="O39" s="110"/>
+      <c r="P39" s="21"/>
+      <c r="Q39" s="22"/>
+      <c r="R39" s="22"/>
+      <c r="S39" s="22"/>
+      <c r="T39" s="22"/>
+      <c r="U39" s="22"/>
+      <c r="V39" s="22"/>
+      <c r="W39" s="22"/>
+      <c r="X39" s="22"/>
+      <c r="Y39" s="22"/>
+      <c r="Z39" s="22"/>
+    </row>
+    <row r="40" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A40" s="110"/>
+      <c r="B40" s="30">
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="I39" s="52" t="s">
+      <c r="C40" s="149"/>
+      <c r="D40" s="149"/>
+      <c r="E40" s="150"/>
+      <c r="F40" s="151"/>
+      <c r="G40" s="152"/>
+      <c r="H40" s="153"/>
+      <c r="I40" s="153"/>
+      <c r="J40" s="154"/>
+      <c r="K40" s="151"/>
+      <c r="L40" s="152"/>
+      <c r="M40" s="155"/>
+      <c r="N40" s="154"/>
+      <c r="O40" s="110"/>
+      <c r="P40" s="21"/>
+      <c r="Q40" s="22"/>
+      <c r="R40" s="22"/>
+      <c r="S40" s="22"/>
+      <c r="T40" s="22"/>
+      <c r="U40" s="22"/>
+      <c r="V40" s="22"/>
+      <c r="W40" s="22"/>
+      <c r="X40" s="22"/>
+      <c r="Y40" s="22"/>
+      <c r="Z40" s="22"/>
+    </row>
+    <row r="41" spans="1:26" ht="15" customHeight="1">
+      <c r="A41" s="71"/>
+      <c r="B41" s="30">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C41" s="126"/>
+      <c r="D41" s="127"/>
+      <c r="E41" s="128"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="44"/>
+      <c r="I41" s="45"/>
+      <c r="J41" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="K41" s="46"/>
+      <c r="L41" s="47"/>
+      <c r="M41" s="48"/>
+      <c r="N41" s="39" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="O41" s="71"/>
+      <c r="P41" s="21"/>
+      <c r="Q41" s="22"/>
+      <c r="R41" s="22"/>
+      <c r="S41" s="22"/>
+      <c r="T41" s="22"/>
+      <c r="U41" s="22"/>
+      <c r="V41" s="22"/>
+      <c r="W41" s="22"/>
+      <c r="X41" s="22"/>
+      <c r="Y41" s="22"/>
+      <c r="Z41" s="22"/>
+    </row>
+    <row r="42" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A42" s="7"/>
+      <c r="B42" s="148" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="125"/>
+      <c r="D42" s="125"/>
+      <c r="E42" s="125"/>
+      <c r="F42" s="49">
+        <f>IF(SUM(F18:F41)=0,"Completar",SUM(F18:F41))</f>
+        <v>447</v>
+      </c>
+      <c r="G42" s="50">
+        <f>IF(SUM(G18:G41)=0,"Completar",SUM(G18:G41))</f>
+        <v>0.35138888888888881</v>
+      </c>
+      <c r="H42" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="J39" s="53">
-        <f>IF(OR(COUNTIF(J18:J38,"Error")&gt;0,COUNTIF(J18:J38,"Completar")&gt;0),"Error",IF(SUM(J18:J38)=0,"Completar",SUM(J18:J38)))</f>
-        <v>0.27152777777777781</v>
-      </c>
-      <c r="K39" s="54">
-        <f>SUM(K18:K38)</f>
-        <v>16</v>
-      </c>
-      <c r="L39" s="50">
-        <f>SUM(L18:L38)</f>
-        <v>4.4444444444444439E-2</v>
-      </c>
-      <c r="M39" s="55">
-        <f>IF(SUM(M18:M38)=0,"Completar",SUM(M18:M38))</f>
-        <v>308</v>
-      </c>
-      <c r="N39" s="18">
-        <f>IF(OR(COUNTIF(N18:N38,"Error")&gt;0,COUNTIF(N18:N38,"Completar")&gt;0),"Error",IF(SUM(N18:N38)=0,"Completar",SUM(N18:N38)))</f>
-        <v>0.31597222222222227</v>
-      </c>
-      <c r="O39" s="7"/>
-      <c r="P39" s="56"/>
-      <c r="Q39" s="57"/>
-      <c r="R39" s="57"/>
-      <c r="S39" s="57"/>
-      <c r="T39" s="57"/>
-      <c r="U39" s="57"/>
-      <c r="V39" s="57"/>
-      <c r="W39" s="57"/>
-      <c r="X39" s="57"/>
-      <c r="Y39" s="57"/>
-      <c r="Z39" s="57"/>
-    </row>
-    <row r="40" spans="1:26" ht="6" customHeight="1">
-      <c r="A40" s="20"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
-      <c r="L40" s="20"/>
-      <c r="M40" s="20"/>
-      <c r="N40" s="20"/>
-      <c r="O40" s="20"/>
-      <c r="P40" s="23"/>
-      <c r="Q40" s="23"/>
-      <c r="R40" s="23"/>
-      <c r="S40" s="23"/>
-      <c r="T40" s="23"/>
-      <c r="U40" s="23"/>
-      <c r="V40" s="23"/>
-      <c r="W40" s="23"/>
-      <c r="X40" s="23"/>
-      <c r="Y40" s="23"/>
-      <c r="Z40" s="23"/>
-    </row>
-    <row r="41" spans="1:26" ht="15" customHeight="1">
-      <c r="A41" s="4"/>
-      <c r="B41" s="115" t="s">
+      <c r="I42" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="J42" s="53">
+        <f>IF(OR(COUNTIF(J18:J41,"Error")&gt;0,COUNTIF(J18:J41,"Completar")&gt;0),"Error",IF(SUM(J18:J41)=0,"Completar",SUM(J18:J41)))</f>
+        <v>0.35138888888888892</v>
+      </c>
+      <c r="K42" s="54">
+        <f>SUM(K18:K41)</f>
+        <v>23</v>
+      </c>
+      <c r="L42" s="50">
+        <f>SUM(L18:L41)</f>
+        <v>7.1527777777777773E-2</v>
+      </c>
+      <c r="M42" s="55">
+        <f>IF(SUM(M18:M41)=0,"Completar",SUM(M18:M41))</f>
+        <v>411</v>
+      </c>
+      <c r="N42" s="18">
+        <f>IF(OR(COUNTIF(N18:N41,"Error")&gt;0,COUNTIF(N18:N41,"Completar")&gt;0),"Error",IF(SUM(N18:N41)=0,"Completar",SUM(N18:N41)))</f>
+        <v>0.3979166666666667</v>
+      </c>
+      <c r="O42" s="7"/>
+      <c r="P42" s="56"/>
+      <c r="Q42" s="57"/>
+      <c r="R42" s="57"/>
+      <c r="S42" s="57"/>
+      <c r="T42" s="57"/>
+      <c r="U42" s="57"/>
+      <c r="V42" s="57"/>
+      <c r="W42" s="57"/>
+      <c r="X42" s="57"/>
+      <c r="Y42" s="57"/>
+      <c r="Z42" s="57"/>
+    </row>
+    <row r="43" spans="1:26" ht="6" customHeight="1">
+      <c r="A43" s="20"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="20"/>
+      <c r="L43" s="20"/>
+      <c r="M43" s="20"/>
+      <c r="N43" s="20"/>
+      <c r="O43" s="20"/>
+      <c r="P43" s="23"/>
+      <c r="Q43" s="23"/>
+      <c r="R43" s="23"/>
+      <c r="S43" s="23"/>
+      <c r="T43" s="23"/>
+      <c r="U43" s="23"/>
+      <c r="V43" s="23"/>
+      <c r="W43" s="23"/>
+      <c r="X43" s="23"/>
+      <c r="Y43" s="23"/>
+      <c r="Z43" s="23"/>
+    </row>
+    <row r="44" spans="1:26" ht="15" customHeight="1">
+      <c r="A44" s="4"/>
+      <c r="B44" s="113" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="116"/>
-      <c r="D41" s="116"/>
-      <c r="E41" s="117"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="5"/>
-      <c r="L41" s="5"/>
-      <c r="M41" s="5"/>
-      <c r="N41" s="5"/>
-      <c r="O41" s="4"/>
-      <c r="P41" s="6"/>
-      <c r="Q41" s="6"/>
-      <c r="R41" s="6"/>
-      <c r="S41" s="6"/>
-      <c r="T41" s="6"/>
-      <c r="U41" s="6"/>
-      <c r="V41" s="6"/>
-      <c r="W41" s="6"/>
-      <c r="X41" s="6"/>
-      <c r="Y41" s="6"/>
-      <c r="Z41" s="6"/>
-    </row>
-    <row r="42" spans="1:26" ht="30" customHeight="1">
-      <c r="A42" s="7"/>
-      <c r="B42" s="8" t="s">
+      <c r="C44" s="114"/>
+      <c r="D44" s="114"/>
+      <c r="E44" s="115"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5"/>
+      <c r="N44" s="5"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="6"/>
+      <c r="Q44" s="6"/>
+      <c r="R44" s="6"/>
+      <c r="S44" s="6"/>
+      <c r="T44" s="6"/>
+      <c r="U44" s="6"/>
+      <c r="V44" s="6"/>
+      <c r="W44" s="6"/>
+      <c r="X44" s="6"/>
+      <c r="Y44" s="6"/>
+      <c r="Z44" s="6"/>
+    </row>
+    <row r="45" spans="1:26" ht="30" customHeight="1">
+      <c r="A45" s="7"/>
+      <c r="B45" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C45" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D42" s="9" t="s">
+      <c r="D45" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E42" s="10" t="s">
+      <c r="E45" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="7"/>
-      <c r="M42" s="7"/>
-      <c r="N42" s="7"/>
-      <c r="O42" s="7"/>
-      <c r="P42" s="13"/>
-      <c r="Q42" s="14"/>
-      <c r="R42" s="14"/>
-      <c r="S42" s="14"/>
-      <c r="T42" s="14"/>
-      <c r="U42" s="14"/>
-      <c r="V42" s="14"/>
-      <c r="W42" s="14"/>
-      <c r="X42" s="14"/>
-      <c r="Y42" s="14"/>
-      <c r="Z42" s="14"/>
-    </row>
-    <row r="43" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A43" s="15"/>
-      <c r="B43" s="58"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="18" t="str">
-        <f>IFERROR(IF(OR(ISBLANK(C43),ISBLANK(D43)),"Completar",IF(D43&gt;=C43,D43-C43,"Error")),"Error")</f>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="7"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="7"/>
+      <c r="P45" s="13"/>
+      <c r="Q45" s="14"/>
+      <c r="R45" s="14"/>
+      <c r="S45" s="14"/>
+      <c r="T45" s="14"/>
+      <c r="U45" s="14"/>
+      <c r="V45" s="14"/>
+      <c r="W45" s="14"/>
+      <c r="X45" s="14"/>
+      <c r="Y45" s="14"/>
+      <c r="Z45" s="14"/>
+    </row>
+    <row r="46" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A46" s="15"/>
+      <c r="B46" s="58"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="18" t="str">
+        <f>IFERROR(IF(OR(ISBLANK(C46),ISBLANK(D46)),"Completar",IF(D46&gt;=C46,D46-C46,"Error")),"Error")</f>
         <v>Completar</v>
       </c>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
-      <c r="H43" s="15"/>
-      <c r="I43" s="15"/>
-      <c r="J43" s="15"/>
-      <c r="K43" s="15"/>
-      <c r="L43" s="15"/>
-      <c r="M43" s="15"/>
-      <c r="N43" s="15"/>
-      <c r="O43" s="15"/>
-      <c r="P43" s="21"/>
-      <c r="Q43" s="22"/>
-      <c r="R43" s="22"/>
-      <c r="S43" s="22"/>
-      <c r="T43" s="22"/>
-      <c r="U43" s="22"/>
-      <c r="V43" s="22"/>
-      <c r="W43" s="22"/>
-      <c r="X43" s="22"/>
-      <c r="Y43" s="22"/>
-      <c r="Z43" s="22"/>
-    </row>
-    <row r="44" spans="1:26" ht="6" customHeight="1">
-      <c r="A44" s="20"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
-      <c r="K44" s="20"/>
-      <c r="L44" s="20"/>
-      <c r="M44" s="20"/>
-      <c r="N44" s="20"/>
-      <c r="O44" s="20"/>
-      <c r="P44" s="23"/>
-      <c r="Q44" s="23"/>
-      <c r="R44" s="23"/>
-      <c r="S44" s="23"/>
-      <c r="T44" s="23"/>
-      <c r="U44" s="23"/>
-      <c r="V44" s="23"/>
-      <c r="W44" s="23"/>
-      <c r="X44" s="23"/>
-      <c r="Y44" s="23"/>
-      <c r="Z44" s="23"/>
-    </row>
-    <row r="45" spans="1:26">
-      <c r="A45" s="20"/>
-      <c r="B45" s="115" t="s">
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="15"/>
+      <c r="K46" s="15"/>
+      <c r="L46" s="15"/>
+      <c r="M46" s="15"/>
+      <c r="N46" s="15"/>
+      <c r="O46" s="15"/>
+      <c r="P46" s="21"/>
+      <c r="Q46" s="22"/>
+      <c r="R46" s="22"/>
+      <c r="S46" s="22"/>
+      <c r="T46" s="22"/>
+      <c r="U46" s="22"/>
+      <c r="V46" s="22"/>
+      <c r="W46" s="22"/>
+      <c r="X46" s="22"/>
+      <c r="Y46" s="22"/>
+      <c r="Z46" s="22"/>
+    </row>
+    <row r="47" spans="1:26" ht="6" customHeight="1">
+      <c r="A47" s="20"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="20"/>
+      <c r="I47" s="20"/>
+      <c r="J47" s="20"/>
+      <c r="K47" s="20"/>
+      <c r="L47" s="20"/>
+      <c r="M47" s="20"/>
+      <c r="N47" s="20"/>
+      <c r="O47" s="20"/>
+      <c r="P47" s="23"/>
+      <c r="Q47" s="23"/>
+      <c r="R47" s="23"/>
+      <c r="S47" s="23"/>
+      <c r="T47" s="23"/>
+      <c r="U47" s="23"/>
+      <c r="V47" s="23"/>
+      <c r="W47" s="23"/>
+      <c r="X47" s="23"/>
+      <c r="Y47" s="23"/>
+      <c r="Z47" s="23"/>
+    </row>
+    <row r="48" spans="1:26">
+      <c r="A48" s="20"/>
+      <c r="B48" s="113" t="s">
         <v>26</v>
       </c>
-      <c r="C45" s="116"/>
-      <c r="D45" s="116"/>
-      <c r="E45" s="116"/>
-      <c r="F45" s="116"/>
-      <c r="G45" s="116"/>
-      <c r="H45" s="116"/>
-      <c r="I45" s="116"/>
-      <c r="J45" s="116"/>
-      <c r="K45" s="116"/>
-      <c r="L45" s="116"/>
-      <c r="M45" s="116"/>
-      <c r="N45" s="117"/>
-      <c r="O45" s="20"/>
-      <c r="P45" s="59"/>
-      <c r="Q45" s="59"/>
-      <c r="R45" s="59"/>
-      <c r="S45" s="59"/>
-      <c r="T45" s="59"/>
-      <c r="U45" s="59"/>
-      <c r="V45" s="59"/>
-      <c r="W45" s="59"/>
-      <c r="X45" s="59"/>
-      <c r="Y45" s="59"/>
-      <c r="Z45" s="59"/>
-    </row>
-    <row r="46" spans="1:26" ht="15" customHeight="1">
-      <c r="A46" s="20"/>
-      <c r="B46" s="135" t="s">
-        <v>27</v>
-      </c>
-      <c r="C46" s="131"/>
-      <c r="D46" s="136"/>
-      <c r="E46" s="137">
-        <f>M39</f>
-        <v>308</v>
-      </c>
-      <c r="F46" s="136"/>
-      <c r="G46" s="60"/>
-      <c r="H46" s="61"/>
-      <c r="I46" s="61"/>
-      <c r="J46" s="61"/>
-      <c r="K46" s="61"/>
-      <c r="L46" s="61"/>
-      <c r="M46" s="61"/>
-      <c r="N46" s="62"/>
-      <c r="O46" s="20"/>
-      <c r="P46" s="59"/>
-      <c r="Q46" s="59"/>
-      <c r="R46" s="59"/>
-      <c r="S46" s="59"/>
-      <c r="T46" s="59"/>
-      <c r="U46" s="59"/>
-      <c r="V46" s="59"/>
-      <c r="W46" s="59"/>
-      <c r="X46" s="59"/>
-      <c r="Y46" s="59"/>
-      <c r="Z46" s="59"/>
-    </row>
-    <row r="47" spans="1:26">
-      <c r="A47" s="20"/>
-      <c r="B47" s="135" t="s">
-        <v>28</v>
-      </c>
-      <c r="C47" s="131"/>
-      <c r="D47" s="136"/>
-      <c r="E47" s="145">
-        <f>IF(M39="Completar","Completar",IFERROR(M39/(N39*24),"Error"))</f>
-        <v>40.615384615384613</v>
-      </c>
-      <c r="F47" s="136"/>
-      <c r="G47" s="63"/>
-      <c r="H47" s="64"/>
-      <c r="I47" s="64"/>
-      <c r="J47" s="64"/>
-      <c r="K47" s="64"/>
-      <c r="L47" s="64"/>
-      <c r="M47" s="64"/>
-      <c r="N47" s="65"/>
-      <c r="O47" s="20"/>
-      <c r="P47" s="59"/>
-      <c r="Q47" s="59"/>
-      <c r="R47" s="59"/>
-      <c r="S47" s="59"/>
-      <c r="T47" s="59"/>
-      <c r="U47" s="59"/>
-      <c r="V47" s="59"/>
-      <c r="W47" s="59"/>
-      <c r="X47" s="59"/>
-      <c r="Y47" s="59"/>
-      <c r="Z47" s="59"/>
-    </row>
-    <row r="48" spans="1:26" ht="15" customHeight="1">
-      <c r="A48" s="20"/>
-      <c r="B48" s="135" t="s">
-        <v>29</v>
-      </c>
-      <c r="C48" s="131"/>
-      <c r="D48" s="136"/>
-      <c r="E48" s="137">
-        <f>IF(K39=0,0,IFERROR(ROUNDUP(K39/(M39/100),0),"Error"))</f>
-        <v>6</v>
-      </c>
-      <c r="F48" s="136"/>
-      <c r="G48" s="63"/>
-      <c r="H48" s="64"/>
-      <c r="I48" s="64"/>
-      <c r="J48" s="64"/>
-      <c r="K48" s="64"/>
-      <c r="L48" s="64"/>
-      <c r="M48" s="64"/>
-      <c r="N48" s="65"/>
+      <c r="C48" s="114"/>
+      <c r="D48" s="114"/>
+      <c r="E48" s="114"/>
+      <c r="F48" s="114"/>
+      <c r="G48" s="114"/>
+      <c r="H48" s="114"/>
+      <c r="I48" s="114"/>
+      <c r="J48" s="114"/>
+      <c r="K48" s="114"/>
+      <c r="L48" s="114"/>
+      <c r="M48" s="114"/>
+      <c r="N48" s="115"/>
       <c r="O48" s="20"/>
       <c r="P48" s="59"/>
       <c r="Q48" s="59"/>
@@ -3923,24 +4197,24 @@
     </row>
     <row r="49" spans="1:26" ht="15" customHeight="1">
       <c r="A49" s="20"/>
-      <c r="B49" s="135" t="s">
-        <v>30</v>
-      </c>
-      <c r="C49" s="131"/>
-      <c r="D49" s="136"/>
-      <c r="E49" s="144">
-        <f>IF(K39=0,0,IFERROR(K39/M39,"Error"))</f>
-        <v>5.1948051948051951E-2</v>
-      </c>
-      <c r="F49" s="136"/>
-      <c r="G49" s="63"/>
-      <c r="H49" s="64"/>
-      <c r="I49" s="64"/>
-      <c r="J49" s="64"/>
-      <c r="K49" s="64"/>
-      <c r="L49" s="64"/>
-      <c r="M49" s="64"/>
-      <c r="N49" s="65"/>
+      <c r="B49" s="119" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" s="120"/>
+      <c r="D49" s="121"/>
+      <c r="E49" s="131">
+        <f>M42</f>
+        <v>411</v>
+      </c>
+      <c r="F49" s="121"/>
+      <c r="G49" s="60"/>
+      <c r="H49" s="61"/>
+      <c r="I49" s="61"/>
+      <c r="J49" s="61"/>
+      <c r="K49" s="61"/>
+      <c r="L49" s="61"/>
+      <c r="M49" s="61"/>
+      <c r="N49" s="62"/>
       <c r="O49" s="20"/>
       <c r="P49" s="59"/>
       <c r="Q49" s="59"/>
@@ -3954,21 +4228,18 @@
       <c r="Y49" s="59"/>
       <c r="Z49" s="59"/>
     </row>
-    <row r="50" spans="1:26" ht="15" customHeight="1">
+    <row r="50" spans="1:26">
       <c r="A50" s="20"/>
-      <c r="B50" s="135" t="s">
-        <v>31</v>
-      </c>
-      <c r="C50" s="131"/>
-      <c r="D50" s="136"/>
-      <c r="E50" s="66">
-        <f>E5</f>
-        <v>6.9444444444444198E-3</v>
-      </c>
-      <c r="F50" s="67">
-        <f t="shared" ref="F50:F53" si="6">IF(E50="Completar",E50,IFERROR(E50/$E$56,"Error"))</f>
-        <v>2.1505376344085943E-2</v>
-      </c>
+      <c r="B50" s="119" t="s">
+        <v>28</v>
+      </c>
+      <c r="C50" s="120"/>
+      <c r="D50" s="121"/>
+      <c r="E50" s="130">
+        <f>IF(M42="Completar","Completar",IFERROR(M42/(N42*24),"Error"))</f>
+        <v>43.036649214659683</v>
+      </c>
+      <c r="F50" s="121"/>
       <c r="G50" s="63"/>
       <c r="H50" s="64"/>
       <c r="I50" s="64"/>
@@ -3992,19 +4263,16 @@
     </row>
     <row r="51" spans="1:26" ht="15" customHeight="1">
       <c r="A51" s="20"/>
-      <c r="B51" s="135" t="s">
-        <v>32</v>
-      </c>
-      <c r="C51" s="131"/>
-      <c r="D51" s="136"/>
-      <c r="E51" s="66" t="str">
-        <f>E9</f>
-        <v>Completar</v>
-      </c>
-      <c r="F51" s="67" t="str">
-        <f t="shared" si="6"/>
-        <v>Completar</v>
-      </c>
+      <c r="B51" s="119" t="s">
+        <v>29</v>
+      </c>
+      <c r="C51" s="120"/>
+      <c r="D51" s="121"/>
+      <c r="E51" s="131">
+        <f>IF(K42=0,0,IFERROR(ROUNDUP(K42/(M42/100),0),"Error"))</f>
+        <v>6</v>
+      </c>
+      <c r="F51" s="121"/>
       <c r="G51" s="63"/>
       <c r="H51" s="64"/>
       <c r="I51" s="64"/>
@@ -4028,19 +4296,16 @@
     </row>
     <row r="52" spans="1:26" ht="15" customHeight="1">
       <c r="A52" s="20"/>
-      <c r="B52" s="135" t="s">
-        <v>33</v>
-      </c>
-      <c r="C52" s="131"/>
-      <c r="D52" s="136"/>
-      <c r="E52" s="66" t="str">
-        <f>E13</f>
-        <v>Completar</v>
-      </c>
-      <c r="F52" s="67" t="str">
-        <f t="shared" si="6"/>
-        <v>Completar</v>
-      </c>
+      <c r="B52" s="119" t="s">
+        <v>30</v>
+      </c>
+      <c r="C52" s="120"/>
+      <c r="D52" s="121"/>
+      <c r="E52" s="129">
+        <f>IF(K42=0,0,IFERROR(K42/M42,"Error"))</f>
+        <v>5.5961070559610707E-2</v>
+      </c>
+      <c r="F52" s="121"/>
       <c r="G52" s="63"/>
       <c r="H52" s="64"/>
       <c r="I52" s="64"/>
@@ -4064,18 +4329,18 @@
     </row>
     <row r="53" spans="1:26" ht="15" customHeight="1">
       <c r="A53" s="20"/>
-      <c r="B53" s="135" t="s">
-        <v>34</v>
-      </c>
-      <c r="C53" s="131"/>
-      <c r="D53" s="136"/>
-      <c r="E53" s="66" t="str">
-        <f>E43</f>
-        <v>Completar</v>
-      </c>
-      <c r="F53" s="67" t="str">
-        <f t="shared" si="6"/>
-        <v>Completar</v>
+      <c r="B53" s="119" t="s">
+        <v>31</v>
+      </c>
+      <c r="C53" s="120"/>
+      <c r="D53" s="121"/>
+      <c r="E53" s="66">
+        <f>E5</f>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="F53" s="67">
+        <f t="shared" ref="F53:F56" si="6">IF(E53="Completar",E53,IFERROR(E53/$E$59,"Error"))</f>
+        <v>1.6155088852988633E-2</v>
       </c>
       <c r="G53" s="63"/>
       <c r="H53" s="64"/>
@@ -4100,18 +4365,18 @@
     </row>
     <row r="54" spans="1:26" ht="15" customHeight="1">
       <c r="A54" s="20"/>
-      <c r="B54" s="135" t="s">
-        <v>35</v>
-      </c>
-      <c r="C54" s="131"/>
-      <c r="D54" s="136"/>
-      <c r="E54" s="66">
-        <f>L39</f>
-        <v>4.4444444444444439E-2</v>
-      </c>
-      <c r="F54" s="67">
-        <f t="shared" ref="F54:F55" si="7">IF(E54="Completar",E54,IFERROR(E54/$E$56,"Completar"))</f>
-        <v>0.13763440860215051</v>
+      <c r="B54" s="119" t="s">
+        <v>32</v>
+      </c>
+      <c r="C54" s="120"/>
+      <c r="D54" s="121"/>
+      <c r="E54" s="66" t="str">
+        <f>E9</f>
+        <v>Completar</v>
+      </c>
+      <c r="F54" s="67" t="str">
+        <f t="shared" si="6"/>
+        <v>Completar</v>
       </c>
       <c r="G54" s="63"/>
       <c r="H54" s="64"/>
@@ -4136,18 +4401,18 @@
     </row>
     <row r="55" spans="1:26" ht="15" customHeight="1">
       <c r="A55" s="20"/>
-      <c r="B55" s="135" t="s">
-        <v>36</v>
-      </c>
-      <c r="C55" s="131"/>
-      <c r="D55" s="136"/>
-      <c r="E55" s="66">
-        <f>J39</f>
-        <v>0.27152777777777781</v>
-      </c>
-      <c r="F55" s="67">
-        <f t="shared" si="7"/>
-        <v>0.84086021505376352</v>
+      <c r="B55" s="119" t="s">
+        <v>33</v>
+      </c>
+      <c r="C55" s="120"/>
+      <c r="D55" s="121"/>
+      <c r="E55" s="66" t="str">
+        <f>E13</f>
+        <v>Completar</v>
+      </c>
+      <c r="F55" s="67" t="str">
+        <f t="shared" si="6"/>
+        <v>Completar</v>
       </c>
       <c r="G55" s="63"/>
       <c r="H55" s="64"/>
@@ -4172,24 +4437,27 @@
     </row>
     <row r="56" spans="1:26" ht="15" customHeight="1">
       <c r="A56" s="20"/>
-      <c r="B56" s="143" t="s">
-        <v>37</v>
-      </c>
-      <c r="C56" s="119"/>
-      <c r="D56" s="142"/>
-      <c r="E56" s="141">
-        <f>IF(COUNTIF(E50:E55,"Error")&gt;0,"Error",IF(SUM(E50:E55)=0,"Completar",SUM(E50:E55)))</f>
-        <v>0.32291666666666669</v>
-      </c>
-      <c r="F56" s="142"/>
-      <c r="G56" s="68"/>
-      <c r="H56" s="69"/>
-      <c r="I56" s="69"/>
-      <c r="J56" s="69"/>
-      <c r="K56" s="69"/>
-      <c r="L56" s="69"/>
-      <c r="M56" s="69"/>
-      <c r="N56" s="70"/>
+      <c r="B56" s="119" t="s">
+        <v>34</v>
+      </c>
+      <c r="C56" s="120"/>
+      <c r="D56" s="121"/>
+      <c r="E56" s="66" t="str">
+        <f>E46</f>
+        <v>Completar</v>
+      </c>
+      <c r="F56" s="67" t="str">
+        <f t="shared" si="6"/>
+        <v>Completar</v>
+      </c>
+      <c r="G56" s="63"/>
+      <c r="H56" s="64"/>
+      <c r="I56" s="64"/>
+      <c r="J56" s="64"/>
+      <c r="K56" s="64"/>
+      <c r="L56" s="64"/>
+      <c r="M56" s="64"/>
+      <c r="N56" s="65"/>
       <c r="O56" s="20"/>
       <c r="P56" s="59"/>
       <c r="Q56" s="59"/>
@@ -4203,49 +4471,65 @@
       <c r="Y56" s="59"/>
       <c r="Z56" s="59"/>
     </row>
-    <row r="57" spans="1:26" ht="6" customHeight="1">
+    <row r="57" spans="1:26" ht="15" customHeight="1">
       <c r="A57" s="20"/>
-      <c r="B57" s="20"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="20"/>
-      <c r="F57" s="20"/>
-      <c r="G57" s="20"/>
-      <c r="H57" s="20"/>
-      <c r="I57" s="20"/>
-      <c r="J57" s="20"/>
-      <c r="K57" s="20"/>
-      <c r="L57" s="20"/>
-      <c r="M57" s="20"/>
-      <c r="N57" s="20"/>
+      <c r="B57" s="119" t="s">
+        <v>35</v>
+      </c>
+      <c r="C57" s="120"/>
+      <c r="D57" s="121"/>
+      <c r="E57" s="66">
+        <f>L42</f>
+        <v>7.1527777777777773E-2</v>
+      </c>
+      <c r="F57" s="67">
+        <f t="shared" ref="F57:F58" si="7">IF(E57="Completar",E57,IFERROR(E57/$E$59,"Completar"))</f>
+        <v>0.16639741518578349</v>
+      </c>
+      <c r="G57" s="63"/>
+      <c r="H57" s="64"/>
+      <c r="I57" s="64"/>
+      <c r="J57" s="64"/>
+      <c r="K57" s="64"/>
+      <c r="L57" s="64"/>
+      <c r="M57" s="64"/>
+      <c r="N57" s="65"/>
       <c r="O57" s="20"/>
-      <c r="P57" s="20"/>
-      <c r="Q57" s="20"/>
-      <c r="R57" s="20"/>
-      <c r="S57" s="20"/>
-      <c r="T57" s="20"/>
-      <c r="U57" s="20"/>
-      <c r="V57" s="20"/>
-      <c r="W57" s="20"/>
-      <c r="X57" s="20"/>
-      <c r="Y57" s="20"/>
-      <c r="Z57" s="20"/>
-    </row>
-    <row r="58" spans="1:26" hidden="1">
+      <c r="P57" s="59"/>
+      <c r="Q57" s="59"/>
+      <c r="R57" s="59"/>
+      <c r="S57" s="59"/>
+      <c r="T57" s="59"/>
+      <c r="U57" s="59"/>
+      <c r="V57" s="59"/>
+      <c r="W57" s="59"/>
+      <c r="X57" s="59"/>
+      <c r="Y57" s="59"/>
+      <c r="Z57" s="59"/>
+    </row>
+    <row r="58" spans="1:26" ht="15" customHeight="1">
       <c r="A58" s="20"/>
-      <c r="B58" s="59"/>
-      <c r="C58" s="59"/>
-      <c r="D58" s="59"/>
-      <c r="E58" s="59"/>
-      <c r="F58" s="59"/>
-      <c r="G58" s="59"/>
-      <c r="H58" s="59"/>
-      <c r="I58" s="59"/>
-      <c r="J58" s="59"/>
-      <c r="K58" s="59"/>
-      <c r="L58" s="59"/>
-      <c r="M58" s="59"/>
-      <c r="N58" s="59"/>
+      <c r="B58" s="119" t="s">
+        <v>36</v>
+      </c>
+      <c r="C58" s="120"/>
+      <c r="D58" s="121"/>
+      <c r="E58" s="66">
+        <f>J42</f>
+        <v>0.35138888888888892</v>
+      </c>
+      <c r="F58" s="67">
+        <f t="shared" si="7"/>
+        <v>0.81744749596122779</v>
+      </c>
+      <c r="G58" s="63"/>
+      <c r="H58" s="64"/>
+      <c r="I58" s="64"/>
+      <c r="J58" s="64"/>
+      <c r="K58" s="64"/>
+      <c r="L58" s="64"/>
+      <c r="M58" s="64"/>
+      <c r="N58" s="65"/>
       <c r="O58" s="20"/>
       <c r="P58" s="59"/>
       <c r="Q58" s="59"/>
@@ -4259,21 +4543,26 @@
       <c r="Y58" s="59"/>
       <c r="Z58" s="59"/>
     </row>
-    <row r="59" spans="1:26">
+    <row r="59" spans="1:26" ht="15" customHeight="1">
       <c r="A59" s="20"/>
-      <c r="B59" s="59"/>
-      <c r="C59" s="59"/>
-      <c r="D59" s="59"/>
-      <c r="E59" s="59"/>
-      <c r="F59" s="59"/>
-      <c r="G59" s="59"/>
-      <c r="H59" s="59"/>
-      <c r="I59" s="59"/>
-      <c r="J59" s="59"/>
-      <c r="K59" s="59"/>
-      <c r="L59" s="59"/>
-      <c r="M59" s="59"/>
-      <c r="N59" s="59"/>
+      <c r="B59" s="124" t="s">
+        <v>37</v>
+      </c>
+      <c r="C59" s="125"/>
+      <c r="D59" s="123"/>
+      <c r="E59" s="122">
+        <f>IF(COUNTIF(E53:E58,"Error")&gt;0,"Error",IF(SUM(E53:E58)=0,"Completar",SUM(E53:E58)))</f>
+        <v>0.42986111111111114</v>
+      </c>
+      <c r="F59" s="123"/>
+      <c r="G59" s="68"/>
+      <c r="H59" s="69"/>
+      <c r="I59" s="69"/>
+      <c r="J59" s="69"/>
+      <c r="K59" s="69"/>
+      <c r="L59" s="69"/>
+      <c r="M59" s="69"/>
+      <c r="N59" s="70"/>
       <c r="O59" s="20"/>
       <c r="P59" s="59"/>
       <c r="Q59" s="59"/>
@@ -4287,35 +4576,35 @@
       <c r="Y59" s="59"/>
       <c r="Z59" s="59"/>
     </row>
-    <row r="60" spans="1:26">
+    <row r="60" spans="1:26" ht="6" customHeight="1">
       <c r="A60" s="20"/>
-      <c r="B60" s="59"/>
-      <c r="C60" s="59"/>
-      <c r="D60" s="59"/>
-      <c r="E60" s="59"/>
-      <c r="F60" s="59"/>
-      <c r="G60" s="59"/>
-      <c r="H60" s="59"/>
-      <c r="I60" s="59"/>
-      <c r="J60" s="59"/>
-      <c r="K60" s="59"/>
-      <c r="L60" s="59"/>
-      <c r="M60" s="59"/>
-      <c r="N60" s="59"/>
+      <c r="B60" s="20"/>
+      <c r="C60" s="20"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="20"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="20"/>
+      <c r="H60" s="20"/>
+      <c r="I60" s="20"/>
+      <c r="J60" s="20"/>
+      <c r="K60" s="20"/>
+      <c r="L60" s="20"/>
+      <c r="M60" s="20"/>
+      <c r="N60" s="20"/>
       <c r="O60" s="20"/>
-      <c r="P60" s="59"/>
-      <c r="Q60" s="59"/>
-      <c r="R60" s="59"/>
-      <c r="S60" s="59"/>
-      <c r="T60" s="59"/>
-      <c r="U60" s="59"/>
-      <c r="V60" s="59"/>
-      <c r="W60" s="59"/>
-      <c r="X60" s="59"/>
-      <c r="Y60" s="59"/>
-      <c r="Z60" s="59"/>
-    </row>
-    <row r="61" spans="1:26">
+      <c r="P60" s="20"/>
+      <c r="Q60" s="20"/>
+      <c r="R60" s="20"/>
+      <c r="S60" s="20"/>
+      <c r="T60" s="20"/>
+      <c r="U60" s="20"/>
+      <c r="V60" s="20"/>
+      <c r="W60" s="20"/>
+      <c r="X60" s="20"/>
+      <c r="Y60" s="20"/>
+      <c r="Z60" s="20"/>
+    </row>
+    <row r="61" spans="1:26" hidden="1">
       <c r="A61" s="20"/>
       <c r="B61" s="59"/>
       <c r="C61" s="59"/>
@@ -30999,37 +31288,112 @@
       <c r="Y1013" s="59"/>
       <c r="Z1013" s="59"/>
     </row>
+    <row r="1014" spans="1:26">
+      <c r="A1014" s="20"/>
+      <c r="B1014" s="59"/>
+      <c r="C1014" s="59"/>
+      <c r="D1014" s="59"/>
+      <c r="E1014" s="59"/>
+      <c r="F1014" s="59"/>
+      <c r="G1014" s="59"/>
+      <c r="H1014" s="59"/>
+      <c r="I1014" s="59"/>
+      <c r="J1014" s="59"/>
+      <c r="K1014" s="59"/>
+      <c r="L1014" s="59"/>
+      <c r="M1014" s="59"/>
+      <c r="N1014" s="59"/>
+      <c r="O1014" s="20"/>
+      <c r="P1014" s="59"/>
+      <c r="Q1014" s="59"/>
+      <c r="R1014" s="59"/>
+      <c r="S1014" s="59"/>
+      <c r="T1014" s="59"/>
+      <c r="U1014" s="59"/>
+      <c r="V1014" s="59"/>
+      <c r="W1014" s="59"/>
+      <c r="X1014" s="59"/>
+      <c r="Y1014" s="59"/>
+      <c r="Z1014" s="59"/>
+    </row>
+    <row r="1015" spans="1:26">
+      <c r="A1015" s="20"/>
+      <c r="B1015" s="59"/>
+      <c r="C1015" s="59"/>
+      <c r="D1015" s="59"/>
+      <c r="E1015" s="59"/>
+      <c r="F1015" s="59"/>
+      <c r="G1015" s="59"/>
+      <c r="H1015" s="59"/>
+      <c r="I1015" s="59"/>
+      <c r="J1015" s="59"/>
+      <c r="K1015" s="59"/>
+      <c r="L1015" s="59"/>
+      <c r="M1015" s="59"/>
+      <c r="N1015" s="59"/>
+      <c r="O1015" s="20"/>
+      <c r="P1015" s="59"/>
+      <c r="Q1015" s="59"/>
+      <c r="R1015" s="59"/>
+      <c r="S1015" s="59"/>
+      <c r="T1015" s="59"/>
+      <c r="U1015" s="59"/>
+      <c r="V1015" s="59"/>
+      <c r="W1015" s="59"/>
+      <c r="X1015" s="59"/>
+      <c r="Y1015" s="59"/>
+      <c r="Z1015" s="59"/>
+    </row>
+    <row r="1016" spans="1:26">
+      <c r="A1016" s="20"/>
+      <c r="B1016" s="59"/>
+      <c r="C1016" s="59"/>
+      <c r="D1016" s="59"/>
+      <c r="E1016" s="59"/>
+      <c r="F1016" s="59"/>
+      <c r="G1016" s="59"/>
+      <c r="H1016" s="59"/>
+      <c r="I1016" s="59"/>
+      <c r="J1016" s="59"/>
+      <c r="K1016" s="59"/>
+      <c r="L1016" s="59"/>
+      <c r="M1016" s="59"/>
+      <c r="N1016" s="59"/>
+      <c r="O1016" s="20"/>
+      <c r="P1016" s="59"/>
+      <c r="Q1016" s="59"/>
+      <c r="R1016" s="59"/>
+      <c r="S1016" s="59"/>
+      <c r="T1016" s="59"/>
+      <c r="U1016" s="59"/>
+      <c r="V1016" s="59"/>
+      <c r="W1016" s="59"/>
+      <c r="X1016" s="59"/>
+      <c r="Y1016" s="59"/>
+      <c r="Z1016" s="59"/>
+    </row>
   </sheetData>
-  <mergeCells count="57">
-    <mergeCell ref="D1:N1"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="F8:N8"/>
-    <mergeCell ref="F9:N9"/>
-    <mergeCell ref="B15:N15"/>
-    <mergeCell ref="F12:N12"/>
-    <mergeCell ref="F13:N13"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="C24:E24"/>
+  <mergeCells count="59">
+    <mergeCell ref="C33:E33"/>
     <mergeCell ref="C38:E38"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B45:N45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
     <mergeCell ref="N16:N17"/>
     <mergeCell ref="C21:E21"/>
     <mergeCell ref="C20:E20"/>
@@ -31038,33 +31402,44 @@
     <mergeCell ref="H16:J16"/>
     <mergeCell ref="K16:L16"/>
     <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
     <mergeCell ref="M16:M17"/>
     <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B48:N48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B15:N15"/>
+    <mergeCell ref="F12:N12"/>
+    <mergeCell ref="F13:N13"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="D1:N1"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F8:N8"/>
+    <mergeCell ref="F9:N9"/>
   </mergeCells>
-  <conditionalFormatting sqref="D1:XFD24 C3:C24 A39:XFD1048576 A1:B38 N25:XFD38 J27:J38 C30:I37 K30:M37">
+  <conditionalFormatting sqref="D1:XFD24 C3:C24 A42:XFD1048576 N25:XFD35 J27:J35 C30:I35 K30:M35 J41 N41:XFD41 O36:XFD40 A1:B41">
     <cfRule type="cellIs" dxfId="15" priority="35" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:XFD24 C3:C24 A39:XFD1048576 A1:B38 N25:XFD38 J27:J38 C30:I37 K30:M37">
+  <conditionalFormatting sqref="D1:XFD24 C3:C24 A42:XFD1048576 N25:XFD35 J27:J35 C30:I35 K30:M35 J41 N41:XFD41 O36:XFD40 A1:B41">
     <cfRule type="cellIs" dxfId="14" priority="36" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
@@ -31079,12 +31454,12 @@
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F26:M26 C38 F38:I38 K38:M38">
+  <conditionalFormatting sqref="F26:M26 C41 F41:I41 K41:M41">
     <cfRule type="cellIs" dxfId="11" priority="27" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F26:M26 C38 F38:I38 K38:M38">
+  <conditionalFormatting sqref="F26:M26 C41 F41:I41 K41:M41">
     <cfRule type="cellIs" dxfId="10" priority="28" operator="equal">
       <formula>"Error"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Actualizar documentacion MatrizMath y Sel
Se actualizan metricas y diagrama de clases de MatrizMath y Sel.
</commit_message>
<xml_diff>
--- a/Documentacion/MatrizMath/MatrizMath - Planilla de Métricas V2.1.xlsx
+++ b/Documentacion/MatrizMath/MatrizMath - Planilla de Métricas V2.1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
   <si>
     <t>PROYECTO:</t>
   </si>
@@ -189,6 +189,9 @@
   <si>
     <t>normaDos()</t>
   </si>
+  <si>
+    <t>setIdentidad()</t>
+  </si>
 </sst>
 </file>
 
@@ -326,7 +329,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -830,11 +833,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1156,46 +1172,89 @@
     <xf numFmtId="20" fontId="7" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1208,80 +1267,54 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="24">
     <dxf>
       <font>
         <color rgb="FFFFFFFF"/>
@@ -1321,6 +1354,37 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFC00000"/>
           <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
       <border>
@@ -1638,7 +1702,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
@@ -1649,8 +1713,8 @@
           <c:yMode val="edge"/>
           <c:x val="3.3565974707706982E-2"/>
           <c:y val="7.4074152627750078E-2"/>
-          <c:w val="0.40158680164979438"/>
-          <c:h val="0.85185169474450084"/>
+          <c:w val="0.40158680164979443"/>
+          <c:h val="0.85185169474450095"/>
         </c:manualLayout>
       </c:layout>
       <c:pieChart>
@@ -1738,7 +1802,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Métricas!$B$53:$B$58</c:f>
+              <c:f>Métricas!$B$54:$B$59</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1764,9 +1828,9 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Métricas!$C$53:$C$58</c:f>
+              <c:f>Métricas!$C$54:$C$59</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>@</c:formatCode>
                 <c:ptCount val="6"/>
               </c:numCache>
             </c:numRef>
@@ -1777,7 +1841,6 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
       <c:spPr>
@@ -1796,7 +1859,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1808,13 +1871,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2092,7 +2155,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2100,13 +2163,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z1016"/>
+  <dimension ref="A1:Z1017"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42:E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
@@ -2122,23 +2185,23 @@
   <sheetData>
     <row r="1" spans="1:26" ht="23.25" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="159" t="s">
+      <c r="B1" s="117" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="149"/>
-      <c r="D1" s="158" t="s">
+      <c r="C1" s="113"/>
+      <c r="D1" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="149"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="149"/>
-      <c r="H1" s="149"/>
-      <c r="I1" s="149"/>
-      <c r="J1" s="149"/>
-      <c r="K1" s="149"/>
-      <c r="L1" s="149"/>
-      <c r="M1" s="149"/>
-      <c r="N1" s="149"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
+      <c r="N1" s="113"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -2182,12 +2245,12 @@
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
       <c r="A3" s="4"/>
-      <c r="B3" s="112" t="s">
+      <c r="B3" s="114" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="113"/>
-      <c r="D3" s="113"/>
-      <c r="E3" s="114"/>
+      <c r="C3" s="115"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="116"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -2313,12 +2376,12 @@
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1">
       <c r="A7" s="4"/>
-      <c r="B7" s="112" t="s">
+      <c r="B7" s="114" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="113"/>
-      <c r="D7" s="113"/>
-      <c r="E7" s="114"/>
+      <c r="C7" s="115"/>
+      <c r="D7" s="115"/>
+      <c r="E7" s="116"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -2355,15 +2418,15 @@
       <c r="E8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="148"/>
-      <c r="G8" s="149"/>
-      <c r="H8" s="149"/>
-      <c r="I8" s="149"/>
-      <c r="J8" s="149"/>
-      <c r="K8" s="149"/>
-      <c r="L8" s="149"/>
-      <c r="M8" s="149"/>
-      <c r="N8" s="149"/>
+      <c r="F8" s="118"/>
+      <c r="G8" s="113"/>
+      <c r="H8" s="113"/>
+      <c r="I8" s="113"/>
+      <c r="J8" s="113"/>
+      <c r="K8" s="113"/>
+      <c r="L8" s="113"/>
+      <c r="M8" s="113"/>
+      <c r="N8" s="113"/>
       <c r="O8" s="7"/>
       <c r="P8" s="13"/>
       <c r="Q8" s="14"/>
@@ -2390,15 +2453,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C9),ISBLANK(D9)),"Completar",IF(D9&gt;=C9,D9-C9,"Error")),"Error")</f>
         <v>Completar</v>
       </c>
-      <c r="F9" s="150"/>
-      <c r="G9" s="149"/>
-      <c r="H9" s="149"/>
-      <c r="I9" s="149"/>
-      <c r="J9" s="149"/>
-      <c r="K9" s="149"/>
-      <c r="L9" s="149"/>
-      <c r="M9" s="149"/>
-      <c r="N9" s="149"/>
+      <c r="F9" s="119"/>
+      <c r="G9" s="113"/>
+      <c r="H9" s="113"/>
+      <c r="I9" s="113"/>
+      <c r="J9" s="113"/>
+      <c r="K9" s="113"/>
+      <c r="L9" s="113"/>
+      <c r="M9" s="113"/>
+      <c r="N9" s="113"/>
       <c r="O9" s="15"/>
       <c r="P9" s="21"/>
       <c r="Q9" s="22"/>
@@ -2442,12 +2505,12 @@
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" s="4"/>
-      <c r="B11" s="112" t="s">
+      <c r="B11" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="113"/>
-      <c r="D11" s="113"/>
-      <c r="E11" s="114"/>
+      <c r="C11" s="115"/>
+      <c r="D11" s="115"/>
+      <c r="E11" s="116"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -2484,15 +2547,15 @@
       <c r="E12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="148"/>
-      <c r="G12" s="149"/>
-      <c r="H12" s="149"/>
-      <c r="I12" s="149"/>
-      <c r="J12" s="149"/>
-      <c r="K12" s="149"/>
-      <c r="L12" s="149"/>
-      <c r="M12" s="149"/>
-      <c r="N12" s="149"/>
+      <c r="F12" s="118"/>
+      <c r="G12" s="113"/>
+      <c r="H12" s="113"/>
+      <c r="I12" s="113"/>
+      <c r="J12" s="113"/>
+      <c r="K12" s="113"/>
+      <c r="L12" s="113"/>
+      <c r="M12" s="113"/>
+      <c r="N12" s="113"/>
       <c r="O12" s="7"/>
       <c r="P12" s="13"/>
       <c r="Q12" s="14"/>
@@ -2517,15 +2580,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C13),ISBLANK(D13)),"Completar",IF(D13&gt;=C13,D13-C13,"Error")),"Error")</f>
         <v>Completar</v>
       </c>
-      <c r="F13" s="150"/>
-      <c r="G13" s="149"/>
-      <c r="H13" s="149"/>
-      <c r="I13" s="149"/>
-      <c r="J13" s="149"/>
-      <c r="K13" s="149"/>
-      <c r="L13" s="149"/>
-      <c r="M13" s="149"/>
-      <c r="N13" s="149"/>
+      <c r="F13" s="119"/>
+      <c r="G13" s="113"/>
+      <c r="H13" s="113"/>
+      <c r="I13" s="113"/>
+      <c r="J13" s="113"/>
+      <c r="K13" s="113"/>
+      <c r="L13" s="113"/>
+      <c r="M13" s="113"/>
+      <c r="N13" s="113"/>
       <c r="O13" s="15"/>
       <c r="P13" s="21"/>
       <c r="Q13" s="22"/>
@@ -2569,21 +2632,21 @@
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1">
       <c r="A15" s="4"/>
-      <c r="B15" s="112" t="s">
+      <c r="B15" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="113"/>
-      <c r="D15" s="113"/>
-      <c r="E15" s="113"/>
-      <c r="F15" s="113"/>
-      <c r="G15" s="113"/>
-      <c r="H15" s="113"/>
-      <c r="I15" s="113"/>
-      <c r="J15" s="113"/>
-      <c r="K15" s="113"/>
-      <c r="L15" s="113"/>
-      <c r="M15" s="113"/>
-      <c r="N15" s="114"/>
+      <c r="C15" s="115"/>
+      <c r="D15" s="115"/>
+      <c r="E15" s="115"/>
+      <c r="F15" s="115"/>
+      <c r="G15" s="115"/>
+      <c r="H15" s="115"/>
+      <c r="I15" s="115"/>
+      <c r="J15" s="115"/>
+      <c r="K15" s="115"/>
+      <c r="L15" s="115"/>
+      <c r="M15" s="115"/>
+      <c r="N15" s="116"/>
       <c r="O15" s="4"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
@@ -2599,31 +2662,31 @@
     </row>
     <row r="16" spans="1:26" ht="16.5" customHeight="1">
       <c r="A16" s="7"/>
-      <c r="B16" s="131" t="s">
+      <c r="B16" s="140" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="133" t="s">
+      <c r="C16" s="142" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="134"/>
-      <c r="E16" s="134"/>
-      <c r="F16" s="141" t="s">
+      <c r="D16" s="143"/>
+      <c r="E16" s="143"/>
+      <c r="F16" s="136" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="142"/>
-      <c r="H16" s="140" t="s">
+      <c r="G16" s="137"/>
+      <c r="H16" s="135" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="123"/>
-      <c r="J16" s="123"/>
-      <c r="K16" s="141" t="s">
+      <c r="I16" s="121"/>
+      <c r="J16" s="121"/>
+      <c r="K16" s="136" t="s">
         <v>14</v>
       </c>
-      <c r="L16" s="142"/>
-      <c r="M16" s="143" t="s">
+      <c r="L16" s="137"/>
+      <c r="M16" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="N16" s="138" t="s">
+      <c r="N16" s="130" t="s">
         <v>6</v>
       </c>
       <c r="O16" s="7"/>
@@ -2641,10 +2704,10 @@
     </row>
     <row r="17" spans="1:26" ht="30" customHeight="1">
       <c r="A17" s="7"/>
-      <c r="B17" s="132"/>
-      <c r="C17" s="135"/>
-      <c r="D17" s="136"/>
-      <c r="E17" s="136"/>
+      <c r="B17" s="141"/>
+      <c r="C17" s="144"/>
+      <c r="D17" s="145"/>
+      <c r="E17" s="145"/>
       <c r="F17" s="26" t="s">
         <v>16</v>
       </c>
@@ -2666,8 +2729,8 @@
       <c r="L17" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="M17" s="144"/>
-      <c r="N17" s="139"/>
+      <c r="M17" s="139"/>
+      <c r="N17" s="131"/>
       <c r="O17" s="7"/>
       <c r="P17" s="13"/>
       <c r="Q17" s="14"/>
@@ -2684,14 +2747,14 @@
     <row r="18" spans="1:26">
       <c r="A18" s="15"/>
       <c r="B18" s="30">
-        <f t="shared" ref="B18:B41" si="0">ROW($B18)-16</f>
+        <f t="shared" ref="B18:B40" si="0">ROW($B18)-16</f>
         <v>2</v>
       </c>
-      <c r="C18" s="137" t="s">
+      <c r="C18" s="132" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="123"/>
-      <c r="E18" s="123"/>
+      <c r="D18" s="121"/>
+      <c r="E18" s="121"/>
       <c r="F18" s="31">
         <v>60</v>
       </c>
@@ -2740,11 +2803,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C19" s="137" t="s">
+      <c r="C19" s="132" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="123"/>
-      <c r="E19" s="123"/>
+      <c r="D19" s="121"/>
+      <c r="E19" s="121"/>
       <c r="F19" s="31">
         <v>4</v>
       </c>
@@ -2793,11 +2856,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C20" s="137" t="s">
+      <c r="C20" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="123"/>
-      <c r="E20" s="123"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="121"/>
       <c r="F20" s="31">
         <v>8</v>
       </c>
@@ -2846,11 +2909,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C21" s="137" t="s">
+      <c r="C21" s="132" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="123"/>
-      <c r="E21" s="123"/>
+      <c r="D21" s="121"/>
+      <c r="E21" s="121"/>
       <c r="F21" s="31">
         <v>10</v>
       </c>
@@ -2899,11 +2962,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C22" s="124" t="s">
+      <c r="C22" s="133" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="129"/>
-      <c r="E22" s="129"/>
+      <c r="D22" s="134"/>
+      <c r="E22" s="134"/>
       <c r="F22" s="70">
         <v>8</v>
       </c>
@@ -2952,11 +3015,11 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C23" s="120" t="s">
+      <c r="C23" s="126" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="123"/>
-      <c r="E23" s="123"/>
+      <c r="D23" s="121"/>
+      <c r="E23" s="121"/>
       <c r="F23" s="40">
         <v>13</v>
       </c>
@@ -3005,11 +3068,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C24" s="120" t="s">
+      <c r="C24" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="123"/>
-      <c r="E24" s="123"/>
+      <c r="D24" s="121"/>
+      <c r="E24" s="121"/>
       <c r="F24" s="40">
         <v>25</v>
       </c>
@@ -3058,11 +3121,11 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C25" s="120" t="s">
+      <c r="C25" s="126" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="123"/>
-      <c r="E25" s="123"/>
+      <c r="D25" s="121"/>
+      <c r="E25" s="121"/>
       <c r="F25" s="40">
         <v>20</v>
       </c>
@@ -3111,11 +3174,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C26" s="120" t="s">
+      <c r="C26" s="126" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="123"/>
-      <c r="E26" s="123"/>
+      <c r="D26" s="121"/>
+      <c r="E26" s="121"/>
       <c r="F26" s="40">
         <v>16</v>
       </c>
@@ -3164,11 +3227,11 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C27" s="120" t="s">
+      <c r="C27" s="126" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="123"/>
-      <c r="E27" s="123"/>
+      <c r="D27" s="121"/>
+      <c r="E27" s="121"/>
       <c r="F27" s="40">
         <v>30</v>
       </c>
@@ -3217,11 +3280,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C28" s="120" t="s">
+      <c r="C28" s="126" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="121"/>
-      <c r="E28" s="122"/>
+      <c r="D28" s="151"/>
+      <c r="E28" s="152"/>
       <c r="F28" s="82">
         <v>30</v>
       </c>
@@ -3270,11 +3333,11 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C29" s="120" t="s">
+      <c r="C29" s="126" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="121"/>
-      <c r="E29" s="122"/>
+      <c r="D29" s="151"/>
+      <c r="E29" s="152"/>
       <c r="F29" s="82">
         <v>15</v>
       </c>
@@ -3323,11 +3386,11 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C30" s="120" t="s">
+      <c r="C30" s="126" t="s">
         <v>51</v>
       </c>
-      <c r="D30" s="121"/>
-      <c r="E30" s="122"/>
+      <c r="D30" s="151"/>
+      <c r="E30" s="152"/>
       <c r="F30" s="82">
         <v>25</v>
       </c>
@@ -3376,11 +3439,11 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C31" s="120" t="s">
+      <c r="C31" s="126" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="121"/>
-      <c r="E31" s="122"/>
+      <c r="D31" s="151"/>
+      <c r="E31" s="152"/>
       <c r="F31" s="82">
         <v>18</v>
       </c>
@@ -3429,11 +3492,11 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C32" s="120" t="s">
+      <c r="C32" s="126" t="s">
         <v>47</v>
       </c>
-      <c r="D32" s="121"/>
-      <c r="E32" s="122"/>
+      <c r="D32" s="151"/>
+      <c r="E32" s="152"/>
       <c r="F32" s="82">
         <v>17</v>
       </c>
@@ -3447,7 +3510,7 @@
         <v>0.87847222222222221</v>
       </c>
       <c r="J32" s="85">
-        <f t="shared" ref="J32:J40" si="4">IFERROR(IF(OR(ISBLANK(H32),ISBLANK(I32)),"",IF(I32&gt;=H32,I32-H32,"Error")),"Error")</f>
+        <f t="shared" ref="J32:J41" si="4">IFERROR(IF(OR(ISBLANK(H32),ISBLANK(I32)),"",IF(I32&gt;=H32,I32-H32,"Error")),"Error")</f>
         <v>1.4583333333333282E-2</v>
       </c>
       <c r="K32" s="86">
@@ -3478,15 +3541,15 @@
     </row>
     <row r="33" spans="1:26" s="98" customFormat="1" ht="15" customHeight="1">
       <c r="A33" s="90"/>
-      <c r="B33" s="110">
+      <c r="B33" s="109">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C33" s="124" t="s">
+      <c r="C33" s="133" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="125"/>
-      <c r="E33" s="126"/>
+      <c r="D33" s="146"/>
+      <c r="E33" s="147"/>
       <c r="F33" s="91">
         <v>20</v>
       </c>
@@ -3531,15 +3594,15 @@
     </row>
     <row r="34" spans="1:26" s="98" customFormat="1" ht="15" customHeight="1">
       <c r="A34" s="90"/>
-      <c r="B34" s="110">
+      <c r="B34" s="109">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C34" s="124" t="s">
+      <c r="C34" s="133" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="125"/>
-      <c r="E34" s="126"/>
+      <c r="D34" s="146"/>
+      <c r="E34" s="147"/>
       <c r="F34" s="91">
         <v>18</v>
       </c>
@@ -3584,15 +3647,15 @@
     </row>
     <row r="35" spans="1:26" s="98" customFormat="1" ht="15" customHeight="1">
       <c r="A35" s="90"/>
-      <c r="B35" s="110">
+      <c r="B35" s="109">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C35" s="124" t="s">
+      <c r="C35" s="133" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="129"/>
-      <c r="E35" s="130"/>
+      <c r="D35" s="134"/>
+      <c r="E35" s="150"/>
       <c r="F35" s="91">
         <v>20</v>
       </c>
@@ -3637,15 +3700,15 @@
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1">
       <c r="A36" s="81"/>
-      <c r="B36" s="110">
+      <c r="B36" s="109">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C36" s="117" t="s">
+      <c r="C36" s="154" t="s">
         <v>54</v>
       </c>
-      <c r="D36" s="118"/>
-      <c r="E36" s="119"/>
+      <c r="D36" s="155"/>
+      <c r="E36" s="156"/>
       <c r="F36" s="105">
         <v>20</v>
       </c>
@@ -3690,15 +3753,15 @@
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1">
       <c r="A37" s="81"/>
-      <c r="B37" s="110">
+      <c r="B37" s="109">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C37" s="117" t="s">
+      <c r="C37" s="154" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="118"/>
-      <c r="E37" s="119"/>
+      <c r="D37" s="155"/>
+      <c r="E37" s="156"/>
       <c r="F37" s="105">
         <v>20</v>
       </c>
@@ -3743,15 +3806,15 @@
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1">
       <c r="A38" s="99"/>
-      <c r="B38" s="110">
+      <c r="B38" s="109">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C38" s="127" t="s">
+      <c r="C38" s="148" t="s">
         <v>53</v>
       </c>
-      <c r="D38" s="127"/>
-      <c r="E38" s="128"/>
+      <c r="D38" s="148"/>
+      <c r="E38" s="149"/>
       <c r="F38" s="105">
         <v>25</v>
       </c>
@@ -3796,15 +3859,15 @@
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1">
       <c r="A39" s="99"/>
-      <c r="B39" s="110">
+      <c r="B39" s="109">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="C39" s="127" t="s">
+      <c r="C39" s="148" t="s">
         <v>56</v>
       </c>
-      <c r="D39" s="127"/>
-      <c r="E39" s="128"/>
+      <c r="D39" s="148"/>
+      <c r="E39" s="149"/>
       <c r="F39" s="105">
         <v>25</v>
       </c>
@@ -3853,11 +3916,11 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C40" s="117" t="s">
+      <c r="C40" s="154" t="s">
         <v>57</v>
       </c>
-      <c r="D40" s="118"/>
-      <c r="E40" s="119"/>
+      <c r="D40" s="155"/>
+      <c r="E40" s="156"/>
       <c r="F40" s="105">
         <v>25</v>
       </c>
@@ -3870,7 +3933,7 @@
       <c r="I40" s="104">
         <v>0.40972222222222227</v>
       </c>
-      <c r="J40" s="111">
+      <c r="J40" s="110">
         <f t="shared" si="4"/>
         <v>7.6388888888889173E-3</v>
       </c>
@@ -3900,31 +3963,46 @@
       <c r="Y40" s="22"/>
       <c r="Z40" s="22"/>
     </row>
-    <row r="41" spans="1:26" ht="15" customHeight="1">
-      <c r="A41" s="67"/>
+    <row r="41" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A41" s="111"/>
       <c r="B41" s="30">
-        <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="C41" s="154"/>
-      <c r="D41" s="154"/>
-      <c r="E41" s="155"/>
-      <c r="F41" s="82"/>
-      <c r="G41" s="89"/>
-      <c r="H41" s="41"/>
-      <c r="I41" s="42"/>
-      <c r="J41" s="85" t="str">
-        <f t="shared" ref="J41" si="5">IFERROR(IF(OR(ISBLANK(H41),ISBLANK(I41)),"",IF(I41&gt;=H41,I41-H41,"Error")),"Error")</f>
-        <v/>
-      </c>
-      <c r="K41" s="86"/>
-      <c r="L41" s="109"/>
-      <c r="M41" s="82"/>
-      <c r="N41" s="88" t="str">
+      <c r="C41" s="154" t="s">
+        <v>58</v>
+      </c>
+      <c r="D41" s="155"/>
+      <c r="E41" s="156"/>
+      <c r="F41" s="105">
+        <v>20</v>
+      </c>
+      <c r="G41" s="106">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="H41" s="103">
+        <v>3.6111111111111115E-2</v>
+      </c>
+      <c r="I41" s="104">
+        <v>5.8333333333333327E-2</v>
+      </c>
+      <c r="J41" s="110">
+        <f t="shared" si="4"/>
+        <v>2.2222222222222213E-2</v>
+      </c>
+      <c r="K41" s="105">
+        <v>0</v>
+      </c>
+      <c r="L41" s="108">
+        <v>0</v>
+      </c>
+      <c r="M41" s="105">
+        <v>18</v>
+      </c>
+      <c r="N41" s="77">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="O41" s="67"/>
+        <v>2.2222222222222213E-2</v>
+      </c>
+      <c r="O41" s="111"/>
       <c r="P41" s="21"/>
       <c r="Q41" s="22"/>
       <c r="R41" s="22"/>
@@ -3937,264 +4015,261 @@
       <c r="Y41" s="22"/>
       <c r="Z41" s="22"/>
     </row>
-    <row r="42" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A42" s="7"/>
-      <c r="B42" s="115" t="s">
+    <row r="42" spans="1:26" ht="15" customHeight="1">
+      <c r="A42" s="67"/>
+      <c r="B42" s="30">
+        <v>26</v>
+      </c>
+      <c r="C42" s="154"/>
+      <c r="D42" s="155"/>
+      <c r="E42" s="156"/>
+      <c r="F42" s="105"/>
+      <c r="G42" s="106"/>
+      <c r="H42" s="103"/>
+      <c r="I42" s="104"/>
+      <c r="J42" s="110"/>
+      <c r="K42" s="105"/>
+      <c r="L42" s="108"/>
+      <c r="M42" s="105"/>
+      <c r="N42" s="77"/>
+      <c r="O42" s="67"/>
+      <c r="P42" s="21"/>
+      <c r="Q42" s="22"/>
+      <c r="R42" s="22"/>
+      <c r="S42" s="22"/>
+      <c r="T42" s="22"/>
+      <c r="U42" s="22"/>
+      <c r="V42" s="22"/>
+      <c r="W42" s="22"/>
+      <c r="X42" s="22"/>
+      <c r="Y42" s="22"/>
+      <c r="Z42" s="22"/>
+    </row>
+    <row r="43" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A43" s="7"/>
+      <c r="B43" s="153" t="s">
         <v>23</v>
       </c>
-      <c r="C42" s="116"/>
-      <c r="D42" s="116"/>
-      <c r="E42" s="116"/>
-      <c r="F42" s="46">
-        <f>IF(SUM(F18:F41)=0,"Completar",SUM(F18:F41))</f>
-        <v>472</v>
-      </c>
-      <c r="G42" s="47">
-        <f>IF(SUM(G18:G41)=0,"Completar",SUM(G18:G41))</f>
-        <v>0.36874999999999991</v>
-      </c>
-      <c r="H42" s="48" t="s">
+      <c r="C43" s="163"/>
+      <c r="D43" s="163"/>
+      <c r="E43" s="164"/>
+      <c r="F43" s="46">
+        <f>IF(SUM(F18:F42)=0,"Completar",SUM(F18:F42))</f>
+        <v>492</v>
+      </c>
+      <c r="G43" s="47">
+        <f>IF(SUM(G18:G42)=0,"Completar",SUM(G18:G42))</f>
+        <v>0.38263888888888881</v>
+      </c>
+      <c r="H43" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="I42" s="49" t="s">
+      <c r="I43" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="J42" s="101">
-        <f>IF(OR(COUNTIF(J18:J41,"Error")&gt;0,COUNTIF(J18:J41,"Completar")&gt;0),"Error",IF(SUM(J18:J41)=0,"Completar",SUM(J18:J41)))</f>
-        <v>0.35902777777777817</v>
-      </c>
-      <c r="K42" s="50">
-        <f>SUM(K18:K41)</f>
+      <c r="J43" s="101">
+        <f>IF(OR(COUNTIF(J18:J42,"Error")&gt;0,COUNTIF(J18:J42,"Completar")&gt;0),"Error",IF(SUM(J18:J42)=0,"Completar",SUM(J18:J42)))</f>
+        <v>0.38125000000000037</v>
+      </c>
+      <c r="K43" s="50">
+        <f>SUM(K18:K42)</f>
         <v>25</v>
       </c>
-      <c r="L42" s="47">
-        <f>SUM(L18:L41)</f>
+      <c r="L43" s="47">
+        <f>SUM(L18:L42)</f>
         <v>7.4305555555555555E-2</v>
       </c>
-      <c r="M42" s="51">
-        <f>IF(SUM(M18:M41)=0,"Completar",SUM(M18:M41))</f>
-        <v>439</v>
-      </c>
-      <c r="N42" s="18">
-        <f>IF(OR(COUNTIF(N18:N41,"Error")&gt;0,COUNTIF(N18:N41,"Completar")&gt;0),"Error",IF(SUM(N18:N41)=0,"Completar",SUM(N18:N41)))</f>
-        <v>0.43333333333333363</v>
-      </c>
-      <c r="O42" s="7"/>
-      <c r="P42" s="52"/>
-      <c r="Q42" s="53"/>
-      <c r="R42" s="53"/>
-      <c r="S42" s="53"/>
-      <c r="T42" s="53"/>
-      <c r="U42" s="53"/>
-      <c r="V42" s="53"/>
-      <c r="W42" s="53"/>
-      <c r="X42" s="53"/>
-      <c r="Y42" s="53"/>
-      <c r="Z42" s="53"/>
-    </row>
-    <row r="43" spans="1:26" ht="6" customHeight="1">
-      <c r="A43" s="20"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
-      <c r="K43" s="20"/>
-      <c r="L43" s="20"/>
-      <c r="M43" s="20"/>
-      <c r="N43" s="20"/>
-      <c r="O43" s="20"/>
-      <c r="P43" s="23"/>
-      <c r="Q43" s="23"/>
-      <c r="R43" s="23"/>
-      <c r="S43" s="23"/>
-      <c r="T43" s="23"/>
-      <c r="U43" s="23"/>
-      <c r="V43" s="23"/>
-      <c r="W43" s="23"/>
-      <c r="X43" s="23"/>
-      <c r="Y43" s="23"/>
-      <c r="Z43" s="23"/>
-    </row>
-    <row r="44" spans="1:26" ht="15" customHeight="1">
-      <c r="A44" s="4"/>
-      <c r="B44" s="112" t="s">
+      <c r="M43" s="51">
+        <f>IF(SUM(M18:M42)=0,"Completar",SUM(M18:M42))</f>
+        <v>457</v>
+      </c>
+      <c r="N43" s="18">
+        <f>IF(OR(COUNTIF(N18:N42,"Error")&gt;0,COUNTIF(N18:N42,"Completar")&gt;0),"Error",IF(SUM(N18:N42)=0,"Completar",SUM(N18:N42)))</f>
+        <v>0.45555555555555582</v>
+      </c>
+      <c r="O43" s="7"/>
+      <c r="P43" s="52"/>
+      <c r="Q43" s="53"/>
+      <c r="R43" s="53"/>
+      <c r="S43" s="53"/>
+      <c r="T43" s="53"/>
+      <c r="U43" s="53"/>
+      <c r="V43" s="53"/>
+      <c r="W43" s="53"/>
+      <c r="X43" s="53"/>
+      <c r="Y43" s="53"/>
+      <c r="Z43" s="53"/>
+    </row>
+    <row r="44" spans="1:26" ht="6" customHeight="1" thickBot="1">
+      <c r="A44" s="20"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="20"/>
+      <c r="L44" s="20"/>
+      <c r="M44" s="20"/>
+      <c r="N44" s="20"/>
+      <c r="O44" s="20"/>
+      <c r="P44" s="23"/>
+      <c r="Q44" s="23"/>
+      <c r="R44" s="23"/>
+      <c r="S44" s="23"/>
+      <c r="T44" s="23"/>
+      <c r="U44" s="23"/>
+      <c r="V44" s="23"/>
+      <c r="W44" s="23"/>
+      <c r="X44" s="23"/>
+      <c r="Y44" s="23"/>
+      <c r="Z44" s="23"/>
+    </row>
+    <row r="45" spans="1:26" ht="15" customHeight="1">
+      <c r="A45" s="4"/>
+      <c r="B45" s="114" t="s">
         <v>25</v>
       </c>
-      <c r="C44" s="113"/>
-      <c r="D44" s="113"/>
-      <c r="E44" s="114"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
-      <c r="J44" s="5"/>
-      <c r="K44" s="5"/>
-      <c r="L44" s="5"/>
-      <c r="M44" s="5"/>
-      <c r="N44" s="5"/>
-      <c r="O44" s="4"/>
-      <c r="P44" s="6"/>
-      <c r="Q44" s="6"/>
-      <c r="R44" s="6"/>
-      <c r="S44" s="6"/>
-      <c r="T44" s="6"/>
-      <c r="U44" s="6"/>
-      <c r="V44" s="6"/>
-      <c r="W44" s="6"/>
-      <c r="X44" s="6"/>
-      <c r="Y44" s="6"/>
-      <c r="Z44" s="6"/>
-    </row>
-    <row r="45" spans="1:26" ht="30" customHeight="1">
-      <c r="A45" s="7"/>
-      <c r="B45" s="8" t="s">
+      <c r="C45" s="161"/>
+      <c r="D45" s="161"/>
+      <c r="E45" s="162"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="5"/>
+      <c r="O45" s="4"/>
+      <c r="P45" s="6"/>
+      <c r="Q45" s="6"/>
+      <c r="R45" s="6"/>
+      <c r="S45" s="6"/>
+      <c r="T45" s="6"/>
+      <c r="U45" s="6"/>
+      <c r="V45" s="6"/>
+      <c r="W45" s="6"/>
+      <c r="X45" s="6"/>
+      <c r="Y45" s="6"/>
+      <c r="Z45" s="6"/>
+    </row>
+    <row r="46" spans="1:26" ht="30" customHeight="1">
+      <c r="A46" s="7"/>
+      <c r="B46" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C45" s="9" t="s">
+      <c r="C46" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="9" t="s">
+      <c r="D46" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E45" s="10" t="s">
+      <c r="E46" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="7"/>
-      <c r="K45" s="7"/>
-      <c r="L45" s="7"/>
-      <c r="M45" s="7"/>
-      <c r="N45" s="7"/>
-      <c r="O45" s="7"/>
-      <c r="P45" s="13"/>
-      <c r="Q45" s="14"/>
-      <c r="R45" s="14"/>
-      <c r="S45" s="14"/>
-      <c r="T45" s="14"/>
-      <c r="U45" s="14"/>
-      <c r="V45" s="14"/>
-      <c r="W45" s="14"/>
-      <c r="X45" s="14"/>
-      <c r="Y45" s="14"/>
-      <c r="Z45" s="14"/>
-    </row>
-    <row r="46" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A46" s="15"/>
-      <c r="B46" s="54"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="18" t="str">
-        <f>IFERROR(IF(OR(ISBLANK(C46),ISBLANK(D46)),"Completar",IF(D46&gt;=C46,D46-C46,"Error")),"Error")</f>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="7"/>
+      <c r="N46" s="7"/>
+      <c r="O46" s="7"/>
+      <c r="P46" s="13"/>
+      <c r="Q46" s="14"/>
+      <c r="R46" s="14"/>
+      <c r="S46" s="14"/>
+      <c r="T46" s="14"/>
+      <c r="U46" s="14"/>
+      <c r="V46" s="14"/>
+      <c r="W46" s="14"/>
+      <c r="X46" s="14"/>
+      <c r="Y46" s="14"/>
+      <c r="Z46" s="14"/>
+    </row>
+    <row r="47" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A47" s="15"/>
+      <c r="B47" s="54"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="18" t="str">
+        <f>IFERROR(IF(OR(ISBLANK(C47),ISBLANK(D47)),"Completar",IF(D47&gt;=C47,D47-C47,"Error")),"Error")</f>
         <v>Completar</v>
       </c>
-      <c r="F46" s="15"/>
-      <c r="G46" s="15"/>
-      <c r="H46" s="15"/>
-      <c r="I46" s="15"/>
-      <c r="J46" s="15"/>
-      <c r="K46" s="15"/>
-      <c r="L46" s="15"/>
-      <c r="M46" s="15"/>
-      <c r="N46" s="15"/>
-      <c r="O46" s="15"/>
-      <c r="P46" s="21"/>
-      <c r="Q46" s="22"/>
-      <c r="R46" s="22"/>
-      <c r="S46" s="22"/>
-      <c r="T46" s="22"/>
-      <c r="U46" s="22"/>
-      <c r="V46" s="22"/>
-      <c r="W46" s="22"/>
-      <c r="X46" s="22"/>
-      <c r="Y46" s="22"/>
-      <c r="Z46" s="22"/>
-    </row>
-    <row r="47" spans="1:26" ht="6" customHeight="1">
-      <c r="A47" s="20"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
-      <c r="I47" s="20"/>
-      <c r="J47" s="20"/>
-      <c r="K47" s="20"/>
-      <c r="L47" s="20"/>
-      <c r="M47" s="20"/>
-      <c r="N47" s="20"/>
-      <c r="O47" s="20"/>
-      <c r="P47" s="23"/>
-      <c r="Q47" s="23"/>
-      <c r="R47" s="23"/>
-      <c r="S47" s="23"/>
-      <c r="T47" s="23"/>
-      <c r="U47" s="23"/>
-      <c r="V47" s="23"/>
-      <c r="W47" s="23"/>
-      <c r="X47" s="23"/>
-      <c r="Y47" s="23"/>
-      <c r="Z47" s="23"/>
-    </row>
-    <row r="48" spans="1:26">
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="15"/>
+      <c r="K47" s="15"/>
+      <c r="L47" s="15"/>
+      <c r="M47" s="15"/>
+      <c r="N47" s="15"/>
+      <c r="O47" s="15"/>
+      <c r="P47" s="21"/>
+      <c r="Q47" s="22"/>
+      <c r="R47" s="22"/>
+      <c r="S47" s="22"/>
+      <c r="T47" s="22"/>
+      <c r="U47" s="22"/>
+      <c r="V47" s="22"/>
+      <c r="W47" s="22"/>
+      <c r="X47" s="22"/>
+      <c r="Y47" s="22"/>
+      <c r="Z47" s="22"/>
+    </row>
+    <row r="48" spans="1:26" ht="6" customHeight="1" thickBot="1">
       <c r="A48" s="20"/>
-      <c r="B48" s="112" t="s">
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="20"/>
+      <c r="I48" s="20"/>
+      <c r="J48" s="20"/>
+      <c r="K48" s="20"/>
+      <c r="L48" s="20"/>
+      <c r="M48" s="20"/>
+      <c r="N48" s="20"/>
+      <c r="O48" s="20"/>
+      <c r="P48" s="23"/>
+      <c r="Q48" s="23"/>
+      <c r="R48" s="23"/>
+      <c r="S48" s="23"/>
+      <c r="T48" s="23"/>
+      <c r="U48" s="23"/>
+      <c r="V48" s="23"/>
+      <c r="W48" s="23"/>
+      <c r="X48" s="23"/>
+      <c r="Y48" s="23"/>
+      <c r="Z48" s="23"/>
+    </row>
+    <row r="49" spans="1:26">
+      <c r="A49" s="20"/>
+      <c r="B49" s="114" t="s">
         <v>26</v>
       </c>
-      <c r="C48" s="113"/>
-      <c r="D48" s="113"/>
-      <c r="E48" s="113"/>
-      <c r="F48" s="113"/>
-      <c r="G48" s="113"/>
-      <c r="H48" s="113"/>
-      <c r="I48" s="113"/>
-      <c r="J48" s="113"/>
-      <c r="K48" s="113"/>
-      <c r="L48" s="113"/>
-      <c r="M48" s="113"/>
-      <c r="N48" s="114"/>
-      <c r="O48" s="20"/>
-      <c r="P48" s="55"/>
-      <c r="Q48" s="55"/>
-      <c r="R48" s="55"/>
-      <c r="S48" s="55"/>
-      <c r="T48" s="55"/>
-      <c r="U48" s="55"/>
-      <c r="V48" s="55"/>
-      <c r="W48" s="55"/>
-      <c r="X48" s="55"/>
-      <c r="Y48" s="55"/>
-      <c r="Z48" s="55"/>
-    </row>
-    <row r="49" spans="1:26" ht="15" customHeight="1">
-      <c r="A49" s="20"/>
-      <c r="B49" s="145" t="s">
-        <v>27</v>
-      </c>
-      <c r="C49" s="123"/>
-      <c r="D49" s="146"/>
-      <c r="E49" s="147">
-        <f>M42</f>
-        <v>439</v>
-      </c>
-      <c r="F49" s="146"/>
-      <c r="G49" s="56"/>
-      <c r="H49" s="57"/>
-      <c r="I49" s="57"/>
-      <c r="J49" s="57"/>
-      <c r="K49" s="57"/>
-      <c r="L49" s="57"/>
-      <c r="M49" s="57"/>
-      <c r="N49" s="58"/>
+      <c r="C49" s="161"/>
+      <c r="D49" s="161"/>
+      <c r="E49" s="161"/>
+      <c r="F49" s="161"/>
+      <c r="G49" s="161"/>
+      <c r="H49" s="161"/>
+      <c r="I49" s="161"/>
+      <c r="J49" s="161"/>
+      <c r="K49" s="161"/>
+      <c r="L49" s="161"/>
+      <c r="M49" s="161"/>
+      <c r="N49" s="162"/>
       <c r="O49" s="20"/>
       <c r="P49" s="55"/>
       <c r="Q49" s="55"/>
@@ -4208,26 +4283,26 @@
       <c r="Y49" s="55"/>
       <c r="Z49" s="55"/>
     </row>
-    <row r="50" spans="1:26">
+    <row r="50" spans="1:26" ht="15" customHeight="1">
       <c r="A50" s="20"/>
-      <c r="B50" s="145" t="s">
-        <v>28</v>
-      </c>
-      <c r="C50" s="123"/>
-      <c r="D50" s="146"/>
-      <c r="E50" s="157">
-        <f>IF(M42="Completar","Completar",IFERROR(M42/(N42*24),"Error"))</f>
-        <v>42.211538461538431</v>
-      </c>
-      <c r="F50" s="146"/>
-      <c r="G50" s="59"/>
-      <c r="H50" s="60"/>
-      <c r="I50" s="60"/>
-      <c r="J50" s="60"/>
-      <c r="K50" s="60"/>
-      <c r="L50" s="60"/>
-      <c r="M50" s="60"/>
-      <c r="N50" s="61"/>
+      <c r="B50" s="120" t="s">
+        <v>27</v>
+      </c>
+      <c r="C50" s="159"/>
+      <c r="D50" s="160"/>
+      <c r="E50" s="129">
+        <f>M43</f>
+        <v>457</v>
+      </c>
+      <c r="F50" s="122"/>
+      <c r="G50" s="56"/>
+      <c r="H50" s="57"/>
+      <c r="I50" s="57"/>
+      <c r="J50" s="57"/>
+      <c r="K50" s="57"/>
+      <c r="L50" s="57"/>
+      <c r="M50" s="57"/>
+      <c r="N50" s="58"/>
       <c r="O50" s="20"/>
       <c r="P50" s="55"/>
       <c r="Q50" s="55"/>
@@ -4241,18 +4316,18 @@
       <c r="Y50" s="55"/>
       <c r="Z50" s="55"/>
     </row>
-    <row r="51" spans="1:26" ht="15" customHeight="1">
+    <row r="51" spans="1:26">
       <c r="A51" s="20"/>
-      <c r="B51" s="145" t="s">
-        <v>29</v>
-      </c>
-      <c r="C51" s="123"/>
-      <c r="D51" s="146"/>
-      <c r="E51" s="147">
-        <f>IF(K42=0,0,IFERROR(ROUNDUP(K42/(M42/100),0),"Error"))</f>
-        <v>6</v>
-      </c>
-      <c r="F51" s="146"/>
+      <c r="B51" s="120" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" s="159"/>
+      <c r="D51" s="160"/>
+      <c r="E51" s="128">
+        <f>IF(M43="Completar","Completar",IFERROR(M43/(N43*24),"Error"))</f>
+        <v>41.798780487804848</v>
+      </c>
+      <c r="F51" s="122"/>
       <c r="G51" s="59"/>
       <c r="H51" s="60"/>
       <c r="I51" s="60"/>
@@ -4276,16 +4351,16 @@
     </row>
     <row r="52" spans="1:26" ht="15" customHeight="1">
       <c r="A52" s="20"/>
-      <c r="B52" s="145" t="s">
-        <v>30</v>
-      </c>
-      <c r="C52" s="123"/>
-      <c r="D52" s="146"/>
-      <c r="E52" s="156">
-        <f>IF(K42=0,0,IFERROR(K42/M42,"Error"))</f>
-        <v>5.6947608200455579E-2</v>
-      </c>
-      <c r="F52" s="146"/>
+      <c r="B52" s="120" t="s">
+        <v>29</v>
+      </c>
+      <c r="C52" s="159"/>
+      <c r="D52" s="160"/>
+      <c r="E52" s="129">
+        <f>IF(K43=0,0,IFERROR(ROUNDUP(K43/(M43/100),0),"Error"))</f>
+        <v>6</v>
+      </c>
+      <c r="F52" s="122"/>
       <c r="G52" s="59"/>
       <c r="H52" s="60"/>
       <c r="I52" s="60"/>
@@ -4309,19 +4384,16 @@
     </row>
     <row r="53" spans="1:26" ht="15" customHeight="1">
       <c r="A53" s="20"/>
-      <c r="B53" s="145" t="s">
-        <v>31</v>
-      </c>
-      <c r="C53" s="123"/>
-      <c r="D53" s="146"/>
-      <c r="E53" s="62">
-        <f>E5</f>
-        <v>6.9444444444444198E-3</v>
-      </c>
-      <c r="F53" s="63">
-        <f t="shared" ref="F53:F56" si="6">IF(E53="Completar",E53,IFERROR(E53/$E$59,"Error"))</f>
-        <v>1.5772870662460498E-2</v>
-      </c>
+      <c r="B53" s="120" t="s">
+        <v>30</v>
+      </c>
+      <c r="C53" s="159"/>
+      <c r="D53" s="160"/>
+      <c r="E53" s="127">
+        <f>IF(K43=0,0,IFERROR(K43/M43,"Error"))</f>
+        <v>5.4704595185995623E-2</v>
+      </c>
+      <c r="F53" s="122"/>
       <c r="G53" s="59"/>
       <c r="H53" s="60"/>
       <c r="I53" s="60"/>
@@ -4345,18 +4417,18 @@
     </row>
     <row r="54" spans="1:26" ht="15" customHeight="1">
       <c r="A54" s="20"/>
-      <c r="B54" s="145" t="s">
-        <v>32</v>
-      </c>
-      <c r="C54" s="123"/>
-      <c r="D54" s="146"/>
-      <c r="E54" s="62" t="str">
-        <f>E9</f>
-        <v>Completar</v>
-      </c>
-      <c r="F54" s="63" t="str">
-        <f t="shared" si="6"/>
-        <v>Completar</v>
+      <c r="B54" s="120" t="s">
+        <v>31</v>
+      </c>
+      <c r="C54" s="159"/>
+      <c r="D54" s="160"/>
+      <c r="E54" s="62">
+        <f>E5</f>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="F54" s="63">
+        <f t="shared" ref="F54:F57" si="5">IF(E54="Completar",E54,IFERROR(E54/$E$60,"Error"))</f>
+        <v>1.5015015015014951E-2</v>
       </c>
       <c r="G54" s="59"/>
       <c r="H54" s="60"/>
@@ -4381,17 +4453,17 @@
     </row>
     <row r="55" spans="1:26" ht="15" customHeight="1">
       <c r="A55" s="20"/>
-      <c r="B55" s="145" t="s">
-        <v>33</v>
-      </c>
-      <c r="C55" s="123"/>
-      <c r="D55" s="146"/>
+      <c r="B55" s="120" t="s">
+        <v>32</v>
+      </c>
+      <c r="C55" s="159"/>
+      <c r="D55" s="160"/>
       <c r="E55" s="62" t="str">
-        <f>E13</f>
+        <f>E9</f>
         <v>Completar</v>
       </c>
       <c r="F55" s="63" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>Completar</v>
       </c>
       <c r="G55" s="59"/>
@@ -4417,17 +4489,17 @@
     </row>
     <row r="56" spans="1:26" ht="15" customHeight="1">
       <c r="A56" s="20"/>
-      <c r="B56" s="145" t="s">
-        <v>34</v>
-      </c>
-      <c r="C56" s="123"/>
-      <c r="D56" s="146"/>
+      <c r="B56" s="120" t="s">
+        <v>33</v>
+      </c>
+      <c r="C56" s="159"/>
+      <c r="D56" s="160"/>
       <c r="E56" s="62" t="str">
-        <f>E46</f>
+        <f>E13</f>
         <v>Completar</v>
       </c>
       <c r="F56" s="63" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>Completar</v>
       </c>
       <c r="G56" s="59"/>
@@ -4453,18 +4525,18 @@
     </row>
     <row r="57" spans="1:26" ht="15" customHeight="1">
       <c r="A57" s="20"/>
-      <c r="B57" s="145" t="s">
-        <v>35</v>
-      </c>
-      <c r="C57" s="123"/>
-      <c r="D57" s="146"/>
-      <c r="E57" s="62">
-        <f>L42</f>
-        <v>7.4305555555555555E-2</v>
-      </c>
-      <c r="F57" s="63">
-        <f t="shared" ref="F57:F58" si="7">IF(E57="Completar",E57,IFERROR(E57/$E$59,"Completar"))</f>
-        <v>0.16876971608832794</v>
+      <c r="B57" s="120" t="s">
+        <v>34</v>
+      </c>
+      <c r="C57" s="159"/>
+      <c r="D57" s="160"/>
+      <c r="E57" s="62" t="str">
+        <f>E47</f>
+        <v>Completar</v>
+      </c>
+      <c r="F57" s="63" t="str">
+        <f t="shared" si="5"/>
+        <v>Completar</v>
       </c>
       <c r="G57" s="59"/>
       <c r="H57" s="60"/>
@@ -4489,18 +4561,18 @@
     </row>
     <row r="58" spans="1:26" ht="15" customHeight="1">
       <c r="A58" s="20"/>
-      <c r="B58" s="145" t="s">
-        <v>36</v>
-      </c>
-      <c r="C58" s="123"/>
-      <c r="D58" s="146"/>
+      <c r="B58" s="120" t="s">
+        <v>35</v>
+      </c>
+      <c r="C58" s="159"/>
+      <c r="D58" s="160"/>
       <c r="E58" s="62">
-        <f>J42</f>
-        <v>0.35902777777777817</v>
+        <f>L43</f>
+        <v>7.4305555555555555E-2</v>
       </c>
       <c r="F58" s="63">
-        <f t="shared" si="7"/>
-        <v>0.8154574132492115</v>
+        <f t="shared" ref="F58:F59" si="6">IF(E58="Completar",E58,IFERROR(E58/$E$60,"Completar"))</f>
+        <v>0.16066066066066054</v>
       </c>
       <c r="G58" s="59"/>
       <c r="H58" s="60"/>
@@ -4525,24 +4597,27 @@
     </row>
     <row r="59" spans="1:26" ht="15" customHeight="1">
       <c r="A59" s="20"/>
-      <c r="B59" s="153" t="s">
-        <v>37</v>
-      </c>
-      <c r="C59" s="116"/>
-      <c r="D59" s="152"/>
-      <c r="E59" s="151">
-        <f>IF(COUNTIF(E53:E58,"Error")&gt;0,"Error",IF(SUM(E53:E58)=0,"Completar",SUM(E53:E58)))</f>
-        <v>0.44027777777777816</v>
-      </c>
-      <c r="F59" s="152"/>
-      <c r="G59" s="64"/>
-      <c r="H59" s="65"/>
-      <c r="I59" s="65"/>
-      <c r="J59" s="65"/>
-      <c r="K59" s="65"/>
-      <c r="L59" s="65"/>
-      <c r="M59" s="65"/>
-      <c r="N59" s="66"/>
+      <c r="B59" s="120" t="s">
+        <v>36</v>
+      </c>
+      <c r="C59" s="159"/>
+      <c r="D59" s="160"/>
+      <c r="E59" s="62">
+        <f>J43</f>
+        <v>0.38125000000000037</v>
+      </c>
+      <c r="F59" s="63">
+        <f t="shared" si="6"/>
+        <v>0.82432432432432445</v>
+      </c>
+      <c r="G59" s="59"/>
+      <c r="H59" s="60"/>
+      <c r="I59" s="60"/>
+      <c r="J59" s="60"/>
+      <c r="K59" s="60"/>
+      <c r="L59" s="60"/>
+      <c r="M59" s="60"/>
+      <c r="N59" s="61"/>
       <c r="O59" s="20"/>
       <c r="P59" s="55"/>
       <c r="Q59" s="55"/>
@@ -4556,63 +4631,68 @@
       <c r="Y59" s="55"/>
       <c r="Z59" s="55"/>
     </row>
-    <row r="60" spans="1:26" ht="6" customHeight="1">
+    <row r="60" spans="1:26" ht="15" customHeight="1" thickBot="1">
       <c r="A60" s="20"/>
-      <c r="B60" s="20"/>
-      <c r="C60" s="20"/>
-      <c r="D60" s="20"/>
-      <c r="E60" s="20"/>
-      <c r="F60" s="20"/>
-      <c r="G60" s="20"/>
-      <c r="H60" s="20"/>
-      <c r="I60" s="20"/>
-      <c r="J60" s="20"/>
-      <c r="K60" s="20"/>
-      <c r="L60" s="20"/>
-      <c r="M60" s="20"/>
-      <c r="N60" s="20"/>
+      <c r="B60" s="125" t="s">
+        <v>37</v>
+      </c>
+      <c r="C60" s="157"/>
+      <c r="D60" s="158"/>
+      <c r="E60" s="123">
+        <f>IF(COUNTIF(E54:E59,"Error")&gt;0,"Error",IF(SUM(E54:E59)=0,"Completar",SUM(E54:E59)))</f>
+        <v>0.46250000000000036</v>
+      </c>
+      <c r="F60" s="124"/>
+      <c r="G60" s="64"/>
+      <c r="H60" s="65"/>
+      <c r="I60" s="65"/>
+      <c r="J60" s="65"/>
+      <c r="K60" s="65"/>
+      <c r="L60" s="65"/>
+      <c r="M60" s="65"/>
+      <c r="N60" s="66"/>
       <c r="O60" s="20"/>
-      <c r="P60" s="20"/>
-      <c r="Q60" s="20"/>
-      <c r="R60" s="20"/>
-      <c r="S60" s="20"/>
-      <c r="T60" s="20"/>
-      <c r="U60" s="20"/>
-      <c r="V60" s="20"/>
-      <c r="W60" s="20"/>
-      <c r="X60" s="20"/>
-      <c r="Y60" s="20"/>
-      <c r="Z60" s="20"/>
-    </row>
-    <row r="61" spans="1:26" hidden="1">
+      <c r="P60" s="55"/>
+      <c r="Q60" s="55"/>
+      <c r="R60" s="55"/>
+      <c r="S60" s="55"/>
+      <c r="T60" s="55"/>
+      <c r="U60" s="55"/>
+      <c r="V60" s="55"/>
+      <c r="W60" s="55"/>
+      <c r="X60" s="55"/>
+      <c r="Y60" s="55"/>
+      <c r="Z60" s="55"/>
+    </row>
+    <row r="61" spans="1:26" ht="6" customHeight="1">
       <c r="A61" s="20"/>
-      <c r="B61" s="55"/>
-      <c r="C61" s="55"/>
-      <c r="D61" s="55"/>
-      <c r="E61" s="55"/>
-      <c r="F61" s="55"/>
-      <c r="G61" s="55"/>
-      <c r="H61" s="55"/>
-      <c r="I61" s="55"/>
-      <c r="J61" s="55"/>
-      <c r="K61" s="55"/>
-      <c r="L61" s="55"/>
-      <c r="M61" s="55"/>
-      <c r="N61" s="55"/>
+      <c r="B61" s="20"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="20"/>
+      <c r="G61" s="20"/>
+      <c r="H61" s="20"/>
+      <c r="I61" s="20"/>
+      <c r="J61" s="20"/>
+      <c r="K61" s="20"/>
+      <c r="L61" s="20"/>
+      <c r="M61" s="20"/>
+      <c r="N61" s="20"/>
       <c r="O61" s="20"/>
-      <c r="P61" s="55"/>
-      <c r="Q61" s="55"/>
-      <c r="R61" s="55"/>
-      <c r="S61" s="55"/>
-      <c r="T61" s="55"/>
-      <c r="U61" s="55"/>
-      <c r="V61" s="55"/>
-      <c r="W61" s="55"/>
-      <c r="X61" s="55"/>
-      <c r="Y61" s="55"/>
-      <c r="Z61" s="55"/>
-    </row>
-    <row r="62" spans="1:26">
+      <c r="P61" s="20"/>
+      <c r="Q61" s="20"/>
+      <c r="R61" s="20"/>
+      <c r="S61" s="20"/>
+      <c r="T61" s="20"/>
+      <c r="U61" s="20"/>
+      <c r="V61" s="20"/>
+      <c r="W61" s="20"/>
+      <c r="X61" s="20"/>
+      <c r="Y61" s="20"/>
+      <c r="Z61" s="20"/>
+    </row>
+    <row r="62" spans="1:26" hidden="1">
       <c r="A62" s="20"/>
       <c r="B62" s="55"/>
       <c r="C62" s="55"/>
@@ -31352,37 +31432,58 @@
       <c r="Y1016" s="55"/>
       <c r="Z1016" s="55"/>
     </row>
+    <row r="1017" spans="1:26">
+      <c r="A1017" s="20"/>
+      <c r="B1017" s="55"/>
+      <c r="C1017" s="55"/>
+      <c r="D1017" s="55"/>
+      <c r="E1017" s="55"/>
+      <c r="F1017" s="55"/>
+      <c r="G1017" s="55"/>
+      <c r="H1017" s="55"/>
+      <c r="I1017" s="55"/>
+      <c r="J1017" s="55"/>
+      <c r="K1017" s="55"/>
+      <c r="L1017" s="55"/>
+      <c r="M1017" s="55"/>
+      <c r="N1017" s="55"/>
+      <c r="O1017" s="20"/>
+      <c r="P1017" s="55"/>
+      <c r="Q1017" s="55"/>
+      <c r="R1017" s="55"/>
+      <c r="S1017" s="55"/>
+      <c r="T1017" s="55"/>
+      <c r="U1017" s="55"/>
+      <c r="V1017" s="55"/>
+      <c r="W1017" s="55"/>
+      <c r="X1017" s="55"/>
+      <c r="Y1017" s="55"/>
+      <c r="Z1017" s="55"/>
+    </row>
   </sheetData>
-  <mergeCells count="60">
-    <mergeCell ref="D1:N1"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="F8:N8"/>
-    <mergeCell ref="F9:N9"/>
-    <mergeCell ref="B15:N15"/>
-    <mergeCell ref="F12:N12"/>
-    <mergeCell ref="F13:N13"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="C24:E24"/>
+  <mergeCells count="61">
     <mergeCell ref="C41:E41"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B48:N48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
     <mergeCell ref="N16:N17"/>
     <mergeCell ref="C21:E21"/>
     <mergeCell ref="C20:E20"/>
@@ -31393,105 +31494,123 @@
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="M16:M17"/>
     <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B49:N49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B15:N15"/>
+    <mergeCell ref="F12:N12"/>
+    <mergeCell ref="F13:N13"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="D1:N1"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F8:N8"/>
+    <mergeCell ref="F9:N9"/>
   </mergeCells>
-  <conditionalFormatting sqref="D1:XFD24 C3:C24 A42:XFD1048576 C29:I29 K29:M29 J41 C30:M30 C32:I35 J27:J29 A1:B41 J31:J39 N25:XFD41 K32:M36">
+  <conditionalFormatting sqref="D1:XFD24 C3:C24 K32:M36 C29:I29 K29:M29 C30:M30 C32:I35 J27:J29 J31:J39 C61:D1048576 O43:XFD1048576 E50:N1048576 F43:N48 C46:E48 C44:E44 J41:J42 N25:XFD42 A1:B1048576">
+    <cfRule type="cellIs" dxfId="23" priority="37" operator="equal">
+      <formula>"Completar"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:XFD24 C3:C24 K32:M36 C29:I29 K29:M29 C30:M30 C32:I35 J27:J29 J31:J39 C61:D1048576 O43:XFD1048576 E50:N1048576 F43:N48 C46:E48 C44:E44 J41:J42 N25:XFD42 A1:B1048576">
+    <cfRule type="cellIs" dxfId="22" priority="38" operator="equal">
+      <formula>"Error"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25:M25 C26:E26">
     <cfRule type="cellIs" dxfId="21" priority="35" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:XFD24 C3:C24 A42:XFD1048576 C29:I29 K29:M29 J41 C30:M30 C32:I35 J27:J29 A1:B41 J31:J39 N25:XFD41 K32:M36">
+  <conditionalFormatting sqref="C25:M25 C26:E26">
     <cfRule type="cellIs" dxfId="20" priority="36" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25:M25 C26:E26">
-    <cfRule type="cellIs" dxfId="19" priority="33" operator="equal">
+  <conditionalFormatting sqref="F26:M26 C42 F42:I42 K42:M42">
+    <cfRule type="cellIs" dxfId="19" priority="29" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25:M25 C26:E26">
-    <cfRule type="cellIs" dxfId="18" priority="34" operator="equal">
-      <formula>"Error"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F26:M26 C41 F41:I41 K41:M41">
-    <cfRule type="cellIs" dxfId="17" priority="27" operator="equal">
-      <formula>"Completar"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F26:M26 C41 F41:I41 K41:M41">
-    <cfRule type="cellIs" dxfId="16" priority="28" operator="equal">
+  <conditionalFormatting sqref="F26:M26 C42 F42:I42 K42:M42">
+    <cfRule type="cellIs" dxfId="18" priority="30" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:I27 K27:M27">
-    <cfRule type="cellIs" dxfId="15" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="25" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:I27 K27:M27">
-    <cfRule type="cellIs" dxfId="14" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="26" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:M31 C31 F31:I31">
-    <cfRule type="cellIs" dxfId="13" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="21" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:M31 C31 F31:I31">
-    <cfRule type="cellIs" dxfId="12" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="22" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28:M28 C28 F28:I28">
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28:M28 C28 F28:I28">
-    <cfRule type="cellIs" dxfId="10" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:M31 C31 F31:I31">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:M31 C31 F31:I31">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:I28 K28:M28">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:I28 K28:M28">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+      <formula>"Error"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41 F41:I41 K41:M41">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+      <formula>"Completar"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41 F41:I41 K41:M41">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Metricas y Diag.Clases MatrizMath
</commit_message>
<xml_diff>
--- a/Documentacion/MatrizMath/MatrizMath - Planilla de Métricas V2.1.xlsx
+++ b/Documentacion/MatrizMath/MatrizMath - Planilla de Métricas V2.1.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgIII\BranchGus\Documentacion\MatrizMath\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900"/>
   </bookViews>
   <sheets>
     <sheet name="Métricas" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -196,7 +201,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -1181,80 +1186,46 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1267,23 +1238,63 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1292,122 +1303,23 @@
     <xf numFmtId="49" fontId="6" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="165" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC00000"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC00000"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC00000"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <font>
         <color rgb="FFFFFFFF"/>
@@ -1701,9 +1613,18 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -1724,12 +1645,13 @@
           <c:order val="0"/>
           <c:dPt>
             <c:idx val="0"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="FFC000"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-49DD-4FD5-A2AE-26863999DE8F}"/>
               </c:ext>
@@ -1737,12 +1659,13 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="00B0F0"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-49DD-4FD5-A2AE-26863999DE8F}"/>
               </c:ext>
@@ -1750,12 +1673,13 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="0066FF"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-49DD-4FD5-A2AE-26863999DE8F}"/>
               </c:ext>
@@ -1763,12 +1687,13 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="009900"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-49DD-4FD5-A2AE-26863999DE8F}"/>
               </c:ext>
@@ -1776,12 +1701,13 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000009-49DD-4FD5-A2AE-26863999DE8F}"/>
               </c:ext>
@@ -1789,12 +1715,13 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="002060"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000B-49DD-4FD5-A2AE-26863999DE8F}"/>
               </c:ext>
@@ -1828,19 +1755,46 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Métricas!$C$54:$C$59</c:f>
+              <c:f>Métricas!$F$54:$F$59</c:f>
               <c:numCache>
-                <c:formatCode>@</c:formatCode>
+                <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.3157894736842051E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2894736842105338E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4999999999999894E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.5789473684210564E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14078947368421044</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.72236842105263177</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000C-49DD-4FD5-A2AE-26863999DE8F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
       <c:spPr>
@@ -1852,6 +1806,7 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
@@ -2155,21 +2110,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1017"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42:E42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
@@ -2185,23 +2140,23 @@
   <sheetData>
     <row r="1" spans="1:26" ht="23.25" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="117" t="s">
+      <c r="B1" s="164" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="113"/>
-      <c r="D1" s="112" t="s">
+      <c r="C1" s="154"/>
+      <c r="D1" s="163" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
-      <c r="M1" s="113"/>
-      <c r="N1" s="113"/>
+      <c r="E1" s="154"/>
+      <c r="F1" s="154"/>
+      <c r="G1" s="154"/>
+      <c r="H1" s="154"/>
+      <c r="I1" s="154"/>
+      <c r="J1" s="154"/>
+      <c r="K1" s="154"/>
+      <c r="L1" s="154"/>
+      <c r="M1" s="154"/>
+      <c r="N1" s="154"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -2245,12 +2200,12 @@
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
       <c r="A3" s="4"/>
-      <c r="B3" s="114" t="s">
+      <c r="B3" s="115" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="116"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
+      <c r="E3" s="152"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -2376,12 +2331,12 @@
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1">
       <c r="A7" s="4"/>
-      <c r="B7" s="114" t="s">
+      <c r="B7" s="115" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="115"/>
-      <c r="D7" s="115"/>
-      <c r="E7" s="116"/>
+      <c r="C7" s="151"/>
+      <c r="D7" s="151"/>
+      <c r="E7" s="152"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -2418,15 +2373,15 @@
       <c r="E8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="118"/>
-      <c r="G8" s="113"/>
-      <c r="H8" s="113"/>
-      <c r="I8" s="113"/>
-      <c r="J8" s="113"/>
-      <c r="K8" s="113"/>
-      <c r="L8" s="113"/>
-      <c r="M8" s="113"/>
-      <c r="N8" s="113"/>
+      <c r="F8" s="153"/>
+      <c r="G8" s="154"/>
+      <c r="H8" s="154"/>
+      <c r="I8" s="154"/>
+      <c r="J8" s="154"/>
+      <c r="K8" s="154"/>
+      <c r="L8" s="154"/>
+      <c r="M8" s="154"/>
+      <c r="N8" s="154"/>
       <c r="O8" s="7"/>
       <c r="P8" s="13"/>
       <c r="Q8" s="14"/>
@@ -2448,20 +2403,22 @@
       <c r="C9" s="17">
         <v>0.63263888888888886</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="18" t="str">
+      <c r="D9" s="25">
+        <v>0.65</v>
+      </c>
+      <c r="E9" s="18">
         <f>IFERROR(IF(OR(ISBLANK(C9),ISBLANK(D9)),"Completar",IF(D9&gt;=C9,D9-C9,"Error")),"Error")</f>
-        <v>Completar</v>
-      </c>
-      <c r="F9" s="119"/>
-      <c r="G9" s="113"/>
-      <c r="H9" s="113"/>
-      <c r="I9" s="113"/>
-      <c r="J9" s="113"/>
-      <c r="K9" s="113"/>
-      <c r="L9" s="113"/>
-      <c r="M9" s="113"/>
-      <c r="N9" s="113"/>
+        <v>1.736111111111116E-2</v>
+      </c>
+      <c r="F9" s="155"/>
+      <c r="G9" s="154"/>
+      <c r="H9" s="154"/>
+      <c r="I9" s="154"/>
+      <c r="J9" s="154"/>
+      <c r="K9" s="154"/>
+      <c r="L9" s="154"/>
+      <c r="M9" s="154"/>
+      <c r="N9" s="154"/>
       <c r="O9" s="15"/>
       <c r="P9" s="21"/>
       <c r="Q9" s="22"/>
@@ -2505,12 +2462,12 @@
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" s="4"/>
-      <c r="B11" s="114" t="s">
+      <c r="B11" s="115" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="115"/>
-      <c r="D11" s="115"/>
-      <c r="E11" s="116"/>
+      <c r="C11" s="151"/>
+      <c r="D11" s="151"/>
+      <c r="E11" s="152"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -2547,15 +2504,15 @@
       <c r="E12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="118"/>
-      <c r="G12" s="113"/>
-      <c r="H12" s="113"/>
-      <c r="I12" s="113"/>
-      <c r="J12" s="113"/>
-      <c r="K12" s="113"/>
-      <c r="L12" s="113"/>
-      <c r="M12" s="113"/>
-      <c r="N12" s="113"/>
+      <c r="F12" s="153"/>
+      <c r="G12" s="154"/>
+      <c r="H12" s="154"/>
+      <c r="I12" s="154"/>
+      <c r="J12" s="154"/>
+      <c r="K12" s="154"/>
+      <c r="L12" s="154"/>
+      <c r="M12" s="154"/>
+      <c r="N12" s="154"/>
       <c r="O12" s="7"/>
       <c r="P12" s="13"/>
       <c r="Q12" s="14"/>
@@ -2574,21 +2531,25 @@
       <c r="B13" s="16">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="18" t="str">
+      <c r="C13" s="25">
+        <v>0.65069444444444446</v>
+      </c>
+      <c r="D13" s="25">
+        <v>0.66388888888888886</v>
+      </c>
+      <c r="E13" s="18">
         <f>IFERROR(IF(OR(ISBLANK(C13),ISBLANK(D13)),"Completar",IF(D13&gt;=C13,D13-C13,"Error")),"Error")</f>
-        <v>Completar</v>
-      </c>
-      <c r="F13" s="119"/>
-      <c r="G13" s="113"/>
-      <c r="H13" s="113"/>
-      <c r="I13" s="113"/>
-      <c r="J13" s="113"/>
-      <c r="K13" s="113"/>
-      <c r="L13" s="113"/>
-      <c r="M13" s="113"/>
-      <c r="N13" s="113"/>
+        <v>1.3194444444444398E-2</v>
+      </c>
+      <c r="F13" s="155"/>
+      <c r="G13" s="154"/>
+      <c r="H13" s="154"/>
+      <c r="I13" s="154"/>
+      <c r="J13" s="154"/>
+      <c r="K13" s="154"/>
+      <c r="L13" s="154"/>
+      <c r="M13" s="154"/>
+      <c r="N13" s="154"/>
       <c r="O13" s="15"/>
       <c r="P13" s="21"/>
       <c r="Q13" s="22"/>
@@ -2632,21 +2593,21 @@
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1">
       <c r="A15" s="4"/>
-      <c r="B15" s="114" t="s">
+      <c r="B15" s="115" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="115"/>
-      <c r="D15" s="115"/>
-      <c r="E15" s="115"/>
-      <c r="F15" s="115"/>
-      <c r="G15" s="115"/>
-      <c r="H15" s="115"/>
-      <c r="I15" s="115"/>
-      <c r="J15" s="115"/>
-      <c r="K15" s="115"/>
-      <c r="L15" s="115"/>
-      <c r="M15" s="115"/>
-      <c r="N15" s="116"/>
+      <c r="C15" s="151"/>
+      <c r="D15" s="151"/>
+      <c r="E15" s="151"/>
+      <c r="F15" s="151"/>
+      <c r="G15" s="151"/>
+      <c r="H15" s="151"/>
+      <c r="I15" s="151"/>
+      <c r="J15" s="151"/>
+      <c r="K15" s="151"/>
+      <c r="L15" s="151"/>
+      <c r="M15" s="151"/>
+      <c r="N15" s="152"/>
       <c r="O15" s="4"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
@@ -2662,31 +2623,31 @@
     </row>
     <row r="16" spans="1:26" ht="16.5" customHeight="1">
       <c r="A16" s="7"/>
-      <c r="B16" s="140" t="s">
+      <c r="B16" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="142" t="s">
+      <c r="C16" s="134" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="143"/>
-      <c r="E16" s="143"/>
-      <c r="F16" s="136" t="s">
+      <c r="D16" s="135"/>
+      <c r="E16" s="135"/>
+      <c r="F16" s="142" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="137"/>
-      <c r="H16" s="135" t="s">
+      <c r="G16" s="143"/>
+      <c r="H16" s="141" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="121"/>
-      <c r="J16" s="121"/>
-      <c r="K16" s="136" t="s">
+      <c r="I16" s="124"/>
+      <c r="J16" s="124"/>
+      <c r="K16" s="142" t="s">
         <v>14</v>
       </c>
-      <c r="L16" s="137"/>
-      <c r="M16" s="138" t="s">
+      <c r="L16" s="143"/>
+      <c r="M16" s="144" t="s">
         <v>15</v>
       </c>
-      <c r="N16" s="130" t="s">
+      <c r="N16" s="139" t="s">
         <v>6</v>
       </c>
       <c r="O16" s="7"/>
@@ -2704,10 +2665,10 @@
     </row>
     <row r="17" spans="1:26" ht="30" customHeight="1">
       <c r="A17" s="7"/>
-      <c r="B17" s="141"/>
-      <c r="C17" s="144"/>
-      <c r="D17" s="145"/>
-      <c r="E17" s="145"/>
+      <c r="B17" s="133"/>
+      <c r="C17" s="136"/>
+      <c r="D17" s="137"/>
+      <c r="E17" s="137"/>
       <c r="F17" s="26" t="s">
         <v>16</v>
       </c>
@@ -2729,8 +2690,8 @@
       <c r="L17" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="M17" s="139"/>
-      <c r="N17" s="131"/>
+      <c r="M17" s="145"/>
+      <c r="N17" s="140"/>
       <c r="O17" s="7"/>
       <c r="P17" s="13"/>
       <c r="Q17" s="14"/>
@@ -2750,11 +2711,11 @@
         <f t="shared" ref="B18:B40" si="0">ROW($B18)-16</f>
         <v>2</v>
       </c>
-      <c r="C18" s="132" t="s">
+      <c r="C18" s="138" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="121"/>
-      <c r="E18" s="121"/>
+      <c r="D18" s="124"/>
+      <c r="E18" s="124"/>
       <c r="F18" s="31">
         <v>60</v>
       </c>
@@ -2803,11 +2764,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C19" s="132" t="s">
+      <c r="C19" s="138" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="121"/>
-      <c r="E19" s="121"/>
+      <c r="D19" s="124"/>
+      <c r="E19" s="124"/>
       <c r="F19" s="31">
         <v>4</v>
       </c>
@@ -2856,11 +2817,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C20" s="132" t="s">
+      <c r="C20" s="138" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="121"/>
-      <c r="E20" s="121"/>
+      <c r="D20" s="124"/>
+      <c r="E20" s="124"/>
       <c r="F20" s="31">
         <v>8</v>
       </c>
@@ -2909,11 +2870,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C21" s="132" t="s">
+      <c r="C21" s="138" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="121"/>
-      <c r="E21" s="121"/>
+      <c r="D21" s="124"/>
+      <c r="E21" s="124"/>
       <c r="F21" s="31">
         <v>10</v>
       </c>
@@ -2962,11 +2923,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C22" s="133" t="s">
+      <c r="C22" s="125" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="134"/>
-      <c r="E22" s="134"/>
+      <c r="D22" s="130"/>
+      <c r="E22" s="130"/>
       <c r="F22" s="70">
         <v>8</v>
       </c>
@@ -3015,11 +2976,11 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C23" s="126" t="s">
+      <c r="C23" s="121" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="121"/>
-      <c r="E23" s="121"/>
+      <c r="D23" s="124"/>
+      <c r="E23" s="124"/>
       <c r="F23" s="40">
         <v>13</v>
       </c>
@@ -3068,11 +3029,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C24" s="126" t="s">
+      <c r="C24" s="121" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="121"/>
-      <c r="E24" s="121"/>
+      <c r="D24" s="124"/>
+      <c r="E24" s="124"/>
       <c r="F24" s="40">
         <v>25</v>
       </c>
@@ -3121,11 +3082,11 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C25" s="126" t="s">
+      <c r="C25" s="121" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="121"/>
-      <c r="E25" s="121"/>
+      <c r="D25" s="124"/>
+      <c r="E25" s="124"/>
       <c r="F25" s="40">
         <v>20</v>
       </c>
@@ -3174,11 +3135,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C26" s="126" t="s">
+      <c r="C26" s="121" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="121"/>
-      <c r="E26" s="121"/>
+      <c r="D26" s="124"/>
+      <c r="E26" s="124"/>
       <c r="F26" s="40">
         <v>16</v>
       </c>
@@ -3227,11 +3188,11 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C27" s="126" t="s">
+      <c r="C27" s="121" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="121"/>
-      <c r="E27" s="121"/>
+      <c r="D27" s="124"/>
+      <c r="E27" s="124"/>
       <c r="F27" s="40">
         <v>30</v>
       </c>
@@ -3280,11 +3241,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C28" s="126" t="s">
+      <c r="C28" s="121" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="151"/>
-      <c r="E28" s="152"/>
+      <c r="D28" s="122"/>
+      <c r="E28" s="123"/>
       <c r="F28" s="82">
         <v>30</v>
       </c>
@@ -3333,11 +3294,11 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C29" s="126" t="s">
+      <c r="C29" s="121" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="151"/>
-      <c r="E29" s="152"/>
+      <c r="D29" s="122"/>
+      <c r="E29" s="123"/>
       <c r="F29" s="82">
         <v>15</v>
       </c>
@@ -3386,11 +3347,11 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C30" s="126" t="s">
+      <c r="C30" s="121" t="s">
         <v>51</v>
       </c>
-      <c r="D30" s="151"/>
-      <c r="E30" s="152"/>
+      <c r="D30" s="122"/>
+      <c r="E30" s="123"/>
       <c r="F30" s="82">
         <v>25</v>
       </c>
@@ -3439,11 +3400,11 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C31" s="126" t="s">
+      <c r="C31" s="121" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="151"/>
-      <c r="E31" s="152"/>
+      <c r="D31" s="122"/>
+      <c r="E31" s="123"/>
       <c r="F31" s="82">
         <v>18</v>
       </c>
@@ -3492,11 +3453,11 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C32" s="126" t="s">
+      <c r="C32" s="121" t="s">
         <v>47</v>
       </c>
-      <c r="D32" s="151"/>
-      <c r="E32" s="152"/>
+      <c r="D32" s="122"/>
+      <c r="E32" s="123"/>
       <c r="F32" s="82">
         <v>17</v>
       </c>
@@ -3545,11 +3506,11 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C33" s="133" t="s">
+      <c r="C33" s="125" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="146"/>
-      <c r="E33" s="147"/>
+      <c r="D33" s="126"/>
+      <c r="E33" s="127"/>
       <c r="F33" s="91">
         <v>20</v>
       </c>
@@ -3598,11 +3559,11 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C34" s="133" t="s">
+      <c r="C34" s="125" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="146"/>
-      <c r="E34" s="147"/>
+      <c r="D34" s="126"/>
+      <c r="E34" s="127"/>
       <c r="F34" s="91">
         <v>18</v>
       </c>
@@ -3651,11 +3612,11 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C35" s="133" t="s">
+      <c r="C35" s="125" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="134"/>
-      <c r="E35" s="150"/>
+      <c r="D35" s="130"/>
+      <c r="E35" s="131"/>
       <c r="F35" s="91">
         <v>20</v>
       </c>
@@ -3704,11 +3665,11 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C36" s="154" t="s">
+      <c r="C36" s="112" t="s">
         <v>54</v>
       </c>
-      <c r="D36" s="155"/>
-      <c r="E36" s="156"/>
+      <c r="D36" s="113"/>
+      <c r="E36" s="114"/>
       <c r="F36" s="105">
         <v>20</v>
       </c>
@@ -3757,11 +3718,11 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C37" s="154" t="s">
+      <c r="C37" s="112" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="155"/>
-      <c r="E37" s="156"/>
+      <c r="D37" s="113"/>
+      <c r="E37" s="114"/>
       <c r="F37" s="105">
         <v>20</v>
       </c>
@@ -3810,11 +3771,11 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C38" s="148" t="s">
+      <c r="C38" s="128" t="s">
         <v>53</v>
       </c>
-      <c r="D38" s="148"/>
-      <c r="E38" s="149"/>
+      <c r="D38" s="128"/>
+      <c r="E38" s="129"/>
       <c r="F38" s="105">
         <v>25</v>
       </c>
@@ -3863,11 +3824,11 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="C39" s="148" t="s">
+      <c r="C39" s="128" t="s">
         <v>56</v>
       </c>
-      <c r="D39" s="148"/>
-      <c r="E39" s="149"/>
+      <c r="D39" s="128"/>
+      <c r="E39" s="129"/>
       <c r="F39" s="105">
         <v>25</v>
       </c>
@@ -3916,11 +3877,11 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C40" s="154" t="s">
+      <c r="C40" s="112" t="s">
         <v>57</v>
       </c>
-      <c r="D40" s="155"/>
-      <c r="E40" s="156"/>
+      <c r="D40" s="113"/>
+      <c r="E40" s="114"/>
       <c r="F40" s="105">
         <v>25</v>
       </c>
@@ -3968,11 +3929,11 @@
       <c r="B41" s="30">
         <v>25</v>
       </c>
-      <c r="C41" s="154" t="s">
+      <c r="C41" s="112" t="s">
         <v>58</v>
       </c>
-      <c r="D41" s="155"/>
-      <c r="E41" s="156"/>
+      <c r="D41" s="113"/>
+      <c r="E41" s="114"/>
       <c r="F41" s="105">
         <v>20</v>
       </c>
@@ -4020,9 +3981,9 @@
       <c r="B42" s="30">
         <v>26</v>
       </c>
-      <c r="C42" s="154"/>
-      <c r="D42" s="155"/>
-      <c r="E42" s="156"/>
+      <c r="C42" s="112"/>
+      <c r="D42" s="113"/>
+      <c r="E42" s="114"/>
       <c r="F42" s="105"/>
       <c r="G42" s="106"/>
       <c r="H42" s="103"/>
@@ -4047,12 +4008,12 @@
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A43" s="7"/>
-      <c r="B43" s="153" t="s">
+      <c r="B43" s="118" t="s">
         <v>23</v>
       </c>
-      <c r="C43" s="163"/>
-      <c r="D43" s="163"/>
-      <c r="E43" s="164"/>
+      <c r="C43" s="119"/>
+      <c r="D43" s="119"/>
+      <c r="E43" s="120"/>
       <c r="F43" s="46">
         <f>IF(SUM(F18:F42)=0,"Completar",SUM(F18:F42))</f>
         <v>492</v>
@@ -4130,12 +4091,12 @@
     </row>
     <row r="45" spans="1:26" ht="15" customHeight="1">
       <c r="A45" s="4"/>
-      <c r="B45" s="114" t="s">
+      <c r="B45" s="115" t="s">
         <v>25</v>
       </c>
-      <c r="C45" s="161"/>
-      <c r="D45" s="161"/>
-      <c r="E45" s="162"/>
+      <c r="C45" s="116"/>
+      <c r="D45" s="116"/>
+      <c r="E45" s="117"/>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
@@ -4196,12 +4157,18 @@
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A47" s="15"/>
-      <c r="B47" s="54"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="18" t="str">
+      <c r="B47" s="54">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="C47" s="25">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D47" s="25">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="E47" s="18">
         <f>IFERROR(IF(OR(ISBLANK(C47),ISBLANK(D47)),"Completar",IF(D47&gt;=C47,D47-C47,"Error")),"Error")</f>
-        <v>Completar</v>
+        <v>3.4722222222222265E-2</v>
       </c>
       <c r="F47" s="15"/>
       <c r="G47" s="15"/>
@@ -4255,21 +4222,21 @@
     </row>
     <row r="49" spans="1:26">
       <c r="A49" s="20"/>
-      <c r="B49" s="114" t="s">
+      <c r="B49" s="115" t="s">
         <v>26</v>
       </c>
-      <c r="C49" s="161"/>
-      <c r="D49" s="161"/>
-      <c r="E49" s="161"/>
-      <c r="F49" s="161"/>
-      <c r="G49" s="161"/>
-      <c r="H49" s="161"/>
-      <c r="I49" s="161"/>
-      <c r="J49" s="161"/>
-      <c r="K49" s="161"/>
-      <c r="L49" s="161"/>
-      <c r="M49" s="161"/>
-      <c r="N49" s="162"/>
+      <c r="C49" s="116"/>
+      <c r="D49" s="116"/>
+      <c r="E49" s="116"/>
+      <c r="F49" s="116"/>
+      <c r="G49" s="116"/>
+      <c r="H49" s="116"/>
+      <c r="I49" s="116"/>
+      <c r="J49" s="116"/>
+      <c r="K49" s="116"/>
+      <c r="L49" s="116"/>
+      <c r="M49" s="116"/>
+      <c r="N49" s="117"/>
       <c r="O49" s="20"/>
       <c r="P49" s="55"/>
       <c r="Q49" s="55"/>
@@ -4285,16 +4252,16 @@
     </row>
     <row r="50" spans="1:26" ht="15" customHeight="1">
       <c r="A50" s="20"/>
-      <c r="B50" s="120" t="s">
+      <c r="B50" s="146" t="s">
         <v>27</v>
       </c>
-      <c r="C50" s="159"/>
-      <c r="D50" s="160"/>
-      <c r="E50" s="129">
+      <c r="C50" s="147"/>
+      <c r="D50" s="148"/>
+      <c r="E50" s="149">
         <f>M43</f>
         <v>457</v>
       </c>
-      <c r="F50" s="122"/>
+      <c r="F50" s="150"/>
       <c r="G50" s="56"/>
       <c r="H50" s="57"/>
       <c r="I50" s="57"/>
@@ -4318,16 +4285,16 @@
     </row>
     <row r="51" spans="1:26">
       <c r="A51" s="20"/>
-      <c r="B51" s="120" t="s">
+      <c r="B51" s="146" t="s">
         <v>28</v>
       </c>
-      <c r="C51" s="159"/>
-      <c r="D51" s="160"/>
-      <c r="E51" s="128">
+      <c r="C51" s="147"/>
+      <c r="D51" s="148"/>
+      <c r="E51" s="162">
         <f>IF(M43="Completar","Completar",IFERROR(M43/(N43*24),"Error"))</f>
         <v>41.798780487804848</v>
       </c>
-      <c r="F51" s="122"/>
+      <c r="F51" s="150"/>
       <c r="G51" s="59"/>
       <c r="H51" s="60"/>
       <c r="I51" s="60"/>
@@ -4351,16 +4318,16 @@
     </row>
     <row r="52" spans="1:26" ht="15" customHeight="1">
       <c r="A52" s="20"/>
-      <c r="B52" s="120" t="s">
+      <c r="B52" s="146" t="s">
         <v>29</v>
       </c>
-      <c r="C52" s="159"/>
-      <c r="D52" s="160"/>
-      <c r="E52" s="129">
+      <c r="C52" s="147"/>
+      <c r="D52" s="148"/>
+      <c r="E52" s="149">
         <f>IF(K43=0,0,IFERROR(ROUNDUP(K43/(M43/100),0),"Error"))</f>
         <v>6</v>
       </c>
-      <c r="F52" s="122"/>
+      <c r="F52" s="150"/>
       <c r="G52" s="59"/>
       <c r="H52" s="60"/>
       <c r="I52" s="60"/>
@@ -4384,16 +4351,16 @@
     </row>
     <row r="53" spans="1:26" ht="15" customHeight="1">
       <c r="A53" s="20"/>
-      <c r="B53" s="120" t="s">
+      <c r="B53" s="146" t="s">
         <v>30</v>
       </c>
-      <c r="C53" s="159"/>
-      <c r="D53" s="160"/>
-      <c r="E53" s="127">
+      <c r="C53" s="147"/>
+      <c r="D53" s="148"/>
+      <c r="E53" s="161">
         <f>IF(K43=0,0,IFERROR(K43/M43,"Error"))</f>
         <v>5.4704595185995623E-2</v>
       </c>
-      <c r="F53" s="122"/>
+      <c r="F53" s="150"/>
       <c r="G53" s="59"/>
       <c r="H53" s="60"/>
       <c r="I53" s="60"/>
@@ -4417,18 +4384,18 @@
     </row>
     <row r="54" spans="1:26" ht="15" customHeight="1">
       <c r="A54" s="20"/>
-      <c r="B54" s="120" t="s">
+      <c r="B54" s="146" t="s">
         <v>31</v>
       </c>
-      <c r="C54" s="159"/>
-      <c r="D54" s="160"/>
+      <c r="C54" s="147"/>
+      <c r="D54" s="148"/>
       <c r="E54" s="62">
         <f>E5</f>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="F54" s="63">
         <f t="shared" ref="F54:F57" si="5">IF(E54="Completar",E54,IFERROR(E54/$E$60,"Error"))</f>
-        <v>1.5015015015014951E-2</v>
+        <v>1.3157894736842051E-2</v>
       </c>
       <c r="G54" s="59"/>
       <c r="H54" s="60"/>
@@ -4453,18 +4420,18 @@
     </row>
     <row r="55" spans="1:26" ht="15" customHeight="1">
       <c r="A55" s="20"/>
-      <c r="B55" s="120" t="s">
+      <c r="B55" s="146" t="s">
         <v>32</v>
       </c>
-      <c r="C55" s="159"/>
-      <c r="D55" s="160"/>
-      <c r="E55" s="62" t="str">
+      <c r="C55" s="147"/>
+      <c r="D55" s="148"/>
+      <c r="E55" s="62">
         <f>E9</f>
-        <v>Completar</v>
-      </c>
-      <c r="F55" s="63" t="str">
+        <v>1.736111111111116E-2</v>
+      </c>
+      <c r="F55" s="63">
         <f t="shared" si="5"/>
-        <v>Completar</v>
+        <v>3.2894736842105338E-2</v>
       </c>
       <c r="G55" s="59"/>
       <c r="H55" s="60"/>
@@ -4489,18 +4456,18 @@
     </row>
     <row r="56" spans="1:26" ht="15" customHeight="1">
       <c r="A56" s="20"/>
-      <c r="B56" s="120" t="s">
+      <c r="B56" s="146" t="s">
         <v>33</v>
       </c>
-      <c r="C56" s="159"/>
-      <c r="D56" s="160"/>
-      <c r="E56" s="62" t="str">
+      <c r="C56" s="147"/>
+      <c r="D56" s="148"/>
+      <c r="E56" s="62">
         <f>E13</f>
-        <v>Completar</v>
-      </c>
-      <c r="F56" s="63" t="str">
+        <v>1.3194444444444398E-2</v>
+      </c>
+      <c r="F56" s="63">
         <f t="shared" si="5"/>
-        <v>Completar</v>
+        <v>2.4999999999999894E-2</v>
       </c>
       <c r="G56" s="59"/>
       <c r="H56" s="60"/>
@@ -4525,18 +4492,18 @@
     </row>
     <row r="57" spans="1:26" ht="15" customHeight="1">
       <c r="A57" s="20"/>
-      <c r="B57" s="120" t="s">
+      <c r="B57" s="146" t="s">
         <v>34</v>
       </c>
-      <c r="C57" s="159"/>
-      <c r="D57" s="160"/>
-      <c r="E57" s="62" t="str">
+      <c r="C57" s="147"/>
+      <c r="D57" s="148"/>
+      <c r="E57" s="62">
         <f>E47</f>
-        <v>Completar</v>
-      </c>
-      <c r="F57" s="63" t="str">
+        <v>3.4722222222222265E-2</v>
+      </c>
+      <c r="F57" s="63">
         <f t="shared" si="5"/>
-        <v>Completar</v>
+        <v>6.5789473684210564E-2</v>
       </c>
       <c r="G57" s="59"/>
       <c r="H57" s="60"/>
@@ -4561,18 +4528,18 @@
     </row>
     <row r="58" spans="1:26" ht="15" customHeight="1">
       <c r="A58" s="20"/>
-      <c r="B58" s="120" t="s">
+      <c r="B58" s="146" t="s">
         <v>35</v>
       </c>
-      <c r="C58" s="159"/>
-      <c r="D58" s="160"/>
+      <c r="C58" s="147"/>
+      <c r="D58" s="148"/>
       <c r="E58" s="62">
         <f>L43</f>
         <v>7.4305555555555555E-2</v>
       </c>
       <c r="F58" s="63">
         <f t="shared" ref="F58:F59" si="6">IF(E58="Completar",E58,IFERROR(E58/$E$60,"Completar"))</f>
-        <v>0.16066066066066054</v>
+        <v>0.14078947368421044</v>
       </c>
       <c r="G58" s="59"/>
       <c r="H58" s="60"/>
@@ -4597,18 +4564,18 @@
     </row>
     <row r="59" spans="1:26" ht="15" customHeight="1">
       <c r="A59" s="20"/>
-      <c r="B59" s="120" t="s">
+      <c r="B59" s="146" t="s">
         <v>36</v>
       </c>
-      <c r="C59" s="159"/>
-      <c r="D59" s="160"/>
+      <c r="C59" s="147"/>
+      <c r="D59" s="148"/>
       <c r="E59" s="62">
         <f>J43</f>
         <v>0.38125000000000037</v>
       </c>
       <c r="F59" s="63">
         <f t="shared" si="6"/>
-        <v>0.82432432432432445</v>
+        <v>0.72236842105263177</v>
       </c>
       <c r="G59" s="59"/>
       <c r="H59" s="60"/>
@@ -4633,16 +4600,16 @@
     </row>
     <row r="60" spans="1:26" ht="15" customHeight="1" thickBot="1">
       <c r="A60" s="20"/>
-      <c r="B60" s="125" t="s">
+      <c r="B60" s="158" t="s">
         <v>37</v>
       </c>
-      <c r="C60" s="157"/>
-      <c r="D60" s="158"/>
-      <c r="E60" s="123">
+      <c r="C60" s="159"/>
+      <c r="D60" s="160"/>
+      <c r="E60" s="156">
         <f>IF(COUNTIF(E54:E59,"Error")&gt;0,"Error",IF(SUM(E54:E59)=0,"Completar",SUM(E54:E59)))</f>
-        <v>0.46250000000000036</v>
-      </c>
-      <c r="F60" s="124"/>
+        <v>0.52777777777777812</v>
+      </c>
+      <c r="F60" s="157"/>
       <c r="G60" s="64"/>
       <c r="H60" s="65"/>
       <c r="I60" s="65"/>
@@ -31462,44 +31429,13 @@
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B49:N49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="D1:N1"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F8:N8"/>
+    <mergeCell ref="F9:N9"/>
     <mergeCell ref="B15:N15"/>
     <mergeCell ref="F12:N12"/>
     <mergeCell ref="F13:N13"/>
@@ -31516,101 +31452,132 @@
     <mergeCell ref="E53:F53"/>
     <mergeCell ref="B53:D53"/>
     <mergeCell ref="E51:F51"/>
-    <mergeCell ref="D1:N1"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="F8:N8"/>
-    <mergeCell ref="F9:N9"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B49:N49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C40:E40"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:XFD24 C3:C24 K32:M36 C29:I29 K29:M29 C30:M30 C32:I35 J27:J29 J31:J39 C61:D1048576 O43:XFD1048576 E50:N1048576 F43:N48 C46:E48 C44:E44 J41:J42 N25:XFD42 A1:B1048576">
-    <cfRule type="cellIs" dxfId="23" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="37" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:XFD24 C3:C24 K32:M36 C29:I29 K29:M29 C30:M30 C32:I35 J27:J29 J31:J39 C61:D1048576 O43:XFD1048576 E50:N1048576 F43:N48 C46:E48 C44:E44 J41:J42 N25:XFD42 A1:B1048576">
-    <cfRule type="cellIs" dxfId="22" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="38" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:M25 C26:E26">
-    <cfRule type="cellIs" dxfId="21" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="35" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:M25 C26:E26">
-    <cfRule type="cellIs" dxfId="20" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="36" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F26:M26 C42 F42:I42 K42:M42">
-    <cfRule type="cellIs" dxfId="19" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="29" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F26:M26 C42 F42:I42 K42:M42">
-    <cfRule type="cellIs" dxfId="18" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="30" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:I27 K27:M27">
-    <cfRule type="cellIs" dxfId="17" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="25" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:I27 K27:M27">
-    <cfRule type="cellIs" dxfId="16" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="26" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:M31 C31 F31:I31">
-    <cfRule type="cellIs" dxfId="15" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="21" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:M31 C31 F31:I31">
-    <cfRule type="cellIs" dxfId="14" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="22" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28:M28 C28 F28:I28">
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="17" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28:M28 C28 F28:I28">
-    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="18" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:M31 C31 F31:I31">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="12" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:M31 C31 F31:I31">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="11" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:I28 K28:M28">
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:I28 K28:M28">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41 F41:I41 K41:M41">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41 F41:I41 K41:M41">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Valores Metricas Vector... Matriz...
</commit_message>
<xml_diff>
--- a/Documentacion/MatrizMath/MatrizMath - Planilla de Métricas V2.1.xlsx
+++ b/Documentacion/MatrizMath/MatrizMath - Planilla de Métricas V2.1.xlsx
@@ -855,7 +855,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1061,9 +1061,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="7" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1177,97 +1174,30 @@
     <xf numFmtId="20" fontId="7" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1276,19 +1206,6 @@
     </xf>
     <xf numFmtId="49" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1303,16 +1220,93 @@
     <xf numFmtId="49" fontId="6" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1805,7 +1799,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1898,7 +1891,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1933,7 +1926,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2121,7 +2114,7 @@
   <dimension ref="A1:Z1017"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+      <selection activeCell="C42" sqref="C42:E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
@@ -2140,23 +2133,23 @@
   <sheetData>
     <row r="1" spans="1:26" ht="23.25" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="164" t="s">
+      <c r="B1" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="154"/>
-      <c r="D1" s="163" t="s">
+      <c r="C1" s="111"/>
+      <c r="D1" s="110" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="154"/>
-      <c r="F1" s="154"/>
-      <c r="G1" s="154"/>
-      <c r="H1" s="154"/>
-      <c r="I1" s="154"/>
-      <c r="J1" s="154"/>
-      <c r="K1" s="154"/>
-      <c r="L1" s="154"/>
-      <c r="M1" s="154"/>
-      <c r="N1" s="154"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="111"/>
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="111"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -2200,12 +2193,12 @@
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
       <c r="A3" s="4"/>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
-      <c r="E3" s="152"/>
+      <c r="C3" s="113"/>
+      <c r="D3" s="113"/>
+      <c r="E3" s="114"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -2331,12 +2324,12 @@
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1">
       <c r="A7" s="4"/>
-      <c r="B7" s="115" t="s">
+      <c r="B7" s="112" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="151"/>
-      <c r="D7" s="151"/>
-      <c r="E7" s="152"/>
+      <c r="C7" s="113"/>
+      <c r="D7" s="113"/>
+      <c r="E7" s="114"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -2373,15 +2366,15 @@
       <c r="E8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="153"/>
-      <c r="G8" s="154"/>
-      <c r="H8" s="154"/>
-      <c r="I8" s="154"/>
-      <c r="J8" s="154"/>
-      <c r="K8" s="154"/>
-      <c r="L8" s="154"/>
-      <c r="M8" s="154"/>
-      <c r="N8" s="154"/>
+      <c r="F8" s="116"/>
+      <c r="G8" s="111"/>
+      <c r="H8" s="111"/>
+      <c r="I8" s="111"/>
+      <c r="J8" s="111"/>
+      <c r="K8" s="111"/>
+      <c r="L8" s="111"/>
+      <c r="M8" s="111"/>
+      <c r="N8" s="111"/>
       <c r="O8" s="7"/>
       <c r="P8" s="13"/>
       <c r="Q8" s="14"/>
@@ -2410,15 +2403,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C9),ISBLANK(D9)),"Completar",IF(D9&gt;=C9,D9-C9,"Error")),"Error")</f>
         <v>1.736111111111116E-2</v>
       </c>
-      <c r="F9" s="155"/>
-      <c r="G9" s="154"/>
-      <c r="H9" s="154"/>
-      <c r="I9" s="154"/>
-      <c r="J9" s="154"/>
-      <c r="K9" s="154"/>
-      <c r="L9" s="154"/>
-      <c r="M9" s="154"/>
-      <c r="N9" s="154"/>
+      <c r="F9" s="117"/>
+      <c r="G9" s="111"/>
+      <c r="H9" s="111"/>
+      <c r="I9" s="111"/>
+      <c r="J9" s="111"/>
+      <c r="K9" s="111"/>
+      <c r="L9" s="111"/>
+      <c r="M9" s="111"/>
+      <c r="N9" s="111"/>
       <c r="O9" s="15"/>
       <c r="P9" s="21"/>
       <c r="Q9" s="22"/>
@@ -2462,12 +2455,12 @@
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" s="4"/>
-      <c r="B11" s="115" t="s">
+      <c r="B11" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="151"/>
-      <c r="D11" s="151"/>
-      <c r="E11" s="152"/>
+      <c r="C11" s="113"/>
+      <c r="D11" s="113"/>
+      <c r="E11" s="114"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -2504,15 +2497,15 @@
       <c r="E12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="153"/>
-      <c r="G12" s="154"/>
-      <c r="H12" s="154"/>
-      <c r="I12" s="154"/>
-      <c r="J12" s="154"/>
-      <c r="K12" s="154"/>
-      <c r="L12" s="154"/>
-      <c r="M12" s="154"/>
-      <c r="N12" s="154"/>
+      <c r="F12" s="116"/>
+      <c r="G12" s="111"/>
+      <c r="H12" s="111"/>
+      <c r="I12" s="111"/>
+      <c r="J12" s="111"/>
+      <c r="K12" s="111"/>
+      <c r="L12" s="111"/>
+      <c r="M12" s="111"/>
+      <c r="N12" s="111"/>
       <c r="O12" s="7"/>
       <c r="P12" s="13"/>
       <c r="Q12" s="14"/>
@@ -2541,15 +2534,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C13),ISBLANK(D13)),"Completar",IF(D13&gt;=C13,D13-C13,"Error")),"Error")</f>
         <v>1.3194444444444398E-2</v>
       </c>
-      <c r="F13" s="155"/>
-      <c r="G13" s="154"/>
-      <c r="H13" s="154"/>
-      <c r="I13" s="154"/>
-      <c r="J13" s="154"/>
-      <c r="K13" s="154"/>
-      <c r="L13" s="154"/>
-      <c r="M13" s="154"/>
-      <c r="N13" s="154"/>
+      <c r="F13" s="117"/>
+      <c r="G13" s="111"/>
+      <c r="H13" s="111"/>
+      <c r="I13" s="111"/>
+      <c r="J13" s="111"/>
+      <c r="K13" s="111"/>
+      <c r="L13" s="111"/>
+      <c r="M13" s="111"/>
+      <c r="N13" s="111"/>
       <c r="O13" s="15"/>
       <c r="P13" s="21"/>
       <c r="Q13" s="22"/>
@@ -2593,21 +2586,21 @@
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1">
       <c r="A15" s="4"/>
-      <c r="B15" s="115" t="s">
+      <c r="B15" s="112" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="151"/>
-      <c r="D15" s="151"/>
-      <c r="E15" s="151"/>
-      <c r="F15" s="151"/>
-      <c r="G15" s="151"/>
-      <c r="H15" s="151"/>
-      <c r="I15" s="151"/>
-      <c r="J15" s="151"/>
-      <c r="K15" s="151"/>
-      <c r="L15" s="151"/>
-      <c r="M15" s="151"/>
-      <c r="N15" s="152"/>
+      <c r="C15" s="113"/>
+      <c r="D15" s="113"/>
+      <c r="E15" s="113"/>
+      <c r="F15" s="113"/>
+      <c r="G15" s="113"/>
+      <c r="H15" s="113"/>
+      <c r="I15" s="113"/>
+      <c r="J15" s="113"/>
+      <c r="K15" s="113"/>
+      <c r="L15" s="113"/>
+      <c r="M15" s="113"/>
+      <c r="N15" s="114"/>
       <c r="O15" s="4"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
@@ -2623,31 +2616,31 @@
     </row>
     <row r="16" spans="1:26" ht="16.5" customHeight="1">
       <c r="A16" s="7"/>
-      <c r="B16" s="132" t="s">
+      <c r="B16" s="147" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="134" t="s">
+      <c r="C16" s="149" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="135"/>
-      <c r="E16" s="135"/>
-      <c r="F16" s="142" t="s">
+      <c r="D16" s="150"/>
+      <c r="E16" s="150"/>
+      <c r="F16" s="143" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="143"/>
-      <c r="H16" s="141" t="s">
+      <c r="G16" s="144"/>
+      <c r="H16" s="142" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="124"/>
-      <c r="J16" s="124"/>
-      <c r="K16" s="142" t="s">
+      <c r="I16" s="127"/>
+      <c r="J16" s="127"/>
+      <c r="K16" s="143" t="s">
         <v>14</v>
       </c>
-      <c r="L16" s="143"/>
-      <c r="M16" s="144" t="s">
+      <c r="L16" s="144"/>
+      <c r="M16" s="145" t="s">
         <v>15</v>
       </c>
-      <c r="N16" s="139" t="s">
+      <c r="N16" s="137" t="s">
         <v>6</v>
       </c>
       <c r="O16" s="7"/>
@@ -2665,10 +2658,10 @@
     </row>
     <row r="17" spans="1:26" ht="30" customHeight="1">
       <c r="A17" s="7"/>
-      <c r="B17" s="133"/>
-      <c r="C17" s="136"/>
-      <c r="D17" s="137"/>
-      <c r="E17" s="137"/>
+      <c r="B17" s="148"/>
+      <c r="C17" s="151"/>
+      <c r="D17" s="152"/>
+      <c r="E17" s="152"/>
       <c r="F17" s="26" t="s">
         <v>16</v>
       </c>
@@ -2690,8 +2683,8 @@
       <c r="L17" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="M17" s="145"/>
-      <c r="N17" s="140"/>
+      <c r="M17" s="146"/>
+      <c r="N17" s="138"/>
       <c r="O17" s="7"/>
       <c r="P17" s="13"/>
       <c r="Q17" s="14"/>
@@ -2708,18 +2701,17 @@
     <row r="18" spans="1:26">
       <c r="A18" s="15"/>
       <c r="B18" s="30">
-        <f t="shared" ref="B18:B40" si="0">ROW($B18)-16</f>
-        <v>2</v>
-      </c>
-      <c r="C18" s="138" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="124"/>
-      <c r="E18" s="124"/>
+      <c r="D18" s="127"/>
+      <c r="E18" s="127"/>
       <c r="F18" s="31">
         <v>60</v>
       </c>
-      <c r="G18" s="89">
+      <c r="G18" s="88">
         <v>1.7361111111111112E-2</v>
       </c>
       <c r="H18" s="32">
@@ -2729,7 +2721,7 @@
         <v>0.68819444444444444</v>
       </c>
       <c r="J18" s="34">
-        <f t="shared" ref="J18:J27" si="1">IFERROR(IF(OR(ISBLANK(H18),ISBLANK(I18)),"",IF(I18&gt;=H18,I18-H18,"Error")),"Error")</f>
+        <f t="shared" ref="J18:J27" si="0">IFERROR(IF(OR(ISBLANK(H18),ISBLANK(I18)),"",IF(I18&gt;=H18,I18-H18,"Error")),"Error")</f>
         <v>2.1527777777777812E-2</v>
       </c>
       <c r="K18" s="35">
@@ -2742,7 +2734,7 @@
         <v>66</v>
       </c>
       <c r="N18" s="38">
-        <f t="shared" ref="N18:N27" si="2">IFERROR(IF(OR(J18="",ISBLANK(L18)),"",J18+L18),"Error")</f>
+        <f t="shared" ref="N18:N27" si="1">IFERROR(IF(OR(J18="",ISBLANK(L18)),"",J18+L18),"Error")</f>
         <v>2.9166666666666702E-2</v>
       </c>
       <c r="O18" s="15"/>
@@ -2761,18 +2753,17 @@
     <row r="19" spans="1:26">
       <c r="A19" s="15"/>
       <c r="B19" s="30">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C19" s="138" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="139" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="124"/>
-      <c r="E19" s="124"/>
+      <c r="D19" s="127"/>
+      <c r="E19" s="127"/>
       <c r="F19" s="31">
         <v>4</v>
       </c>
-      <c r="G19" s="89">
+      <c r="G19" s="88">
         <v>3.472222222222222E-3</v>
       </c>
       <c r="H19" s="32">
@@ -2782,7 +2773,7 @@
         <v>0.69513888888888886</v>
       </c>
       <c r="J19" s="34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4.1666666666666519E-3</v>
       </c>
       <c r="K19" s="35">
@@ -2795,7 +2786,7 @@
         <v>10</v>
       </c>
       <c r="N19" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.1666666666666519E-3</v>
       </c>
       <c r="O19" s="15"/>
@@ -2814,18 +2805,17 @@
     <row r="20" spans="1:26">
       <c r="A20" s="15"/>
       <c r="B20" s="30">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C20" s="138" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="139" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="124"/>
-      <c r="E20" s="124"/>
+      <c r="D20" s="127"/>
+      <c r="E20" s="127"/>
       <c r="F20" s="31">
         <v>8</v>
       </c>
-      <c r="G20" s="89">
+      <c r="G20" s="88">
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="H20" s="32">
@@ -2835,7 +2825,7 @@
         <v>0.70694444444444449</v>
       </c>
       <c r="J20" s="34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.4722222222222099E-3</v>
       </c>
       <c r="K20" s="35">
@@ -2848,7 +2838,7 @@
         <v>5</v>
       </c>
       <c r="N20" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.4722222222222099E-3</v>
       </c>
       <c r="O20" s="15"/>
@@ -2867,18 +2857,17 @@
     <row r="21" spans="1:26">
       <c r="A21" s="15"/>
       <c r="B21" s="30">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C21" s="138" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="139" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="124"/>
-      <c r="E21" s="124"/>
+      <c r="D21" s="127"/>
+      <c r="E21" s="127"/>
       <c r="F21" s="31">
         <v>10</v>
       </c>
-      <c r="G21" s="89">
+      <c r="G21" s="88">
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="H21" s="32">
@@ -2888,7 +2877,7 @@
         <v>0.71736111111111112</v>
       </c>
       <c r="J21" s="34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5.5555555555555358E-3</v>
       </c>
       <c r="K21" s="35">
@@ -2901,7 +2890,7 @@
         <v>17</v>
       </c>
       <c r="N21" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5.5555555555555358E-3</v>
       </c>
       <c r="O21" s="15"/>
@@ -2917,74 +2906,72 @@
       <c r="Y21" s="22"/>
       <c r="Z21" s="22"/>
     </row>
-    <row r="22" spans="1:26" s="80" customFormat="1">
+    <row r="22" spans="1:26" s="79" customFormat="1">
       <c r="A22" s="68"/>
-      <c r="B22" s="69">
+      <c r="B22" s="30">
+        <v>5</v>
+      </c>
+      <c r="C22" s="140" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="141"/>
+      <c r="E22" s="141"/>
+      <c r="F22" s="69">
+        <v>8</v>
+      </c>
+      <c r="G22" s="94">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="H22" s="70">
+        <v>0.6777777777777777</v>
+      </c>
+      <c r="I22" s="71">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="J22" s="72">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C22" s="125" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="130"/>
-      <c r="E22" s="130"/>
-      <c r="F22" s="70">
-        <v>8</v>
-      </c>
-      <c r="G22" s="95">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="H22" s="71">
-        <v>0.6777777777777777</v>
-      </c>
-      <c r="I22" s="72">
-        <v>0.69097222222222221</v>
-      </c>
-      <c r="J22" s="73">
+        <v>1.3194444444444509E-2</v>
+      </c>
+      <c r="K22" s="73">
+        <v>1</v>
+      </c>
+      <c r="L22" s="74">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="M22" s="75">
+        <v>11</v>
+      </c>
+      <c r="N22" s="76">
         <f t="shared" si="1"/>
-        <v>1.3194444444444509E-2</v>
-      </c>
-      <c r="K22" s="74">
-        <v>1</v>
-      </c>
-      <c r="L22" s="75">
-        <v>3.472222222222222E-3</v>
-      </c>
-      <c r="M22" s="76">
-        <v>11</v>
-      </c>
-      <c r="N22" s="77">
-        <f t="shared" si="2"/>
         <v>1.6666666666666732E-2</v>
       </c>
       <c r="O22" s="68"/>
-      <c r="P22" s="78"/>
-      <c r="Q22" s="79"/>
-      <c r="R22" s="79"/>
-      <c r="S22" s="79"/>
-      <c r="T22" s="79"/>
-      <c r="U22" s="79"/>
-      <c r="V22" s="79"/>
-      <c r="W22" s="79"/>
-      <c r="X22" s="79"/>
-      <c r="Y22" s="79"/>
-      <c r="Z22" s="79"/>
+      <c r="P22" s="77"/>
+      <c r="Q22" s="78"/>
+      <c r="R22" s="78"/>
+      <c r="S22" s="78"/>
+      <c r="T22" s="78"/>
+      <c r="U22" s="78"/>
+      <c r="V22" s="78"/>
+      <c r="W22" s="78"/>
+      <c r="X22" s="78"/>
+      <c r="Y22" s="78"/>
+      <c r="Z22" s="78"/>
     </row>
     <row r="23" spans="1:26">
       <c r="A23" s="15"/>
       <c r="B23" s="30">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C23" s="121" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="126" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="124"/>
-      <c r="E23" s="124"/>
+      <c r="D23" s="127"/>
+      <c r="E23" s="127"/>
       <c r="F23" s="40">
         <v>13</v>
       </c>
-      <c r="G23" s="89">
+      <c r="G23" s="88">
         <v>1.2499999999999999E-2</v>
       </c>
       <c r="H23" s="41">
@@ -2994,7 +2981,7 @@
         <v>0.7055555555555556</v>
       </c>
       <c r="J23" s="34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9.7222222222222987E-3</v>
       </c>
       <c r="K23" s="43">
@@ -3007,7 +2994,7 @@
         <v>16</v>
       </c>
       <c r="N23" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>9.7222222222222987E-3</v>
       </c>
       <c r="O23" s="15"/>
@@ -3026,18 +3013,17 @@
     <row r="24" spans="1:26">
       <c r="A24" s="15"/>
       <c r="B24" s="30">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C24" s="121" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="124"/>
-      <c r="E24" s="124"/>
+      <c r="D24" s="127"/>
+      <c r="E24" s="127"/>
       <c r="F24" s="40">
         <v>25</v>
       </c>
-      <c r="G24" s="89">
+      <c r="G24" s="88">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="H24" s="41">
@@ -3047,7 +3033,7 @@
         <v>0.72222222222222221</v>
       </c>
       <c r="J24" s="34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9.7222222222221877E-3</v>
       </c>
       <c r="K24" s="43">
@@ -3060,7 +3046,7 @@
         <v>13</v>
       </c>
       <c r="N24" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.5277777777777744E-2</v>
       </c>
       <c r="O24" s="15"/>
@@ -3079,18 +3065,17 @@
     <row r="25" spans="1:26">
       <c r="A25" s="67"/>
       <c r="B25" s="30">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="C25" s="121" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="126" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="124"/>
-      <c r="E25" s="124"/>
+      <c r="D25" s="127"/>
+      <c r="E25" s="127"/>
       <c r="F25" s="40">
         <v>20</v>
       </c>
-      <c r="G25" s="89">
+      <c r="G25" s="88">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="H25" s="41">
@@ -3100,7 +3085,7 @@
         <v>0.74930555555555556</v>
       </c>
       <c r="J25" s="34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.2499999999999956E-2</v>
       </c>
       <c r="K25" s="43">
@@ -3113,7 +3098,7 @@
         <v>17</v>
       </c>
       <c r="N25" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.2499999999999956E-2</v>
       </c>
       <c r="O25" s="67"/>
@@ -3132,18 +3117,17 @@
     <row r="26" spans="1:26" ht="15" customHeight="1">
       <c r="A26" s="67"/>
       <c r="B26" s="30">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C26" s="121" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="126" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="124"/>
-      <c r="E26" s="124"/>
+      <c r="D26" s="127"/>
+      <c r="E26" s="127"/>
       <c r="F26" s="40">
         <v>16</v>
       </c>
-      <c r="G26" s="89">
+      <c r="G26" s="88">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="H26" s="41">
@@ -3153,7 +3137,7 @@
         <v>0.75694444444444453</v>
       </c>
       <c r="J26" s="34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6.2500000000000888E-3</v>
       </c>
       <c r="K26" s="43">
@@ -3166,7 +3150,7 @@
         <v>17</v>
       </c>
       <c r="N26" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6.9444444444445334E-3</v>
       </c>
       <c r="O26" s="67"/>
@@ -3185,18 +3169,17 @@
     <row r="27" spans="1:26" ht="15" customHeight="1">
       <c r="A27" s="67"/>
       <c r="B27" s="30">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="C27" s="121" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="126" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="124"/>
-      <c r="E27" s="124"/>
+      <c r="D27" s="127"/>
+      <c r="E27" s="127"/>
       <c r="F27" s="40">
         <v>30</v>
       </c>
-      <c r="G27" s="89">
+      <c r="G27" s="88">
         <v>2.4305555555555556E-2</v>
       </c>
       <c r="H27" s="41">
@@ -3206,7 +3189,7 @@
         <v>0.77430555555555547</v>
       </c>
       <c r="J27" s="34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.5277777777777724E-2</v>
       </c>
       <c r="K27" s="43">
@@ -3219,7 +3202,7 @@
         <v>16</v>
       </c>
       <c r="N27" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.5277777777777724E-2</v>
       </c>
       <c r="O27" s="67"/>
@@ -3238,37 +3221,36 @@
     <row r="28" spans="1:26" ht="15" customHeight="1">
       <c r="A28" s="67"/>
       <c r="B28" s="30">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="C28" s="121" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="126" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="122"/>
-      <c r="E28" s="123"/>
-      <c r="F28" s="82">
+      <c r="D28" s="158"/>
+      <c r="E28" s="159"/>
+      <c r="F28" s="81">
         <v>30</v>
       </c>
-      <c r="G28" s="89">
+      <c r="G28" s="88">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="H28" s="83">
+      <c r="H28" s="82">
         <v>0.91527777777777775</v>
       </c>
-      <c r="I28" s="84">
+      <c r="I28" s="83">
         <v>0.95208333333333339</v>
       </c>
       <c r="J28" s="34">
         <f>IFERROR(IF(OR(ISBLANK(H28),ISBLANK(I28)),"",IF(I28&gt;=H28,I28-H28,"Error")),"Error")</f>
         <v>3.6805555555555647E-2</v>
       </c>
-      <c r="K28" s="86">
+      <c r="K28" s="85">
         <v>2</v>
       </c>
-      <c r="L28" s="89">
+      <c r="L28" s="88">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="M28" s="87">
+      <c r="M28" s="86">
         <v>26</v>
       </c>
       <c r="N28" s="38">
@@ -3291,40 +3273,39 @@
     <row r="29" spans="1:26" ht="15" customHeight="1">
       <c r="A29" s="67"/>
       <c r="B29" s="30">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="C29" s="121" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="126" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="122"/>
-      <c r="E29" s="123"/>
-      <c r="F29" s="82">
+      <c r="D29" s="158"/>
+      <c r="E29" s="159"/>
+      <c r="F29" s="81">
         <v>15</v>
       </c>
-      <c r="G29" s="89">
+      <c r="G29" s="88">
         <v>3.472222222222222E-3</v>
       </c>
-      <c r="H29" s="83">
+      <c r="H29" s="82">
         <v>0.99375000000000002</v>
       </c>
-      <c r="I29" s="84">
+      <c r="I29" s="83">
         <v>0.99791666666666667</v>
       </c>
       <c r="J29" s="34">
         <f>IFERROR(IF(OR(ISBLANK(H29),ISBLANK(I29)),"",IF(I29&gt;=H29,I29-H29,"Error")),"Error")</f>
         <v>4.1666666666666519E-3</v>
       </c>
-      <c r="K29" s="86">
+      <c r="K29" s="85">
         <v>0</v>
       </c>
-      <c r="L29" s="89">
+      <c r="L29" s="88">
         <v>0</v>
       </c>
-      <c r="M29" s="87">
+      <c r="M29" s="86">
         <v>7</v>
       </c>
-      <c r="N29" s="88">
+      <c r="N29" s="87">
         <f>IFERROR(IF(OR(J29="",ISBLANK(L29)),"",J29+L29),"Error")</f>
         <v>4.1666666666666519E-3</v>
       </c>
@@ -3342,46 +3323,45 @@
       <c r="Z29" s="22"/>
     </row>
     <row r="30" spans="1:26" ht="15" customHeight="1">
-      <c r="A30" s="100"/>
+      <c r="A30" s="99"/>
       <c r="B30" s="30">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="C30" s="121" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="126" t="s">
         <v>51</v>
       </c>
-      <c r="D30" s="122"/>
-      <c r="E30" s="123"/>
-      <c r="F30" s="82">
+      <c r="D30" s="158"/>
+      <c r="E30" s="159"/>
+      <c r="F30" s="81">
         <v>25</v>
       </c>
-      <c r="G30" s="89">
+      <c r="G30" s="88">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="H30" s="83">
+      <c r="H30" s="82">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="I30" s="84">
+      <c r="I30" s="83">
         <v>6.25E-2</v>
       </c>
       <c r="J30" s="34">
         <f>IFERROR(IF(OR(ISBLANK(H30),ISBLANK(I30)),"",IF(I30&gt;=H30,I30-H30,"Error")),"Error")</f>
         <v>4.1666666666666671E-2</v>
       </c>
-      <c r="K30" s="86">
+      <c r="K30" s="85">
         <v>2</v>
       </c>
-      <c r="L30" s="89">
+      <c r="L30" s="88">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="M30" s="87">
+      <c r="M30" s="86">
         <v>16</v>
       </c>
-      <c r="N30" s="88">
-        <f t="shared" ref="N30:N41" si="3">IFERROR(IF(OR(J30="",ISBLANK(L30)),"",J30+L30),"Error")</f>
+      <c r="N30" s="87">
+        <f t="shared" ref="N30:N41" si="2">IFERROR(IF(OR(J30="",ISBLANK(L30)),"",J30+L30),"Error")</f>
         <v>5.5555555555555559E-2</v>
       </c>
-      <c r="O30" s="100"/>
+      <c r="O30" s="99"/>
       <c r="P30" s="21"/>
       <c r="Q30" s="22"/>
       <c r="R30" s="22"/>
@@ -3395,46 +3375,45 @@
       <c r="Z30" s="22"/>
     </row>
     <row r="31" spans="1:26" ht="15" customHeight="1">
-      <c r="A31" s="100"/>
+      <c r="A31" s="99"/>
       <c r="B31" s="30">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="C31" s="121" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="126" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="122"/>
-      <c r="E31" s="123"/>
-      <c r="F31" s="82">
+      <c r="D31" s="158"/>
+      <c r="E31" s="159"/>
+      <c r="F31" s="81">
         <v>18</v>
       </c>
-      <c r="G31" s="89">
+      <c r="G31" s="88">
         <v>9.0277777777777787E-3</v>
       </c>
-      <c r="H31" s="83">
+      <c r="H31" s="82">
         <v>0.77430555555555547</v>
       </c>
-      <c r="I31" s="84">
+      <c r="I31" s="83">
         <v>0.78472222222222221</v>
       </c>
-      <c r="J31" s="85">
+      <c r="J31" s="84">
         <f>IFERROR(IF(OR(ISBLANK(H31),ISBLANK(I31)),"",IF(I31&gt;=H31,I31-H31,"Error")),"Error")</f>
         <v>1.0416666666666741E-2</v>
       </c>
-      <c r="K31" s="86">
+      <c r="K31" s="85">
         <v>2</v>
       </c>
-      <c r="L31" s="89">
+      <c r="L31" s="88">
         <v>2.7777777777777779E-3</v>
       </c>
-      <c r="M31" s="87">
+      <c r="M31" s="86">
         <v>21</v>
       </c>
-      <c r="N31" s="88">
-        <f t="shared" si="3"/>
+      <c r="N31" s="87">
+        <f t="shared" si="2"/>
         <v>1.3194444444444519E-2</v>
       </c>
-      <c r="O31" s="100"/>
+      <c r="O31" s="99"/>
       <c r="P31" s="21"/>
       <c r="Q31" s="22"/>
       <c r="R31" s="22"/>
@@ -3448,46 +3427,45 @@
       <c r="Z31" s="22"/>
     </row>
     <row r="32" spans="1:26" ht="15" customHeight="1">
-      <c r="A32" s="100"/>
+      <c r="A32" s="99"/>
       <c r="B32" s="30">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="C32" s="121" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="126" t="s">
         <v>47</v>
       </c>
-      <c r="D32" s="122"/>
-      <c r="E32" s="123"/>
-      <c r="F32" s="82">
+      <c r="D32" s="158"/>
+      <c r="E32" s="159"/>
+      <c r="F32" s="81">
         <v>17</v>
       </c>
-      <c r="G32" s="89">
+      <c r="G32" s="88">
         <v>2.4305555555555556E-2</v>
       </c>
-      <c r="H32" s="83">
+      <c r="H32" s="82">
         <v>0.86388888888888893</v>
       </c>
-      <c r="I32" s="84">
+      <c r="I32" s="83">
         <v>0.87847222222222221</v>
       </c>
-      <c r="J32" s="85">
-        <f t="shared" ref="J32:J41" si="4">IFERROR(IF(OR(ISBLANK(H32),ISBLANK(I32)),"",IF(I32&gt;=H32,I32-H32,"Error")),"Error")</f>
+      <c r="J32" s="84">
+        <f t="shared" ref="J32:J41" si="3">IFERROR(IF(OR(ISBLANK(H32),ISBLANK(I32)),"",IF(I32&gt;=H32,I32-H32,"Error")),"Error")</f>
         <v>1.4583333333333282E-2</v>
       </c>
-      <c r="K32" s="86">
+      <c r="K32" s="85">
         <v>0</v>
       </c>
-      <c r="L32" s="89">
+      <c r="L32" s="88">
         <v>0</v>
       </c>
-      <c r="M32" s="87">
+      <c r="M32" s="86">
         <v>17</v>
       </c>
-      <c r="N32" s="88">
-        <f t="shared" si="3"/>
+      <c r="N32" s="87">
+        <f t="shared" si="2"/>
         <v>1.4583333333333282E-2</v>
       </c>
-      <c r="O32" s="81"/>
+      <c r="O32" s="80"/>
       <c r="P32" s="21"/>
       <c r="Q32" s="22"/>
       <c r="R32" s="22"/>
@@ -3500,206 +3478,202 @@
       <c r="Y32" s="22"/>
       <c r="Z32" s="22"/>
     </row>
-    <row r="33" spans="1:26" s="98" customFormat="1" ht="15" customHeight="1">
-      <c r="A33" s="90"/>
-      <c r="B33" s="109">
-        <f t="shared" si="0"/>
+    <row r="33" spans="1:26" s="97" customFormat="1" ht="15" customHeight="1">
+      <c r="A33" s="89"/>
+      <c r="B33" s="30">
+        <v>16</v>
+      </c>
+      <c r="C33" s="140" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" s="153"/>
+      <c r="E33" s="154"/>
+      <c r="F33" s="90">
+        <v>20</v>
+      </c>
+      <c r="G33" s="94">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H33" s="91">
+        <v>0.91388888888888886</v>
+      </c>
+      <c r="I33" s="92">
+        <v>0.93541666666666667</v>
+      </c>
+      <c r="J33" s="84">
+        <f t="shared" si="3"/>
+        <v>2.1527777777777812E-2</v>
+      </c>
+      <c r="K33" s="93">
+        <v>1</v>
+      </c>
+      <c r="L33" s="106">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="M33" s="90">
+        <v>13</v>
+      </c>
+      <c r="N33" s="87">
+        <f t="shared" si="2"/>
+        <v>2.29166666666667E-2</v>
+      </c>
+      <c r="O33" s="89"/>
+      <c r="P33" s="95"/>
+      <c r="Q33" s="96"/>
+      <c r="R33" s="96"/>
+      <c r="S33" s="96"/>
+      <c r="T33" s="96"/>
+      <c r="U33" s="96"/>
+      <c r="V33" s="96"/>
+      <c r="W33" s="96"/>
+      <c r="X33" s="96"/>
+      <c r="Y33" s="96"/>
+      <c r="Z33" s="96"/>
+    </row>
+    <row r="34" spans="1:26" s="97" customFormat="1" ht="15" customHeight="1">
+      <c r="A34" s="89"/>
+      <c r="B34" s="30">
         <v>17</v>
       </c>
-      <c r="C33" s="125" t="s">
-        <v>48</v>
-      </c>
-      <c r="D33" s="126"/>
-      <c r="E33" s="127"/>
-      <c r="F33" s="91">
-        <v>20</v>
-      </c>
-      <c r="G33" s="95">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="H33" s="92">
-        <v>0.91388888888888886</v>
-      </c>
-      <c r="I33" s="93">
-        <v>0.93541666666666667</v>
-      </c>
-      <c r="J33" s="85">
-        <f t="shared" si="4"/>
-        <v>2.1527777777777812E-2</v>
-      </c>
-      <c r="K33" s="94">
-        <v>1</v>
-      </c>
-      <c r="L33" s="107">
-        <v>1.3888888888888889E-3</v>
-      </c>
-      <c r="M33" s="91">
-        <v>13</v>
-      </c>
-      <c r="N33" s="88">
-        <f t="shared" si="3"/>
-        <v>2.29166666666667E-2</v>
-      </c>
-      <c r="O33" s="90"/>
-      <c r="P33" s="96"/>
-      <c r="Q33" s="97"/>
-      <c r="R33" s="97"/>
-      <c r="S33" s="97"/>
-      <c r="T33" s="97"/>
-      <c r="U33" s="97"/>
-      <c r="V33" s="97"/>
-      <c r="W33" s="97"/>
-      <c r="X33" s="97"/>
-      <c r="Y33" s="97"/>
-      <c r="Z33" s="97"/>
-    </row>
-    <row r="34" spans="1:26" s="98" customFormat="1" ht="15" customHeight="1">
-      <c r="A34" s="90"/>
-      <c r="B34" s="109">
-        <f t="shared" si="0"/>
+      <c r="C34" s="140" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="153"/>
+      <c r="E34" s="154"/>
+      <c r="F34" s="90">
         <v>18</v>
       </c>
-      <c r="C34" s="125" t="s">
-        <v>49</v>
-      </c>
-      <c r="D34" s="126"/>
-      <c r="E34" s="127"/>
-      <c r="F34" s="91">
-        <v>18</v>
-      </c>
-      <c r="G34" s="95">
+      <c r="G34" s="94">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="H34" s="92">
+      <c r="H34" s="91">
         <v>0.93611111111111101</v>
       </c>
-      <c r="I34" s="93">
+      <c r="I34" s="92">
         <v>0.95972222222222225</v>
       </c>
-      <c r="J34" s="85">
-        <f t="shared" si="4"/>
-        <v>2.3611111111111249E-2</v>
-      </c>
-      <c r="K34" s="94">
-        <v>0</v>
-      </c>
-      <c r="L34" s="107">
-        <v>0</v>
-      </c>
-      <c r="M34" s="91">
-        <v>14</v>
-      </c>
-      <c r="N34" s="88">
+      <c r="J34" s="84">
         <f t="shared" si="3"/>
         <v>2.3611111111111249E-2</v>
       </c>
-      <c r="O34" s="90"/>
-      <c r="P34" s="96"/>
-      <c r="Q34" s="97"/>
-      <c r="R34" s="97"/>
-      <c r="S34" s="97"/>
-      <c r="T34" s="97"/>
-      <c r="U34" s="97"/>
-      <c r="V34" s="97"/>
-      <c r="W34" s="97"/>
-      <c r="X34" s="97"/>
-      <c r="Y34" s="97"/>
-      <c r="Z34" s="97"/>
-    </row>
-    <row r="35" spans="1:26" s="98" customFormat="1" ht="15" customHeight="1">
-      <c r="A35" s="90"/>
-      <c r="B35" s="109">
-        <f t="shared" si="0"/>
+      <c r="K34" s="93">
+        <v>0</v>
+      </c>
+      <c r="L34" s="106">
+        <v>0</v>
+      </c>
+      <c r="M34" s="90">
+        <v>14</v>
+      </c>
+      <c r="N34" s="87">
+        <f t="shared" si="2"/>
+        <v>2.3611111111111249E-2</v>
+      </c>
+      <c r="O34" s="89"/>
+      <c r="P34" s="95"/>
+      <c r="Q34" s="96"/>
+      <c r="R34" s="96"/>
+      <c r="S34" s="96"/>
+      <c r="T34" s="96"/>
+      <c r="U34" s="96"/>
+      <c r="V34" s="96"/>
+      <c r="W34" s="96"/>
+      <c r="X34" s="96"/>
+      <c r="Y34" s="96"/>
+      <c r="Z34" s="96"/>
+    </row>
+    <row r="35" spans="1:26" s="97" customFormat="1" ht="15" customHeight="1">
+      <c r="A35" s="89"/>
+      <c r="B35" s="30">
+        <v>18</v>
+      </c>
+      <c r="C35" s="140" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" s="141"/>
+      <c r="E35" s="157"/>
+      <c r="F35" s="90">
+        <v>20</v>
+      </c>
+      <c r="G35" s="94">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H35" s="101">
+        <v>0.96527777777777779</v>
+      </c>
+      <c r="I35" s="92">
+        <v>0.98263888888888884</v>
+      </c>
+      <c r="J35" s="84">
+        <f t="shared" si="3"/>
+        <v>1.7361111111111049E-2</v>
+      </c>
+      <c r="K35" s="93">
+        <v>1</v>
+      </c>
+      <c r="L35" s="106">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="M35" s="90">
+        <v>15</v>
+      </c>
+      <c r="N35" s="87">
+        <f t="shared" si="2"/>
+        <v>1.9444444444444382E-2</v>
+      </c>
+      <c r="O35" s="89"/>
+      <c r="P35" s="95"/>
+      <c r="Q35" s="96"/>
+      <c r="R35" s="96"/>
+      <c r="S35" s="96"/>
+      <c r="T35" s="96"/>
+      <c r="U35" s="96"/>
+      <c r="V35" s="96"/>
+      <c r="W35" s="96"/>
+      <c r="X35" s="96"/>
+      <c r="Y35" s="96"/>
+      <c r="Z35" s="96"/>
+    </row>
+    <row r="36" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A36" s="80"/>
+      <c r="B36" s="30">
         <v>19</v>
       </c>
-      <c r="C35" s="125" t="s">
-        <v>50</v>
-      </c>
-      <c r="D35" s="130"/>
-      <c r="E35" s="131"/>
-      <c r="F35" s="91">
+      <c r="C36" s="128" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="129"/>
+      <c r="E36" s="130"/>
+      <c r="F36" s="104">
         <v>20</v>
       </c>
-      <c r="G35" s="95">
+      <c r="G36" s="105">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="H35" s="102">
-        <v>0.96527777777777779</v>
-      </c>
-      <c r="I35" s="93">
-        <v>0.98263888888888884</v>
-      </c>
-      <c r="J35" s="85">
-        <f t="shared" si="4"/>
-        <v>1.7361111111111049E-2</v>
-      </c>
-      <c r="K35" s="94">
-        <v>1</v>
-      </c>
-      <c r="L35" s="107">
-        <v>2.0833333333333333E-3</v>
-      </c>
-      <c r="M35" s="91">
-        <v>15</v>
-      </c>
-      <c r="N35" s="88">
+      <c r="H36" s="102">
+        <v>0</v>
+      </c>
+      <c r="I36" s="103">
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="J36" s="84">
         <f t="shared" si="3"/>
-        <v>1.9444444444444382E-2</v>
-      </c>
-      <c r="O35" s="90"/>
-      <c r="P35" s="96"/>
-      <c r="Q35" s="97"/>
-      <c r="R35" s="97"/>
-      <c r="S35" s="97"/>
-      <c r="T35" s="97"/>
-      <c r="U35" s="97"/>
-      <c r="V35" s="97"/>
-      <c r="W35" s="97"/>
-      <c r="X35" s="97"/>
-      <c r="Y35" s="97"/>
-      <c r="Z35" s="97"/>
-    </row>
-    <row r="36" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A36" s="81"/>
-      <c r="B36" s="109">
-        <f t="shared" si="0"/>
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="K36" s="93">
+        <v>2</v>
+      </c>
+      <c r="L36" s="106">
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="M36" s="90">
         <v>20</v>
       </c>
-      <c r="C36" s="112" t="s">
-        <v>54</v>
-      </c>
-      <c r="D36" s="113"/>
-      <c r="E36" s="114"/>
-      <c r="F36" s="105">
-        <v>20</v>
-      </c>
-      <c r="G36" s="106">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="H36" s="103">
-        <v>0</v>
-      </c>
-      <c r="I36" s="104">
-        <v>2.4999999999999998E-2</v>
-      </c>
-      <c r="J36" s="85">
-        <f t="shared" si="4"/>
-        <v>2.4999999999999998E-2</v>
-      </c>
-      <c r="K36" s="94">
-        <v>2</v>
-      </c>
-      <c r="L36" s="107">
-        <v>2.7777777777777779E-3</v>
-      </c>
-      <c r="M36" s="91">
-        <v>20</v>
-      </c>
-      <c r="N36" s="88">
-        <f t="shared" si="3"/>
+      <c r="N36" s="87">
+        <f t="shared" si="2"/>
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="O36" s="81"/>
+      <c r="O36" s="80"/>
       <c r="P36" s="21"/>
       <c r="Q36" s="22"/>
       <c r="R36" s="22"/>
@@ -3713,46 +3687,45 @@
       <c r="Z36" s="22"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A37" s="81"/>
-      <c r="B37" s="109">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="C37" s="112" t="s">
+      <c r="A37" s="80"/>
+      <c r="B37" s="30">
+        <v>20</v>
+      </c>
+      <c r="C37" s="128" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="113"/>
-      <c r="E37" s="114"/>
-      <c r="F37" s="105">
+      <c r="D37" s="129"/>
+      <c r="E37" s="130"/>
+      <c r="F37" s="104">
         <v>20</v>
       </c>
-      <c r="G37" s="106">
+      <c r="G37" s="105">
         <v>1.7361111111111112E-2</v>
       </c>
-      <c r="H37" s="103">
+      <c r="H37" s="102">
         <v>4.0972222222222222E-2</v>
       </c>
-      <c r="I37" s="104">
+      <c r="I37" s="103">
         <v>5.486111111111111E-2</v>
       </c>
-      <c r="J37" s="85">
-        <f t="shared" si="4"/>
+      <c r="J37" s="84">
+        <f t="shared" si="3"/>
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="K37" s="105">
+      <c r="K37" s="104">
         <v>2</v>
       </c>
-      <c r="L37" s="108">
+      <c r="L37" s="107">
         <v>9.7222222222222224E-3</v>
       </c>
-      <c r="M37" s="105">
+      <c r="M37" s="104">
         <v>15</v>
       </c>
-      <c r="N37" s="88">
-        <f t="shared" si="3"/>
+      <c r="N37" s="87">
+        <f t="shared" si="2"/>
         <v>2.361111111111111E-2</v>
       </c>
-      <c r="O37" s="81"/>
+      <c r="O37" s="80"/>
       <c r="P37" s="21"/>
       <c r="Q37" s="22"/>
       <c r="R37" s="22"/>
@@ -3766,46 +3739,45 @@
       <c r="Z37" s="22"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A38" s="99"/>
-      <c r="B38" s="109">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="C38" s="128" t="s">
+      <c r="A38" s="98"/>
+      <c r="B38" s="30">
+        <v>21</v>
+      </c>
+      <c r="C38" s="155" t="s">
         <v>53</v>
       </c>
-      <c r="D38" s="128"/>
-      <c r="E38" s="129"/>
-      <c r="F38" s="105">
+      <c r="D38" s="155"/>
+      <c r="E38" s="156"/>
+      <c r="F38" s="104">
         <v>25</v>
       </c>
-      <c r="G38" s="106">
+      <c r="G38" s="105">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="H38" s="103">
+      <c r="H38" s="102">
         <v>5.6944444444444443E-2</v>
       </c>
-      <c r="I38" s="104">
+      <c r="I38" s="103">
         <v>7.6388888888888895E-2</v>
       </c>
-      <c r="J38" s="85">
-        <f t="shared" si="4"/>
+      <c r="J38" s="84">
+        <f t="shared" si="3"/>
         <v>1.9444444444444452E-2</v>
       </c>
-      <c r="K38" s="105">
+      <c r="K38" s="104">
         <v>2</v>
       </c>
-      <c r="L38" s="108">
+      <c r="L38" s="107">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="M38" s="105">
+      <c r="M38" s="104">
         <v>16</v>
       </c>
-      <c r="N38" s="88">
-        <f t="shared" si="3"/>
+      <c r="N38" s="87">
+        <f t="shared" si="2"/>
         <v>3.333333333333334E-2</v>
       </c>
-      <c r="O38" s="99"/>
+      <c r="O38" s="98"/>
       <c r="P38" s="21"/>
       <c r="Q38" s="22"/>
       <c r="R38" s="22"/>
@@ -3819,46 +3791,45 @@
       <c r="Z38" s="22"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A39" s="99"/>
-      <c r="B39" s="109">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="C39" s="128" t="s">
+      <c r="A39" s="98"/>
+      <c r="B39" s="30">
+        <v>22</v>
+      </c>
+      <c r="C39" s="155" t="s">
         <v>56</v>
       </c>
-      <c r="D39" s="128"/>
-      <c r="E39" s="129"/>
-      <c r="F39" s="105">
+      <c r="D39" s="155"/>
+      <c r="E39" s="156"/>
+      <c r="F39" s="104">
         <v>25</v>
       </c>
-      <c r="G39" s="106">
+      <c r="G39" s="105">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="H39" s="103">
+      <c r="H39" s="102">
         <v>0.37013888888888885</v>
       </c>
-      <c r="I39" s="104">
+      <c r="I39" s="103">
         <v>0.39166666666666666</v>
       </c>
-      <c r="J39" s="73">
-        <f t="shared" si="4"/>
+      <c r="J39" s="72">
+        <f t="shared" si="3"/>
         <v>2.1527777777777812E-2</v>
       </c>
-      <c r="K39" s="105">
+      <c r="K39" s="104">
         <v>3</v>
       </c>
-      <c r="L39" s="108">
+      <c r="L39" s="107">
         <v>3.472222222222222E-3</v>
       </c>
-      <c r="M39" s="105">
+      <c r="M39" s="104">
         <v>62</v>
       </c>
-      <c r="N39" s="77">
-        <f t="shared" si="3"/>
+      <c r="N39" s="76">
+        <f t="shared" si="2"/>
         <v>2.5000000000000036E-2</v>
       </c>
-      <c r="O39" s="99"/>
+      <c r="O39" s="98"/>
       <c r="P39" s="21"/>
       <c r="Q39" s="22"/>
       <c r="R39" s="22"/>
@@ -3872,46 +3843,45 @@
       <c r="Z39" s="22"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A40" s="99"/>
+      <c r="A40" s="98"/>
       <c r="B40" s="30">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="C40" s="112" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" s="128" t="s">
         <v>57</v>
       </c>
-      <c r="D40" s="113"/>
-      <c r="E40" s="114"/>
-      <c r="F40" s="105">
+      <c r="D40" s="129"/>
+      <c r="E40" s="130"/>
+      <c r="F40" s="104">
         <v>25</v>
       </c>
-      <c r="G40" s="106">
+      <c r="G40" s="105">
         <v>1.7361111111111112E-2</v>
       </c>
-      <c r="H40" s="103">
+      <c r="H40" s="102">
         <v>0.40208333333333335</v>
       </c>
-      <c r="I40" s="104">
+      <c r="I40" s="103">
         <v>0.40972222222222227</v>
       </c>
-      <c r="J40" s="110">
-        <f t="shared" si="4"/>
-        <v>7.6388888888889173E-3</v>
-      </c>
-      <c r="K40" s="105">
-        <v>0</v>
-      </c>
-      <c r="L40" s="108">
-        <v>0</v>
-      </c>
-      <c r="M40" s="105">
-        <v>9</v>
-      </c>
-      <c r="N40" s="77">
+      <c r="J40" s="108">
         <f t="shared" si="3"/>
         <v>7.6388888888889173E-3</v>
       </c>
-      <c r="O40" s="99"/>
+      <c r="K40" s="104">
+        <v>0</v>
+      </c>
+      <c r="L40" s="107">
+        <v>0</v>
+      </c>
+      <c r="M40" s="104">
+        <v>9</v>
+      </c>
+      <c r="N40" s="76">
+        <f t="shared" si="2"/>
+        <v>7.6388888888889173E-3</v>
+      </c>
+      <c r="O40" s="98"/>
       <c r="P40" s="21"/>
       <c r="Q40" s="22"/>
       <c r="R40" s="22"/>
@@ -3925,45 +3895,45 @@
       <c r="Z40" s="22"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A41" s="111"/>
+      <c r="A41" s="109"/>
       <c r="B41" s="30">
-        <v>25</v>
-      </c>
-      <c r="C41" s="112" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" s="128" t="s">
         <v>58</v>
       </c>
-      <c r="D41" s="113"/>
-      <c r="E41" s="114"/>
-      <c r="F41" s="105">
+      <c r="D41" s="129"/>
+      <c r="E41" s="130"/>
+      <c r="F41" s="104">
         <v>20</v>
       </c>
-      <c r="G41" s="106">
+      <c r="G41" s="105">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="H41" s="103">
+      <c r="H41" s="102">
         <v>3.6111111111111115E-2</v>
       </c>
-      <c r="I41" s="104">
+      <c r="I41" s="103">
         <v>5.8333333333333327E-2</v>
       </c>
-      <c r="J41" s="110">
-        <f t="shared" si="4"/>
-        <v>2.2222222222222213E-2</v>
-      </c>
-      <c r="K41" s="105">
-        <v>0</v>
-      </c>
-      <c r="L41" s="108">
-        <v>0</v>
-      </c>
-      <c r="M41" s="105">
-        <v>18</v>
-      </c>
-      <c r="N41" s="77">
+      <c r="J41" s="108">
         <f t="shared" si="3"/>
         <v>2.2222222222222213E-2</v>
       </c>
-      <c r="O41" s="111"/>
+      <c r="K41" s="104">
+        <v>0</v>
+      </c>
+      <c r="L41" s="107">
+        <v>0</v>
+      </c>
+      <c r="M41" s="104">
+        <v>18</v>
+      </c>
+      <c r="N41" s="76">
+        <f t="shared" si="2"/>
+        <v>2.2222222222222213E-2</v>
+      </c>
+      <c r="O41" s="109"/>
       <c r="P41" s="21"/>
       <c r="Q41" s="22"/>
       <c r="R41" s="22"/>
@@ -3978,21 +3948,19 @@
     </row>
     <row r="42" spans="1:26" ht="15" customHeight="1">
       <c r="A42" s="67"/>
-      <c r="B42" s="30">
-        <v>26</v>
-      </c>
-      <c r="C42" s="112"/>
-      <c r="D42" s="113"/>
-      <c r="E42" s="114"/>
-      <c r="F42" s="105"/>
-      <c r="G42" s="106"/>
-      <c r="H42" s="103"/>
-      <c r="I42" s="104"/>
-      <c r="J42" s="110"/>
-      <c r="K42" s="105"/>
-      <c r="L42" s="108"/>
-      <c r="M42" s="105"/>
-      <c r="N42" s="77"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="128"/>
+      <c r="D42" s="129"/>
+      <c r="E42" s="130"/>
+      <c r="F42" s="104"/>
+      <c r="G42" s="105"/>
+      <c r="H42" s="102"/>
+      <c r="I42" s="103"/>
+      <c r="J42" s="108"/>
+      <c r="K42" s="104"/>
+      <c r="L42" s="107"/>
+      <c r="M42" s="104"/>
+      <c r="N42" s="76"/>
       <c r="O42" s="67"/>
       <c r="P42" s="21"/>
       <c r="Q42" s="22"/>
@@ -4008,12 +3976,12 @@
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A43" s="7"/>
-      <c r="B43" s="118" t="s">
+      <c r="B43" s="160" t="s">
         <v>23</v>
       </c>
-      <c r="C43" s="119"/>
-      <c r="D43" s="119"/>
-      <c r="E43" s="120"/>
+      <c r="C43" s="161"/>
+      <c r="D43" s="161"/>
+      <c r="E43" s="162"/>
       <c r="F43" s="46">
         <f>IF(SUM(F18:F42)=0,"Completar",SUM(F18:F42))</f>
         <v>492</v>
@@ -4028,7 +3996,7 @@
       <c r="I43" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="J43" s="101">
+      <c r="J43" s="100">
         <f>IF(OR(COUNTIF(J18:J42,"Error")&gt;0,COUNTIF(J18:J42,"Completar")&gt;0),"Error",IF(SUM(J18:J42)=0,"Completar",SUM(J18:J42)))</f>
         <v>0.38125000000000037</v>
       </c>
@@ -4091,12 +4059,12 @@
     </row>
     <row r="45" spans="1:26" ht="15" customHeight="1">
       <c r="A45" s="4"/>
-      <c r="B45" s="115" t="s">
+      <c r="B45" s="112" t="s">
         <v>25</v>
       </c>
-      <c r="C45" s="116"/>
-      <c r="D45" s="116"/>
-      <c r="E45" s="117"/>
+      <c r="C45" s="134"/>
+      <c r="D45" s="134"/>
+      <c r="E45" s="135"/>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
@@ -4222,21 +4190,21 @@
     </row>
     <row r="49" spans="1:26">
       <c r="A49" s="20"/>
-      <c r="B49" s="115" t="s">
+      <c r="B49" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="C49" s="116"/>
-      <c r="D49" s="116"/>
-      <c r="E49" s="116"/>
-      <c r="F49" s="116"/>
-      <c r="G49" s="116"/>
-      <c r="H49" s="116"/>
-      <c r="I49" s="116"/>
-      <c r="J49" s="116"/>
-      <c r="K49" s="116"/>
-      <c r="L49" s="116"/>
-      <c r="M49" s="116"/>
-      <c r="N49" s="117"/>
+      <c r="C49" s="134"/>
+      <c r="D49" s="134"/>
+      <c r="E49" s="134"/>
+      <c r="F49" s="134"/>
+      <c r="G49" s="134"/>
+      <c r="H49" s="134"/>
+      <c r="I49" s="134"/>
+      <c r="J49" s="134"/>
+      <c r="K49" s="134"/>
+      <c r="L49" s="134"/>
+      <c r="M49" s="134"/>
+      <c r="N49" s="135"/>
       <c r="O49" s="20"/>
       <c r="P49" s="55"/>
       <c r="Q49" s="55"/>
@@ -4252,16 +4220,16 @@
     </row>
     <row r="50" spans="1:26" ht="15" customHeight="1">
       <c r="A50" s="20"/>
-      <c r="B50" s="146" t="s">
+      <c r="B50" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="C50" s="147"/>
-      <c r="D50" s="148"/>
-      <c r="E50" s="149">
+      <c r="C50" s="119"/>
+      <c r="D50" s="120"/>
+      <c r="E50" s="136">
         <f>M43</f>
         <v>457</v>
       </c>
-      <c r="F50" s="150"/>
+      <c r="F50" s="132"/>
       <c r="G50" s="56"/>
       <c r="H50" s="57"/>
       <c r="I50" s="57"/>
@@ -4285,16 +4253,16 @@
     </row>
     <row r="51" spans="1:26">
       <c r="A51" s="20"/>
-      <c r="B51" s="146" t="s">
+      <c r="B51" s="118" t="s">
         <v>28</v>
       </c>
-      <c r="C51" s="147"/>
-      <c r="D51" s="148"/>
-      <c r="E51" s="162">
+      <c r="C51" s="119"/>
+      <c r="D51" s="120"/>
+      <c r="E51" s="133">
         <f>IF(M43="Completar","Completar",IFERROR(M43/(N43*24),"Error"))</f>
         <v>41.798780487804848</v>
       </c>
-      <c r="F51" s="150"/>
+      <c r="F51" s="132"/>
       <c r="G51" s="59"/>
       <c r="H51" s="60"/>
       <c r="I51" s="60"/>
@@ -4318,16 +4286,16 @@
     </row>
     <row r="52" spans="1:26" ht="15" customHeight="1">
       <c r="A52" s="20"/>
-      <c r="B52" s="146" t="s">
+      <c r="B52" s="118" t="s">
         <v>29</v>
       </c>
-      <c r="C52" s="147"/>
-      <c r="D52" s="148"/>
-      <c r="E52" s="149">
+      <c r="C52" s="119"/>
+      <c r="D52" s="120"/>
+      <c r="E52" s="136">
         <f>IF(K43=0,0,IFERROR(ROUNDUP(K43/(M43/100),0),"Error"))</f>
         <v>6</v>
       </c>
-      <c r="F52" s="150"/>
+      <c r="F52" s="132"/>
       <c r="G52" s="59"/>
       <c r="H52" s="60"/>
       <c r="I52" s="60"/>
@@ -4351,16 +4319,16 @@
     </row>
     <row r="53" spans="1:26" ht="15" customHeight="1">
       <c r="A53" s="20"/>
-      <c r="B53" s="146" t="s">
+      <c r="B53" s="118" t="s">
         <v>30</v>
       </c>
-      <c r="C53" s="147"/>
-      <c r="D53" s="148"/>
-      <c r="E53" s="161">
+      <c r="C53" s="119"/>
+      <c r="D53" s="120"/>
+      <c r="E53" s="131">
         <f>IF(K43=0,0,IFERROR(K43/M43,"Error"))</f>
         <v>5.4704595185995623E-2</v>
       </c>
-      <c r="F53" s="150"/>
+      <c r="F53" s="132"/>
       <c r="G53" s="59"/>
       <c r="H53" s="60"/>
       <c r="I53" s="60"/>
@@ -4384,17 +4352,17 @@
     </row>
     <row r="54" spans="1:26" ht="15" customHeight="1">
       <c r="A54" s="20"/>
-      <c r="B54" s="146" t="s">
+      <c r="B54" s="118" t="s">
         <v>31</v>
       </c>
-      <c r="C54" s="147"/>
-      <c r="D54" s="148"/>
+      <c r="C54" s="119"/>
+      <c r="D54" s="120"/>
       <c r="E54" s="62">
         <f>E5</f>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="F54" s="63">
-        <f t="shared" ref="F54:F57" si="5">IF(E54="Completar",E54,IFERROR(E54/$E$60,"Error"))</f>
+        <f t="shared" ref="F54:F57" si="4">IF(E54="Completar",E54,IFERROR(E54/$E$60,"Error"))</f>
         <v>1.3157894736842051E-2</v>
       </c>
       <c r="G54" s="59"/>
@@ -4420,17 +4388,17 @@
     </row>
     <row r="55" spans="1:26" ht="15" customHeight="1">
       <c r="A55" s="20"/>
-      <c r="B55" s="146" t="s">
+      <c r="B55" s="118" t="s">
         <v>32</v>
       </c>
-      <c r="C55" s="147"/>
-      <c r="D55" s="148"/>
+      <c r="C55" s="119"/>
+      <c r="D55" s="120"/>
       <c r="E55" s="62">
         <f>E9</f>
         <v>1.736111111111116E-2</v>
       </c>
       <c r="F55" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.2894736842105338E-2</v>
       </c>
       <c r="G55" s="59"/>
@@ -4456,17 +4424,17 @@
     </row>
     <row r="56" spans="1:26" ht="15" customHeight="1">
       <c r="A56" s="20"/>
-      <c r="B56" s="146" t="s">
+      <c r="B56" s="118" t="s">
         <v>33</v>
       </c>
-      <c r="C56" s="147"/>
-      <c r="D56" s="148"/>
+      <c r="C56" s="119"/>
+      <c r="D56" s="120"/>
       <c r="E56" s="62">
         <f>E13</f>
         <v>1.3194444444444398E-2</v>
       </c>
       <c r="F56" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.4999999999999894E-2</v>
       </c>
       <c r="G56" s="59"/>
@@ -4492,17 +4460,17 @@
     </row>
     <row r="57" spans="1:26" ht="15" customHeight="1">
       <c r="A57" s="20"/>
-      <c r="B57" s="146" t="s">
+      <c r="B57" s="118" t="s">
         <v>34</v>
       </c>
-      <c r="C57" s="147"/>
-      <c r="D57" s="148"/>
+      <c r="C57" s="119"/>
+      <c r="D57" s="120"/>
       <c r="E57" s="62">
         <f>E47</f>
         <v>3.4722222222222265E-2</v>
       </c>
       <c r="F57" s="63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6.5789473684210564E-2</v>
       </c>
       <c r="G57" s="59"/>
@@ -4528,17 +4496,17 @@
     </row>
     <row r="58" spans="1:26" ht="15" customHeight="1">
       <c r="A58" s="20"/>
-      <c r="B58" s="146" t="s">
+      <c r="B58" s="118" t="s">
         <v>35</v>
       </c>
-      <c r="C58" s="147"/>
-      <c r="D58" s="148"/>
+      <c r="C58" s="119"/>
+      <c r="D58" s="120"/>
       <c r="E58" s="62">
         <f>L43</f>
         <v>7.4305555555555555E-2</v>
       </c>
       <c r="F58" s="63">
-        <f t="shared" ref="F58:F59" si="6">IF(E58="Completar",E58,IFERROR(E58/$E$60,"Completar"))</f>
+        <f t="shared" ref="F58:F59" si="5">IF(E58="Completar",E58,IFERROR(E58/$E$60,"Completar"))</f>
         <v>0.14078947368421044</v>
       </c>
       <c r="G58" s="59"/>
@@ -4564,17 +4532,17 @@
     </row>
     <row r="59" spans="1:26" ht="15" customHeight="1">
       <c r="A59" s="20"/>
-      <c r="B59" s="146" t="s">
+      <c r="B59" s="118" t="s">
         <v>36</v>
       </c>
-      <c r="C59" s="147"/>
-      <c r="D59" s="148"/>
+      <c r="C59" s="119"/>
+      <c r="D59" s="120"/>
       <c r="E59" s="62">
         <f>J43</f>
         <v>0.38125000000000037</v>
       </c>
       <c r="F59" s="63">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.72236842105263177</v>
       </c>
       <c r="G59" s="59"/>
@@ -4600,16 +4568,16 @@
     </row>
     <row r="60" spans="1:26" ht="15" customHeight="1" thickBot="1">
       <c r="A60" s="20"/>
-      <c r="B60" s="158" t="s">
+      <c r="B60" s="123" t="s">
         <v>37</v>
       </c>
-      <c r="C60" s="159"/>
-      <c r="D60" s="160"/>
-      <c r="E60" s="156">
+      <c r="C60" s="124"/>
+      <c r="D60" s="125"/>
+      <c r="E60" s="121">
         <f>IF(COUNTIF(E54:E59,"Error")&gt;0,"Error",IF(SUM(E54:E59)=0,"Completar",SUM(E54:E59)))</f>
         <v>0.52777777777777812</v>
       </c>
-      <c r="F60" s="157"/>
+      <c r="F60" s="122"/>
       <c r="G60" s="64"/>
       <c r="H60" s="65"/>
       <c r="I60" s="65"/>
@@ -31429,13 +31397,44 @@
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="D1:N1"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="F8:N8"/>
-    <mergeCell ref="F9:N9"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B49:N49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="B52:D52"/>
     <mergeCell ref="B15:N15"/>
     <mergeCell ref="F12:N12"/>
     <mergeCell ref="F13:N13"/>
@@ -31452,132 +31451,101 @@
     <mergeCell ref="E53:F53"/>
     <mergeCell ref="B53:D53"/>
     <mergeCell ref="E51:F51"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B49:N49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="D1:N1"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F8:N8"/>
+    <mergeCell ref="F9:N9"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:XFD24 C3:C24 K32:M36 C29:I29 K29:M29 C30:M30 C32:I35 J27:J29 J31:J39 C61:D1048576 O43:XFD1048576 E50:N1048576 F43:N48 C46:E48 C44:E44 J41:J42 N25:XFD42 A1:B1048576">
-    <cfRule type="cellIs" dxfId="17" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="37" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:XFD24 C3:C24 K32:M36 C29:I29 K29:M29 C30:M30 C32:I35 J27:J29 J31:J39 C61:D1048576 O43:XFD1048576 E50:N1048576 F43:N48 C46:E48 C44:E44 J41:J42 N25:XFD42 A1:B1048576">
-    <cfRule type="cellIs" dxfId="16" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="38" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:M25 C26:E26">
-    <cfRule type="cellIs" dxfId="15" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="35" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:M25 C26:E26">
-    <cfRule type="cellIs" dxfId="14" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="36" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F26:M26 C42 F42:I42 K42:M42">
-    <cfRule type="cellIs" dxfId="13" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="29" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F26:M26 C42 F42:I42 K42:M42">
-    <cfRule type="cellIs" dxfId="12" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="30" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:I27 K27:M27">
-    <cfRule type="cellIs" dxfId="11" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="25" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:I27 K27:M27">
-    <cfRule type="cellIs" dxfId="10" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="26" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:M31 C31 F31:I31">
-    <cfRule type="cellIs" dxfId="9" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="21" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:M31 C31 F31:I31">
-    <cfRule type="cellIs" dxfId="8" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="22" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28:M28 C28 F28:I28">
-    <cfRule type="cellIs" dxfId="7" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="17" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28:M28 C28 F28:I28">
-    <cfRule type="cellIs" dxfId="6" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="18" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:M31 C31 F31:I31">
-    <cfRule type="cellIs" dxfId="5" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:M31 C31 F31:I31">
-    <cfRule type="cellIs" dxfId="4" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:I28 K28:M28">
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:I28 K28:M28">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41 F41:I41 K41:M41">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41 F41:I41 K41:M41">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>